<commit_message>
Criação da pasta "Prototipo (parcial)" a qual possui o prototipo em baixa fidelidade das telas de cadastro do sistema. Estas telas deverão ser geradas na sprint 1. Para a sprint 2, serão adicionadas telas de consulta e do motor de regra, a qual no protipo chamaremos de configuração de regras.
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -774,25 +774,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1164,10 +1164,10 @@
   <dimension ref="A1:EE76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="N3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="Y38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="X3" sqref="X3"/>
+      <selection pane="bottomRight" activeCell="AC46" sqref="AC46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1260,181 +1260,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="82">
+      <c r="D1" s="79">
         <v>42322</v>
       </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="82">
+      <c r="J1" s="79">
         <v>42323</v>
       </c>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="82">
+      <c r="P1" s="79">
         <v>42324</v>
       </c>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="82">
+      <c r="V1" s="79">
         <v>42325</v>
       </c>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
       <c r="AA1" s="12"/>
-      <c r="AB1" s="82">
+      <c r="AB1" s="79">
         <v>42326</v>
       </c>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="80"/>
+      <c r="AE1" s="80"/>
+      <c r="AF1" s="80"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="82">
+      <c r="AH1" s="79">
         <v>42327</v>
       </c>
-      <c r="AI1" s="83"/>
-      <c r="AJ1" s="83"/>
-      <c r="AK1" s="83"/>
-      <c r="AL1" s="83"/>
+      <c r="AI1" s="80"/>
+      <c r="AJ1" s="80"/>
+      <c r="AK1" s="80"/>
+      <c r="AL1" s="80"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="82">
+      <c r="AN1" s="79">
         <v>42328</v>
       </c>
-      <c r="AO1" s="83"/>
-      <c r="AP1" s="83"/>
-      <c r="AQ1" s="83"/>
-      <c r="AR1" s="83"/>
+      <c r="AO1" s="80"/>
+      <c r="AP1" s="80"/>
+      <c r="AQ1" s="80"/>
+      <c r="AR1" s="80"/>
       <c r="AS1" s="12"/>
-      <c r="AT1" s="82">
+      <c r="AT1" s="79">
         <v>42329</v>
       </c>
-      <c r="AU1" s="83"/>
-      <c r="AV1" s="83"/>
-      <c r="AW1" s="83"/>
-      <c r="AX1" s="83"/>
+      <c r="AU1" s="80"/>
+      <c r="AV1" s="80"/>
+      <c r="AW1" s="80"/>
+      <c r="AX1" s="80"/>
       <c r="AY1" s="12"/>
-      <c r="AZ1" s="82">
+      <c r="AZ1" s="79">
         <v>42330</v>
       </c>
-      <c r="BA1" s="83"/>
-      <c r="BB1" s="83"/>
-      <c r="BC1" s="83"/>
-      <c r="BD1" s="83"/>
+      <c r="BA1" s="80"/>
+      <c r="BB1" s="80"/>
+      <c r="BC1" s="80"/>
+      <c r="BD1" s="80"/>
       <c r="BE1" s="12"/>
-      <c r="BF1" s="82">
+      <c r="BF1" s="79">
         <v>42331</v>
       </c>
-      <c r="BG1" s="83"/>
-      <c r="BH1" s="83"/>
-      <c r="BI1" s="83"/>
-      <c r="BJ1" s="83"/>
+      <c r="BG1" s="80"/>
+      <c r="BH1" s="80"/>
+      <c r="BI1" s="80"/>
+      <c r="BJ1" s="80"/>
       <c r="BK1" s="12"/>
-      <c r="BL1" s="82">
+      <c r="BL1" s="79">
         <v>42332</v>
       </c>
-      <c r="BM1" s="83"/>
-      <c r="BN1" s="83"/>
-      <c r="BO1" s="83"/>
-      <c r="BP1" s="83"/>
+      <c r="BM1" s="80"/>
+      <c r="BN1" s="80"/>
+      <c r="BO1" s="80"/>
+      <c r="BP1" s="80"/>
       <c r="BQ1" s="12"/>
-      <c r="BR1" s="82">
+      <c r="BR1" s="79">
         <v>42333</v>
       </c>
-      <c r="BS1" s="83"/>
-      <c r="BT1" s="83"/>
-      <c r="BU1" s="83"/>
-      <c r="BV1" s="83"/>
+      <c r="BS1" s="80"/>
+      <c r="BT1" s="80"/>
+      <c r="BU1" s="80"/>
+      <c r="BV1" s="80"/>
       <c r="BW1" s="12"/>
-      <c r="BX1" s="82">
+      <c r="BX1" s="79">
         <v>42334</v>
       </c>
-      <c r="BY1" s="83"/>
-      <c r="BZ1" s="83"/>
-      <c r="CA1" s="83"/>
-      <c r="CB1" s="83"/>
+      <c r="BY1" s="80"/>
+      <c r="BZ1" s="80"/>
+      <c r="CA1" s="80"/>
+      <c r="CB1" s="80"/>
       <c r="CC1" s="12"/>
-      <c r="CD1" s="82">
+      <c r="CD1" s="79">
         <v>42335</v>
       </c>
-      <c r="CE1" s="83"/>
-      <c r="CF1" s="83"/>
-      <c r="CG1" s="83"/>
-      <c r="CH1" s="83"/>
+      <c r="CE1" s="80"/>
+      <c r="CF1" s="80"/>
+      <c r="CG1" s="80"/>
+      <c r="CH1" s="80"/>
       <c r="CI1" s="12"/>
-      <c r="CJ1" s="82">
+      <c r="CJ1" s="79">
         <v>42336</v>
       </c>
-      <c r="CK1" s="83"/>
-      <c r="CL1" s="83"/>
-      <c r="CM1" s="83"/>
-      <c r="CN1" s="83"/>
+      <c r="CK1" s="80"/>
+      <c r="CL1" s="80"/>
+      <c r="CM1" s="80"/>
+      <c r="CN1" s="80"/>
       <c r="CO1" s="12"/>
-      <c r="CP1" s="82">
+      <c r="CP1" s="79">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="83"/>
-      <c r="CR1" s="83"/>
-      <c r="CS1" s="83"/>
-      <c r="CT1" s="83"/>
+      <c r="CQ1" s="80"/>
+      <c r="CR1" s="80"/>
+      <c r="CS1" s="80"/>
+      <c r="CT1" s="80"/>
       <c r="CU1" s="12"/>
-      <c r="CV1" s="82">
+      <c r="CV1" s="79">
         <v>42338</v>
       </c>
-      <c r="CW1" s="83"/>
-      <c r="CX1" s="83"/>
-      <c r="CY1" s="83"/>
-      <c r="CZ1" s="83"/>
+      <c r="CW1" s="80"/>
+      <c r="CX1" s="80"/>
+      <c r="CY1" s="80"/>
+      <c r="CZ1" s="80"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="82">
+      <c r="DB1" s="79">
         <v>42339</v>
       </c>
-      <c r="DC1" s="83"/>
-      <c r="DD1" s="83"/>
-      <c r="DE1" s="83"/>
-      <c r="DF1" s="83"/>
+      <c r="DC1" s="80"/>
+      <c r="DD1" s="80"/>
+      <c r="DE1" s="80"/>
+      <c r="DF1" s="80"/>
       <c r="DG1" s="12"/>
-      <c r="DH1" s="82">
+      <c r="DH1" s="79">
         <v>42340</v>
       </c>
-      <c r="DI1" s="83"/>
-      <c r="DJ1" s="83"/>
-      <c r="DK1" s="83"/>
-      <c r="DL1" s="83"/>
+      <c r="DI1" s="80"/>
+      <c r="DJ1" s="80"/>
+      <c r="DK1" s="80"/>
+      <c r="DL1" s="80"/>
       <c r="DM1" s="12"/>
-      <c r="DN1" s="82">
+      <c r="DN1" s="79">
         <v>42341</v>
       </c>
-      <c r="DO1" s="83"/>
-      <c r="DP1" s="83"/>
-      <c r="DQ1" s="83"/>
-      <c r="DR1" s="83"/>
+      <c r="DO1" s="80"/>
+      <c r="DP1" s="80"/>
+      <c r="DQ1" s="80"/>
+      <c r="DR1" s="80"/>
       <c r="DS1" s="12"/>
-      <c r="DT1" s="82">
+      <c r="DT1" s="79">
         <v>42342</v>
       </c>
-      <c r="DU1" s="83"/>
-      <c r="DV1" s="83"/>
-      <c r="DW1" s="83"/>
-      <c r="DX1" s="83"/>
+      <c r="DU1" s="80"/>
+      <c r="DV1" s="80"/>
+      <c r="DW1" s="80"/>
+      <c r="DX1" s="80"/>
       <c r="DY1" s="12"/>
-      <c r="DZ1" s="82">
+      <c r="DZ1" s="79">
         <v>42343</v>
       </c>
-      <c r="EA1" s="83"/>
-      <c r="EB1" s="83"/>
-      <c r="EC1" s="83"/>
-      <c r="ED1" s="83"/>
+      <c r="EA1" s="80"/>
+      <c r="EB1" s="80"/>
+      <c r="EC1" s="80"/>
+      <c r="ED1" s="80"/>
       <c r="EE1" s="12"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -1849,7 +1849,9 @@
       <c r="AB3" s="71">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AC3" s="77"/>
+      <c r="AC3" s="72">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="AD3" s="74"/>
       <c r="AE3" s="74"/>
       <c r="AF3" s="75"/>
@@ -2899,7 +2901,7 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="80" t="s">
+      <c r="C10" s="85" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="6">
@@ -3197,7 +3199,7 @@
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="80" t="s">
+      <c r="C12" s="85" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="6">
@@ -5095,7 +5097,7 @@
       <c r="B25" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="84" t="s">
+      <c r="C25" s="82" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="6"/>
@@ -5240,7 +5242,7 @@
       <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="85"/>
+      <c r="C26" s="83"/>
       <c r="D26" s="6"/>
       <c r="E26" s="7"/>
       <c r="F26" s="8"/>
@@ -7986,9 +7988,11 @@
       <c r="Y45" s="9"/>
       <c r="Z45" s="10"/>
       <c r="AA45" s="12"/>
-      <c r="AB45" s="6"/>
+      <c r="AB45" s="6">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="AC45" s="7">
-        <v>0.16666666666666666</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="AD45" s="8"/>
       <c r="AE45" s="9"/>
@@ -8883,7 +8887,7 @@
       <c r="B51" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="79" t="s">
+      <c r="C51" s="84" t="s">
         <v>20</v>
       </c>
       <c r="D51" s="14"/>
@@ -9026,7 +9030,7 @@
       <c r="B52" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="79"/>
+      <c r="C52" s="84"/>
       <c r="D52" s="14"/>
       <c r="E52" s="18"/>
       <c r="F52" s="8"/>
@@ -9882,7 +9886,7 @@
       <c r="B58" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C58" s="79" t="s">
+      <c r="C58" s="84" t="s">
         <v>30</v>
       </c>
       <c r="D58" s="14"/>
@@ -10025,7 +10029,7 @@
       <c r="B59" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="79"/>
+      <c r="C59" s="84"/>
       <c r="D59" s="14"/>
       <c r="E59" s="18"/>
       <c r="F59" s="18"/>
@@ -10166,7 +10170,7 @@
       <c r="B60" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="79"/>
+      <c r="C60" s="84"/>
       <c r="D60" s="14"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
@@ -10913,11 +10917,11 @@
       <c r="Z64" s="31"/>
       <c r="AB64" s="28">
         <f>SUM(AB3:AB61)</f>
-        <v>0.20833333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="AC64" s="29">
         <f>SUM(AC3:AC61)</f>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="AD64" s="30" t="s">
         <v>37</v>
@@ -12294,6 +12298,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="DN1:DR1"/>
+    <mergeCell ref="DT1:DX1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="V1:Z1"/>
     <mergeCell ref="DZ1:ED1"/>
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="C25:C26"/>
@@ -12310,20 +12328,6 @@
     <mergeCell ref="AB1:AF1"/>
     <mergeCell ref="AT1:AX1"/>
     <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="DN1:DR1"/>
-    <mergeCell ref="DT1:DX1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="AN1:AR1"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização da planilha de atividades que não foi na última atualização.
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -793,6 +793,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -817,8 +819,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1185,10 +1185,10 @@
   <dimension ref="A1:EE76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AH3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AD3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="AR18" sqref="AR18"/>
+      <selection pane="bottomRight" activeCell="AI46" sqref="AI46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1281,181 +1281,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="80">
+      <c r="D1" s="82">
         <v>42322</v>
       </c>
-      <c r="E1" s="81"/>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="80">
+      <c r="J1" s="82">
         <v>42323</v>
       </c>
-      <c r="K1" s="81"/>
-      <c r="L1" s="81"/>
-      <c r="M1" s="81"/>
-      <c r="N1" s="81"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="80">
+      <c r="P1" s="82">
         <v>42324</v>
       </c>
-      <c r="Q1" s="81"/>
-      <c r="R1" s="81"/>
-      <c r="S1" s="81"/>
-      <c r="T1" s="81"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="80">
+      <c r="V1" s="82">
         <v>42325</v>
       </c>
-      <c r="W1" s="81"/>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="81"/>
-      <c r="Z1" s="81"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
       <c r="AA1" s="12"/>
-      <c r="AB1" s="80">
+      <c r="AB1" s="82">
         <v>42326</v>
       </c>
-      <c r="AC1" s="81"/>
-      <c r="AD1" s="81"/>
-      <c r="AE1" s="81"/>
-      <c r="AF1" s="81"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="83"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="80">
+      <c r="AH1" s="82">
         <v>42327</v>
       </c>
-      <c r="AI1" s="81"/>
-      <c r="AJ1" s="81"/>
-      <c r="AK1" s="81"/>
-      <c r="AL1" s="81"/>
+      <c r="AI1" s="83"/>
+      <c r="AJ1" s="83"/>
+      <c r="AK1" s="83"/>
+      <c r="AL1" s="83"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="80">
+      <c r="AN1" s="82">
         <v>42328</v>
       </c>
-      <c r="AO1" s="81"/>
-      <c r="AP1" s="81"/>
-      <c r="AQ1" s="81"/>
-      <c r="AR1" s="81"/>
+      <c r="AO1" s="83"/>
+      <c r="AP1" s="83"/>
+      <c r="AQ1" s="83"/>
+      <c r="AR1" s="83"/>
       <c r="AS1" s="12"/>
-      <c r="AT1" s="80">
+      <c r="AT1" s="82">
         <v>42329</v>
       </c>
-      <c r="AU1" s="81"/>
-      <c r="AV1" s="81"/>
-      <c r="AW1" s="81"/>
-      <c r="AX1" s="81"/>
+      <c r="AU1" s="83"/>
+      <c r="AV1" s="83"/>
+      <c r="AW1" s="83"/>
+      <c r="AX1" s="83"/>
       <c r="AY1" s="12"/>
-      <c r="AZ1" s="80">
+      <c r="AZ1" s="82">
         <v>42330</v>
       </c>
-      <c r="BA1" s="81"/>
-      <c r="BB1" s="81"/>
-      <c r="BC1" s="81"/>
-      <c r="BD1" s="81"/>
+      <c r="BA1" s="83"/>
+      <c r="BB1" s="83"/>
+      <c r="BC1" s="83"/>
+      <c r="BD1" s="83"/>
       <c r="BE1" s="12"/>
-      <c r="BF1" s="80">
+      <c r="BF1" s="82">
         <v>42331</v>
       </c>
-      <c r="BG1" s="81"/>
-      <c r="BH1" s="81"/>
-      <c r="BI1" s="81"/>
-      <c r="BJ1" s="81"/>
+      <c r="BG1" s="83"/>
+      <c r="BH1" s="83"/>
+      <c r="BI1" s="83"/>
+      <c r="BJ1" s="83"/>
       <c r="BK1" s="12"/>
-      <c r="BL1" s="80">
+      <c r="BL1" s="82">
         <v>42332</v>
       </c>
-      <c r="BM1" s="81"/>
-      <c r="BN1" s="81"/>
-      <c r="BO1" s="81"/>
-      <c r="BP1" s="81"/>
+      <c r="BM1" s="83"/>
+      <c r="BN1" s="83"/>
+      <c r="BO1" s="83"/>
+      <c r="BP1" s="83"/>
       <c r="BQ1" s="12"/>
-      <c r="BR1" s="80">
+      <c r="BR1" s="82">
         <v>42333</v>
       </c>
-      <c r="BS1" s="81"/>
-      <c r="BT1" s="81"/>
-      <c r="BU1" s="81"/>
-      <c r="BV1" s="81"/>
+      <c r="BS1" s="83"/>
+      <c r="BT1" s="83"/>
+      <c r="BU1" s="83"/>
+      <c r="BV1" s="83"/>
       <c r="BW1" s="12"/>
-      <c r="BX1" s="80">
+      <c r="BX1" s="82">
         <v>42334</v>
       </c>
-      <c r="BY1" s="81"/>
-      <c r="BZ1" s="81"/>
-      <c r="CA1" s="81"/>
-      <c r="CB1" s="81"/>
+      <c r="BY1" s="83"/>
+      <c r="BZ1" s="83"/>
+      <c r="CA1" s="83"/>
+      <c r="CB1" s="83"/>
       <c r="CC1" s="12"/>
-      <c r="CD1" s="80">
+      <c r="CD1" s="82">
         <v>42335</v>
       </c>
-      <c r="CE1" s="81"/>
-      <c r="CF1" s="81"/>
-      <c r="CG1" s="81"/>
-      <c r="CH1" s="81"/>
+      <c r="CE1" s="83"/>
+      <c r="CF1" s="83"/>
+      <c r="CG1" s="83"/>
+      <c r="CH1" s="83"/>
       <c r="CI1" s="12"/>
-      <c r="CJ1" s="80">
+      <c r="CJ1" s="82">
         <v>42336</v>
       </c>
-      <c r="CK1" s="81"/>
-      <c r="CL1" s="81"/>
-      <c r="CM1" s="81"/>
-      <c r="CN1" s="81"/>
+      <c r="CK1" s="83"/>
+      <c r="CL1" s="83"/>
+      <c r="CM1" s="83"/>
+      <c r="CN1" s="83"/>
       <c r="CO1" s="12"/>
-      <c r="CP1" s="80">
+      <c r="CP1" s="82">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="81"/>
-      <c r="CR1" s="81"/>
-      <c r="CS1" s="81"/>
-      <c r="CT1" s="81"/>
+      <c r="CQ1" s="83"/>
+      <c r="CR1" s="83"/>
+      <c r="CS1" s="83"/>
+      <c r="CT1" s="83"/>
       <c r="CU1" s="12"/>
-      <c r="CV1" s="80">
+      <c r="CV1" s="82">
         <v>42338</v>
       </c>
-      <c r="CW1" s="81"/>
-      <c r="CX1" s="81"/>
-      <c r="CY1" s="81"/>
-      <c r="CZ1" s="81"/>
+      <c r="CW1" s="83"/>
+      <c r="CX1" s="83"/>
+      <c r="CY1" s="83"/>
+      <c r="CZ1" s="83"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="80">
+      <c r="DB1" s="82">
         <v>42339</v>
       </c>
-      <c r="DC1" s="81"/>
-      <c r="DD1" s="81"/>
-      <c r="DE1" s="81"/>
-      <c r="DF1" s="81"/>
+      <c r="DC1" s="83"/>
+      <c r="DD1" s="83"/>
+      <c r="DE1" s="83"/>
+      <c r="DF1" s="83"/>
       <c r="DG1" s="12"/>
-      <c r="DH1" s="80">
+      <c r="DH1" s="82">
         <v>42340</v>
       </c>
-      <c r="DI1" s="81"/>
-      <c r="DJ1" s="81"/>
-      <c r="DK1" s="81"/>
-      <c r="DL1" s="81"/>
+      <c r="DI1" s="83"/>
+      <c r="DJ1" s="83"/>
+      <c r="DK1" s="83"/>
+      <c r="DL1" s="83"/>
       <c r="DM1" s="12"/>
-      <c r="DN1" s="80">
+      <c r="DN1" s="82">
         <v>42341</v>
       </c>
-      <c r="DO1" s="81"/>
-      <c r="DP1" s="81"/>
-      <c r="DQ1" s="81"/>
-      <c r="DR1" s="81"/>
+      <c r="DO1" s="83"/>
+      <c r="DP1" s="83"/>
+      <c r="DQ1" s="83"/>
+      <c r="DR1" s="83"/>
       <c r="DS1" s="12"/>
-      <c r="DT1" s="80">
+      <c r="DT1" s="82">
         <v>42342</v>
       </c>
-      <c r="DU1" s="81"/>
-      <c r="DV1" s="81"/>
-      <c r="DW1" s="81"/>
-      <c r="DX1" s="81"/>
+      <c r="DU1" s="83"/>
+      <c r="DV1" s="83"/>
+      <c r="DW1" s="83"/>
+      <c r="DX1" s="83"/>
       <c r="DY1" s="12"/>
-      <c r="DZ1" s="80">
+      <c r="DZ1" s="82">
         <v>42343</v>
       </c>
-      <c r="EA1" s="81"/>
-      <c r="EB1" s="81"/>
-      <c r="EC1" s="81"/>
-      <c r="ED1" s="81"/>
+      <c r="EA1" s="83"/>
+      <c r="EB1" s="83"/>
+      <c r="EC1" s="83"/>
+      <c r="ED1" s="83"/>
       <c r="EE1" s="12"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -2624,7 +2624,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="84" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="14">
@@ -2774,7 +2774,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="82"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -2924,7 +2924,7 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="86" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="6">
@@ -3074,7 +3074,7 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3222,7 +3222,7 @@
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="84" t="s">
+      <c r="C12" s="86" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="6">
@@ -3384,7 +3384,7 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="84"/>
       <c r="D13" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3538,7 +3538,7 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="84"/>
       <c r="D14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -4162,7 +4162,7 @@
       <c r="AO18" s="7"/>
       <c r="AP18" s="8"/>
       <c r="AQ18" s="9"/>
-      <c r="AR18" s="89"/>
+      <c r="AR18" s="81"/>
       <c r="AS18" s="12"/>
       <c r="AT18" s="6"/>
       <c r="AU18" s="7"/>
@@ -5026,7 +5026,7 @@
       <c r="AO24" s="7"/>
       <c r="AP24" s="8"/>
       <c r="AQ24" s="9"/>
-      <c r="AR24" s="88"/>
+      <c r="AR24" s="80"/>
       <c r="AS24" s="12"/>
       <c r="AT24" s="6"/>
       <c r="AU24" s="7"/>
@@ -5128,7 +5128,7 @@
       <c r="B25" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="85" t="s">
+      <c r="C25" s="87" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="6"/>
@@ -5273,7 +5273,7 @@
       <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="86"/>
+      <c r="C26" s="88"/>
       <c r="D26" s="6"/>
       <c r="E26" s="7"/>
       <c r="F26" s="8"/>
@@ -5702,7 +5702,7 @@
       <c r="B29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="82" t="s">
+      <c r="C29" s="84" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="6"/>
@@ -5847,7 +5847,7 @@
       <c r="B30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="82"/>
+      <c r="C30" s="84"/>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
       <c r="F30" s="8"/>
@@ -5990,7 +5990,7 @@
       <c r="B31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="84"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -6854,7 +6854,7 @@
       <c r="B37" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="82" t="s">
+      <c r="C37" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="6"/>
@@ -6999,7 +6999,7 @@
       <c r="B38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="82"/>
+      <c r="C38" s="84"/>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
@@ -8035,7 +8035,7 @@
         <v>0</v>
       </c>
       <c r="AI45" s="58">
-        <v>6.25E-2</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="AJ45" s="59"/>
       <c r="AK45" s="60"/>
@@ -8922,7 +8922,7 @@
       <c r="B51" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="83" t="s">
+      <c r="C51" s="85" t="s">
         <v>20</v>
       </c>
       <c r="D51" s="14"/>
@@ -9065,7 +9065,7 @@
       <c r="B52" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="83"/>
+      <c r="C52" s="85"/>
       <c r="D52" s="14"/>
       <c r="E52" s="18"/>
       <c r="F52" s="8"/>
@@ -9921,7 +9921,7 @@
       <c r="B58" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C58" s="83" t="s">
+      <c r="C58" s="85" t="s">
         <v>30</v>
       </c>
       <c r="D58" s="14"/>
@@ -10064,7 +10064,7 @@
       <c r="B59" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="83"/>
+      <c r="C59" s="85"/>
       <c r="D59" s="14"/>
       <c r="E59" s="18"/>
       <c r="F59" s="18"/>
@@ -10205,7 +10205,7 @@
       <c r="B60" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="83"/>
+      <c r="C60" s="85"/>
       <c r="D60" s="14"/>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
@@ -10972,7 +10972,7 @@
       </c>
       <c r="AI64" s="29">
         <f>SUM(AI3:AI61)</f>
-        <v>0.22916666666666666</v>
+        <v>0.3125</v>
       </c>
       <c r="AJ64" s="30" t="s">
         <v>37</v>
@@ -12444,18 +12444,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="38" t="s">

</xml_diff>

<commit_message>
Ajuste em Prototipos. Modelagem de Classes Lancamento de atividades na planilha Envio das alterações do EA em XML para inclusao em arquivo unico.
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -795,14 +795,14 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1185,10 +1185,10 @@
   <dimension ref="A1:EE76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AD3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AA24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="AI46" sqref="AI46"/>
+      <selection pane="bottomRight" activeCell="AI39" sqref="AI39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1281,181 +1281,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="82">
+      <c r="D1" s="83">
         <v>42322</v>
       </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="82">
+      <c r="J1" s="83">
         <v>42323</v>
       </c>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
+      <c r="K1" s="84"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="82">
+      <c r="P1" s="83">
         <v>42324</v>
       </c>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="82">
+      <c r="V1" s="83">
         <v>42325</v>
       </c>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
       <c r="AA1" s="12"/>
-      <c r="AB1" s="82">
+      <c r="AB1" s="83">
         <v>42326</v>
       </c>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="82">
+      <c r="AH1" s="83">
         <v>42327</v>
       </c>
-      <c r="AI1" s="83"/>
-      <c r="AJ1" s="83"/>
-      <c r="AK1" s="83"/>
-      <c r="AL1" s="83"/>
+      <c r="AI1" s="84"/>
+      <c r="AJ1" s="84"/>
+      <c r="AK1" s="84"/>
+      <c r="AL1" s="84"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="82">
+      <c r="AN1" s="83">
         <v>42328</v>
       </c>
-      <c r="AO1" s="83"/>
-      <c r="AP1" s="83"/>
-      <c r="AQ1" s="83"/>
-      <c r="AR1" s="83"/>
+      <c r="AO1" s="84"/>
+      <c r="AP1" s="84"/>
+      <c r="AQ1" s="84"/>
+      <c r="AR1" s="84"/>
       <c r="AS1" s="12"/>
-      <c r="AT1" s="82">
+      <c r="AT1" s="83">
         <v>42329</v>
       </c>
-      <c r="AU1" s="83"/>
-      <c r="AV1" s="83"/>
-      <c r="AW1" s="83"/>
-      <c r="AX1" s="83"/>
+      <c r="AU1" s="84"/>
+      <c r="AV1" s="84"/>
+      <c r="AW1" s="84"/>
+      <c r="AX1" s="84"/>
       <c r="AY1" s="12"/>
-      <c r="AZ1" s="82">
+      <c r="AZ1" s="83">
         <v>42330</v>
       </c>
-      <c r="BA1" s="83"/>
-      <c r="BB1" s="83"/>
-      <c r="BC1" s="83"/>
-      <c r="BD1" s="83"/>
+      <c r="BA1" s="84"/>
+      <c r="BB1" s="84"/>
+      <c r="BC1" s="84"/>
+      <c r="BD1" s="84"/>
       <c r="BE1" s="12"/>
-      <c r="BF1" s="82">
+      <c r="BF1" s="83">
         <v>42331</v>
       </c>
-      <c r="BG1" s="83"/>
-      <c r="BH1" s="83"/>
-      <c r="BI1" s="83"/>
-      <c r="BJ1" s="83"/>
+      <c r="BG1" s="84"/>
+      <c r="BH1" s="84"/>
+      <c r="BI1" s="84"/>
+      <c r="BJ1" s="84"/>
       <c r="BK1" s="12"/>
-      <c r="BL1" s="82">
+      <c r="BL1" s="83">
         <v>42332</v>
       </c>
-      <c r="BM1" s="83"/>
-      <c r="BN1" s="83"/>
-      <c r="BO1" s="83"/>
-      <c r="BP1" s="83"/>
+      <c r="BM1" s="84"/>
+      <c r="BN1" s="84"/>
+      <c r="BO1" s="84"/>
+      <c r="BP1" s="84"/>
       <c r="BQ1" s="12"/>
-      <c r="BR1" s="82">
+      <c r="BR1" s="83">
         <v>42333</v>
       </c>
-      <c r="BS1" s="83"/>
-      <c r="BT1" s="83"/>
-      <c r="BU1" s="83"/>
-      <c r="BV1" s="83"/>
+      <c r="BS1" s="84"/>
+      <c r="BT1" s="84"/>
+      <c r="BU1" s="84"/>
+      <c r="BV1" s="84"/>
       <c r="BW1" s="12"/>
-      <c r="BX1" s="82">
+      <c r="BX1" s="83">
         <v>42334</v>
       </c>
-      <c r="BY1" s="83"/>
-      <c r="BZ1" s="83"/>
-      <c r="CA1" s="83"/>
-      <c r="CB1" s="83"/>
+      <c r="BY1" s="84"/>
+      <c r="BZ1" s="84"/>
+      <c r="CA1" s="84"/>
+      <c r="CB1" s="84"/>
       <c r="CC1" s="12"/>
-      <c r="CD1" s="82">
+      <c r="CD1" s="83">
         <v>42335</v>
       </c>
-      <c r="CE1" s="83"/>
-      <c r="CF1" s="83"/>
-      <c r="CG1" s="83"/>
-      <c r="CH1" s="83"/>
+      <c r="CE1" s="84"/>
+      <c r="CF1" s="84"/>
+      <c r="CG1" s="84"/>
+      <c r="CH1" s="84"/>
       <c r="CI1" s="12"/>
-      <c r="CJ1" s="82">
+      <c r="CJ1" s="83">
         <v>42336</v>
       </c>
-      <c r="CK1" s="83"/>
-      <c r="CL1" s="83"/>
-      <c r="CM1" s="83"/>
-      <c r="CN1" s="83"/>
+      <c r="CK1" s="84"/>
+      <c r="CL1" s="84"/>
+      <c r="CM1" s="84"/>
+      <c r="CN1" s="84"/>
       <c r="CO1" s="12"/>
-      <c r="CP1" s="82">
+      <c r="CP1" s="83">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="83"/>
-      <c r="CR1" s="83"/>
-      <c r="CS1" s="83"/>
-      <c r="CT1" s="83"/>
+      <c r="CQ1" s="84"/>
+      <c r="CR1" s="84"/>
+      <c r="CS1" s="84"/>
+      <c r="CT1" s="84"/>
       <c r="CU1" s="12"/>
-      <c r="CV1" s="82">
+      <c r="CV1" s="83">
         <v>42338</v>
       </c>
-      <c r="CW1" s="83"/>
-      <c r="CX1" s="83"/>
-      <c r="CY1" s="83"/>
-      <c r="CZ1" s="83"/>
+      <c r="CW1" s="84"/>
+      <c r="CX1" s="84"/>
+      <c r="CY1" s="84"/>
+      <c r="CZ1" s="84"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="82">
+      <c r="DB1" s="83">
         <v>42339</v>
       </c>
-      <c r="DC1" s="83"/>
-      <c r="DD1" s="83"/>
-      <c r="DE1" s="83"/>
-      <c r="DF1" s="83"/>
+      <c r="DC1" s="84"/>
+      <c r="DD1" s="84"/>
+      <c r="DE1" s="84"/>
+      <c r="DF1" s="84"/>
       <c r="DG1" s="12"/>
-      <c r="DH1" s="82">
+      <c r="DH1" s="83">
         <v>42340</v>
       </c>
-      <c r="DI1" s="83"/>
-      <c r="DJ1" s="83"/>
-      <c r="DK1" s="83"/>
-      <c r="DL1" s="83"/>
+      <c r="DI1" s="84"/>
+      <c r="DJ1" s="84"/>
+      <c r="DK1" s="84"/>
+      <c r="DL1" s="84"/>
       <c r="DM1" s="12"/>
-      <c r="DN1" s="82">
+      <c r="DN1" s="83">
         <v>42341</v>
       </c>
-      <c r="DO1" s="83"/>
-      <c r="DP1" s="83"/>
-      <c r="DQ1" s="83"/>
-      <c r="DR1" s="83"/>
+      <c r="DO1" s="84"/>
+      <c r="DP1" s="84"/>
+      <c r="DQ1" s="84"/>
+      <c r="DR1" s="84"/>
       <c r="DS1" s="12"/>
-      <c r="DT1" s="82">
+      <c r="DT1" s="83">
         <v>42342</v>
       </c>
-      <c r="DU1" s="83"/>
-      <c r="DV1" s="83"/>
-      <c r="DW1" s="83"/>
-      <c r="DX1" s="83"/>
+      <c r="DU1" s="84"/>
+      <c r="DV1" s="84"/>
+      <c r="DW1" s="84"/>
+      <c r="DX1" s="84"/>
       <c r="DY1" s="12"/>
-      <c r="DZ1" s="82">
+      <c r="DZ1" s="83">
         <v>42343</v>
       </c>
-      <c r="EA1" s="83"/>
-      <c r="EB1" s="83"/>
-      <c r="EC1" s="83"/>
-      <c r="ED1" s="83"/>
+      <c r="EA1" s="84"/>
+      <c r="EB1" s="84"/>
+      <c r="EC1" s="84"/>
+      <c r="ED1" s="84"/>
       <c r="EE1" s="12"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -2624,7 +2624,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="84" t="s">
+      <c r="C8" s="82" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="14">
@@ -2774,7 +2774,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="84"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3074,7 +3074,7 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="84"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3384,7 +3384,7 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="84"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3538,7 +3538,7 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="84"/>
+      <c r="C14" s="82"/>
       <c r="D14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -5702,7 +5702,7 @@
       <c r="B29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="84" t="s">
+      <c r="C29" s="82" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="6"/>
@@ -5847,7 +5847,7 @@
       <c r="B30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="84"/>
+      <c r="C30" s="82"/>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
       <c r="F30" s="8"/>
@@ -5990,7 +5990,7 @@
       <c r="B31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="84"/>
+      <c r="C31" s="82"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -6733,7 +6733,9 @@
       <c r="V36" s="56">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="W36" s="7"/>
+      <c r="W36" s="7">
+        <v>6.25E-2</v>
+      </c>
       <c r="X36" s="8"/>
       <c r="Y36" s="9"/>
       <c r="Z36" s="54"/>
@@ -6854,7 +6856,7 @@
       <c r="B37" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="84" t="s">
+      <c r="C37" s="82" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="6"/>
@@ -6999,7 +7001,7 @@
       <c r="B38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="84"/>
+      <c r="C38" s="82"/>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
@@ -7024,19 +7026,21 @@
       <c r="Y38" s="55"/>
       <c r="Z38" s="22"/>
       <c r="AA38" s="12"/>
-      <c r="AB38" s="6">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="AB38" s="6"/>
       <c r="AC38" s="7"/>
       <c r="AD38" s="8"/>
       <c r="AE38" s="9"/>
-      <c r="AF38" s="54"/>
+      <c r="AF38" s="10"/>
       <c r="AG38" s="12"/>
-      <c r="AH38" s="6"/>
-      <c r="AI38" s="7"/>
+      <c r="AH38" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="AI38" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="AJ38" s="8"/>
       <c r="AK38" s="9"/>
-      <c r="AL38" s="10"/>
+      <c r="AL38" s="54"/>
       <c r="AM38" s="12"/>
       <c r="AN38" s="6"/>
       <c r="AO38" s="7"/>
@@ -8172,19 +8176,20 @@
       <c r="Y46" s="9"/>
       <c r="Z46" s="10"/>
       <c r="AA46" s="12"/>
-      <c r="AB46" s="6"/>
-      <c r="AC46" s="7"/>
+      <c r="AB46" s="6">
+        <v>0.125</v>
+      </c>
+      <c r="AC46" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="AD46" s="8"/>
       <c r="AE46" s="9"/>
-      <c r="AF46" s="10"/>
+      <c r="AF46" s="54"/>
       <c r="AG46" s="12"/>
-      <c r="AH46" s="6">
-        <v>0.125</v>
-      </c>
+      <c r="AH46" s="6"/>
       <c r="AI46" s="7"/>
       <c r="AJ46" s="8"/>
       <c r="AK46" s="9"/>
-      <c r="AL46" s="54"/>
       <c r="AM46" s="12"/>
       <c r="AN46" s="6"/>
       <c r="AO46" s="7"/>
@@ -10940,7 +10945,7 @@
       </c>
       <c r="W64" s="29">
         <f>SUM(W3:W61)</f>
-        <v>0.22916666666666663</v>
+        <v>0.29166666666666663</v>
       </c>
       <c r="X64" s="30" t="s">
         <v>37</v>
@@ -10952,11 +10957,11 @@
       <c r="Z64" s="31"/>
       <c r="AB64" s="28">
         <f>SUM(AB3:AB61)</f>
-        <v>0.375</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="AC64" s="29">
         <f>SUM(AC3:AC61)</f>
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AD64" s="30" t="s">
         <v>37</v>
@@ -10968,11 +10973,11 @@
       <c r="AF64" s="31"/>
       <c r="AH64" s="28">
         <f>SUM(AH3:AH61)</f>
-        <v>0.29166666666666663</v>
+        <v>0.25</v>
       </c>
       <c r="AI64" s="29">
         <f>SUM(AI3:AI61)</f>
-        <v>0.3125</v>
+        <v>0.39583333333333337</v>
       </c>
       <c r="AJ64" s="30" t="s">
         <v>37</v>
@@ -12333,6 +12338,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="DN1:DR1"/>
+    <mergeCell ref="DT1:DX1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BL1:BP1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BX1:CB1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CP1:CT1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DB1:DF1"/>
+    <mergeCell ref="DH1:DL1"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="AH1:AL1"/>
     <mergeCell ref="AN1:AR1"/>
@@ -12345,24 +12368,6 @@
     <mergeCell ref="P1:T1"/>
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="C25:C26"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CP1:CT1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DB1:DF1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="DN1:DR1"/>
-    <mergeCell ref="DT1:DX1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BL1:BP1"/>
-    <mergeCell ref="BR1:BV1"/>
-    <mergeCell ref="BX1:CB1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="AB1:AF1"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Informações sobre a atualização: * Criação do documento prototipo.docx * Alteração dos protótipos (divisão dos protótipos do cadastrode proposta em arquivos separados do balsamiq e criação de pastas de diretórios para organização) * Revisão e alteração no diagrama de classes (criação de um novo arquivo para não dar erro com os já existentes) * Alteração da planilha de atividades com as horas trabalhadas no dia de hoje 20/11
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -795,14 +795,14 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1185,10 +1185,10 @@
   <dimension ref="A1:EE76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AA24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AK33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="AI39" sqref="AI39"/>
+      <selection pane="bottomRight" activeCell="AR45" sqref="AR45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1281,181 +1281,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="83">
+      <c r="D1" s="82">
         <v>42322</v>
       </c>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="83">
+      <c r="J1" s="82">
         <v>42323</v>
       </c>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="83">
+      <c r="P1" s="82">
         <v>42324</v>
       </c>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="83">
+      <c r="V1" s="82">
         <v>42325</v>
       </c>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
       <c r="AA1" s="12"/>
-      <c r="AB1" s="83">
+      <c r="AB1" s="82">
         <v>42326</v>
       </c>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="83"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="83">
+      <c r="AH1" s="82">
         <v>42327</v>
       </c>
-      <c r="AI1" s="84"/>
-      <c r="AJ1" s="84"/>
-      <c r="AK1" s="84"/>
-      <c r="AL1" s="84"/>
+      <c r="AI1" s="83"/>
+      <c r="AJ1" s="83"/>
+      <c r="AK1" s="83"/>
+      <c r="AL1" s="83"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="83">
+      <c r="AN1" s="82">
         <v>42328</v>
       </c>
-      <c r="AO1" s="84"/>
-      <c r="AP1" s="84"/>
-      <c r="AQ1" s="84"/>
-      <c r="AR1" s="84"/>
+      <c r="AO1" s="83"/>
+      <c r="AP1" s="83"/>
+      <c r="AQ1" s="83"/>
+      <c r="AR1" s="83"/>
       <c r="AS1" s="12"/>
-      <c r="AT1" s="83">
+      <c r="AT1" s="82">
         <v>42329</v>
       </c>
-      <c r="AU1" s="84"/>
-      <c r="AV1" s="84"/>
-      <c r="AW1" s="84"/>
-      <c r="AX1" s="84"/>
+      <c r="AU1" s="83"/>
+      <c r="AV1" s="83"/>
+      <c r="AW1" s="83"/>
+      <c r="AX1" s="83"/>
       <c r="AY1" s="12"/>
-      <c r="AZ1" s="83">
+      <c r="AZ1" s="82">
         <v>42330</v>
       </c>
-      <c r="BA1" s="84"/>
-      <c r="BB1" s="84"/>
-      <c r="BC1" s="84"/>
-      <c r="BD1" s="84"/>
+      <c r="BA1" s="83"/>
+      <c r="BB1" s="83"/>
+      <c r="BC1" s="83"/>
+      <c r="BD1" s="83"/>
       <c r="BE1" s="12"/>
-      <c r="BF1" s="83">
+      <c r="BF1" s="82">
         <v>42331</v>
       </c>
-      <c r="BG1" s="84"/>
-      <c r="BH1" s="84"/>
-      <c r="BI1" s="84"/>
-      <c r="BJ1" s="84"/>
+      <c r="BG1" s="83"/>
+      <c r="BH1" s="83"/>
+      <c r="BI1" s="83"/>
+      <c r="BJ1" s="83"/>
       <c r="BK1" s="12"/>
-      <c r="BL1" s="83">
+      <c r="BL1" s="82">
         <v>42332</v>
       </c>
-      <c r="BM1" s="84"/>
-      <c r="BN1" s="84"/>
-      <c r="BO1" s="84"/>
-      <c r="BP1" s="84"/>
+      <c r="BM1" s="83"/>
+      <c r="BN1" s="83"/>
+      <c r="BO1" s="83"/>
+      <c r="BP1" s="83"/>
       <c r="BQ1" s="12"/>
-      <c r="BR1" s="83">
+      <c r="BR1" s="82">
         <v>42333</v>
       </c>
-      <c r="BS1" s="84"/>
-      <c r="BT1" s="84"/>
-      <c r="BU1" s="84"/>
-      <c r="BV1" s="84"/>
+      <c r="BS1" s="83"/>
+      <c r="BT1" s="83"/>
+      <c r="BU1" s="83"/>
+      <c r="BV1" s="83"/>
       <c r="BW1" s="12"/>
-      <c r="BX1" s="83">
+      <c r="BX1" s="82">
         <v>42334</v>
       </c>
-      <c r="BY1" s="84"/>
-      <c r="BZ1" s="84"/>
-      <c r="CA1" s="84"/>
-      <c r="CB1" s="84"/>
+      <c r="BY1" s="83"/>
+      <c r="BZ1" s="83"/>
+      <c r="CA1" s="83"/>
+      <c r="CB1" s="83"/>
       <c r="CC1" s="12"/>
-      <c r="CD1" s="83">
+      <c r="CD1" s="82">
         <v>42335</v>
       </c>
-      <c r="CE1" s="84"/>
-      <c r="CF1" s="84"/>
-      <c r="CG1" s="84"/>
-      <c r="CH1" s="84"/>
+      <c r="CE1" s="83"/>
+      <c r="CF1" s="83"/>
+      <c r="CG1" s="83"/>
+      <c r="CH1" s="83"/>
       <c r="CI1" s="12"/>
-      <c r="CJ1" s="83">
+      <c r="CJ1" s="82">
         <v>42336</v>
       </c>
-      <c r="CK1" s="84"/>
-      <c r="CL1" s="84"/>
-      <c r="CM1" s="84"/>
-      <c r="CN1" s="84"/>
+      <c r="CK1" s="83"/>
+      <c r="CL1" s="83"/>
+      <c r="CM1" s="83"/>
+      <c r="CN1" s="83"/>
       <c r="CO1" s="12"/>
-      <c r="CP1" s="83">
+      <c r="CP1" s="82">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="84"/>
-      <c r="CR1" s="84"/>
-      <c r="CS1" s="84"/>
-      <c r="CT1" s="84"/>
+      <c r="CQ1" s="83"/>
+      <c r="CR1" s="83"/>
+      <c r="CS1" s="83"/>
+      <c r="CT1" s="83"/>
       <c r="CU1" s="12"/>
-      <c r="CV1" s="83">
+      <c r="CV1" s="82">
         <v>42338</v>
       </c>
-      <c r="CW1" s="84"/>
-      <c r="CX1" s="84"/>
-      <c r="CY1" s="84"/>
-      <c r="CZ1" s="84"/>
+      <c r="CW1" s="83"/>
+      <c r="CX1" s="83"/>
+      <c r="CY1" s="83"/>
+      <c r="CZ1" s="83"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="83">
+      <c r="DB1" s="82">
         <v>42339</v>
       </c>
-      <c r="DC1" s="84"/>
-      <c r="DD1" s="84"/>
-      <c r="DE1" s="84"/>
-      <c r="DF1" s="84"/>
+      <c r="DC1" s="83"/>
+      <c r="DD1" s="83"/>
+      <c r="DE1" s="83"/>
+      <c r="DF1" s="83"/>
       <c r="DG1" s="12"/>
-      <c r="DH1" s="83">
+      <c r="DH1" s="82">
         <v>42340</v>
       </c>
-      <c r="DI1" s="84"/>
-      <c r="DJ1" s="84"/>
-      <c r="DK1" s="84"/>
-      <c r="DL1" s="84"/>
+      <c r="DI1" s="83"/>
+      <c r="DJ1" s="83"/>
+      <c r="DK1" s="83"/>
+      <c r="DL1" s="83"/>
       <c r="DM1" s="12"/>
-      <c r="DN1" s="83">
+      <c r="DN1" s="82">
         <v>42341</v>
       </c>
-      <c r="DO1" s="84"/>
-      <c r="DP1" s="84"/>
-      <c r="DQ1" s="84"/>
-      <c r="DR1" s="84"/>
+      <c r="DO1" s="83"/>
+      <c r="DP1" s="83"/>
+      <c r="DQ1" s="83"/>
+      <c r="DR1" s="83"/>
       <c r="DS1" s="12"/>
-      <c r="DT1" s="83">
+      <c r="DT1" s="82">
         <v>42342</v>
       </c>
-      <c r="DU1" s="84"/>
-      <c r="DV1" s="84"/>
-      <c r="DW1" s="84"/>
-      <c r="DX1" s="84"/>
+      <c r="DU1" s="83"/>
+      <c r="DV1" s="83"/>
+      <c r="DW1" s="83"/>
+      <c r="DX1" s="83"/>
       <c r="DY1" s="12"/>
-      <c r="DZ1" s="83">
+      <c r="DZ1" s="82">
         <v>42343</v>
       </c>
-      <c r="EA1" s="84"/>
-      <c r="EB1" s="84"/>
-      <c r="EC1" s="84"/>
-      <c r="ED1" s="84"/>
+      <c r="EA1" s="83"/>
+      <c r="EB1" s="83"/>
+      <c r="EC1" s="83"/>
+      <c r="ED1" s="83"/>
       <c r="EE1" s="12"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -1890,7 +1890,9 @@
       <c r="AN3" s="71">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AO3" s="77"/>
+      <c r="AO3" s="72">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="AP3" s="74"/>
       <c r="AQ3" s="74"/>
       <c r="AR3" s="75"/>
@@ -2624,7 +2626,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="84" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="14">
@@ -2774,7 +2776,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="82"/>
+      <c r="C9" s="84"/>
       <c r="D9" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3074,7 +3076,7 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3384,7 +3386,7 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="84"/>
       <c r="D13" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3538,7 +3540,7 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="84"/>
       <c r="D14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -5702,7 +5704,7 @@
       <c r="B29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="82" t="s">
+      <c r="C29" s="84" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="6"/>
@@ -5847,7 +5849,7 @@
       <c r="B30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="82"/>
+      <c r="C30" s="84"/>
       <c r="D30" s="6"/>
       <c r="E30" s="7"/>
       <c r="F30" s="8"/>
@@ -5990,7 +5992,7 @@
       <c r="B31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="84"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -6856,7 +6858,7 @@
       <c r="B37" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="82" t="s">
+      <c r="C37" s="84" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="6"/>
@@ -6897,11 +6899,15 @@
       <c r="AK37" s="9"/>
       <c r="AL37" s="10"/>
       <c r="AM37" s="12"/>
-      <c r="AN37" s="6"/>
-      <c r="AO37" s="7"/>
+      <c r="AN37" s="6">
+        <v>0</v>
+      </c>
+      <c r="AO37" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="AP37" s="8"/>
       <c r="AQ37" s="9"/>
-      <c r="AR37" s="10"/>
+      <c r="AR37" s="70"/>
       <c r="AS37" s="12"/>
       <c r="AT37" s="6"/>
       <c r="AU37" s="7"/>
@@ -7001,7 +7007,7 @@
       <c r="B38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="82"/>
+      <c r="C38" s="84"/>
       <c r="D38" s="6"/>
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
@@ -8045,11 +8051,15 @@
       <c r="AK45" s="60"/>
       <c r="AL45" s="79"/>
       <c r="AM45" s="12"/>
-      <c r="AN45" s="6"/>
-      <c r="AO45" s="7"/>
+      <c r="AN45" s="6">
+        <v>0</v>
+      </c>
+      <c r="AO45" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="AP45" s="8"/>
       <c r="AQ45" s="9"/>
-      <c r="AR45" s="10"/>
+      <c r="AR45" s="53"/>
       <c r="AS45" s="12"/>
       <c r="AT45" s="6"/>
       <c r="AU45" s="7"/>
@@ -8335,7 +8345,9 @@
       <c r="AN47" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="AO47" s="7"/>
+      <c r="AO47" s="7">
+        <v>6.25E-2</v>
+      </c>
       <c r="AP47" s="8"/>
       <c r="AQ47" s="9"/>
       <c r="AR47" s="53"/>
@@ -10993,7 +11005,7 @@
       </c>
       <c r="AO64" s="29">
         <f>SUM(AO3:AO61)</f>
-        <v>0</v>
+        <v>0.14583333333333331</v>
       </c>
       <c r="AP64" s="30" t="s">
         <v>37</v>
@@ -11296,9 +11308,9 @@
       <c r="AN65" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="AO65" s="33" t="e">
+      <c r="AO65" s="33">
         <f>AQ64/AO64</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AR65" s="34"/>
       <c r="AT65" s="32" t="s">
@@ -11652,9 +11664,9 @@
       <c r="AN67" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AO67" s="35" t="e">
+      <c r="AO67" s="35">
         <f>1-AO65</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="AR67" s="34"/>
       <c r="AT67" s="32" t="s">
@@ -12338,6 +12350,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CP1:CT1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DB1:DF1"/>
+    <mergeCell ref="DH1:DL1"/>
     <mergeCell ref="AT1:AX1"/>
     <mergeCell ref="AZ1:BD1"/>
     <mergeCell ref="DN1:DR1"/>
@@ -12350,24 +12380,6 @@
     <mergeCell ref="BX1:CB1"/>
     <mergeCell ref="CD1:CH1"/>
     <mergeCell ref="AB1:AF1"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CP1:CT1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DB1:DF1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="AN1:AR1"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C25:C26"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizacao de horas trabalhadas
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -798,14 +798,17 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -821,9 +824,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1191,10 +1191,10 @@
   <dimension ref="A1:EE78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AS3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AW45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="BA4" sqref="BA4"/>
+      <selection pane="bottomRight" activeCell="CE46" sqref="CE46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2642,7 +2642,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="85" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="14">
@@ -2792,7 +2792,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="82"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -2942,7 +2942,7 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="87" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="6">
@@ -3092,7 +3092,7 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="82"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3240,7 +3240,7 @@
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="86" t="s">
+      <c r="C12" s="87" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="6">
@@ -3402,7 +3402,7 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="82"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3556,7 +3556,7 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="82"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -5293,7 +5293,7 @@
       <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="87" t="s">
+      <c r="C26" s="88" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="6"/>
@@ -5438,7 +5438,7 @@
       <c r="B27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="88"/>
+      <c r="C27" s="89"/>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
       <c r="F27" s="8"/>
@@ -5869,7 +5869,7 @@
       <c r="B30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="82" t="s">
+      <c r="C30" s="85" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="6"/>
@@ -6014,7 +6014,7 @@
       <c r="B31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="82"/>
+      <c r="C31" s="85"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -6157,7 +6157,7 @@
       <c r="B32" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="82"/>
+      <c r="C32" s="85"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
@@ -7027,7 +7027,7 @@
       <c r="B38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="82" t="s">
+      <c r="C38" s="85" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="6"/>
@@ -7170,7 +7170,7 @@
       <c r="B39" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="82"/>
+      <c r="C39" s="85"/>
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
@@ -8108,7 +8108,9 @@
       <c r="CD45" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="CE45" s="7"/>
+      <c r="CE45" s="7">
+        <v>0</v>
+      </c>
       <c r="CF45" s="8"/>
       <c r="CG45" s="9"/>
       <c r="CH45" s="54"/>
@@ -8803,16 +8805,20 @@
       <c r="AW50" s="18"/>
       <c r="AX50" s="10"/>
       <c r="AY50" s="12"/>
-      <c r="AZ50" s="14"/>
-      <c r="BA50" s="18"/>
+      <c r="AZ50" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="BA50" s="82">
+        <v>0.125</v>
+      </c>
       <c r="BB50" s="18"/>
       <c r="BC50" s="18"/>
-      <c r="BD50" s="10"/>
+      <c r="BD50" s="54"/>
       <c r="BE50" s="12"/>
       <c r="BF50" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BG50" s="18"/>
+      <c r="BG50" s="82"/>
       <c r="BH50" s="18"/>
       <c r="BI50" s="18"/>
       <c r="BJ50" s="52"/>
@@ -8966,16 +8972,22 @@
       <c r="AW51" s="18"/>
       <c r="AX51" s="10"/>
       <c r="AY51" s="12"/>
-      <c r="AZ51" s="14"/>
-      <c r="BA51" s="18"/>
+      <c r="AZ51" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="BA51" s="82">
+        <v>0.125</v>
+      </c>
       <c r="BB51" s="18"/>
       <c r="BC51" s="18"/>
-      <c r="BD51" s="10"/>
+      <c r="BD51" s="54"/>
       <c r="BE51" s="12"/>
       <c r="BF51" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BG51" s="18"/>
+      <c r="BG51" s="82">
+        <v>0.125</v>
+      </c>
       <c r="BH51" s="18"/>
       <c r="BI51" s="18"/>
       <c r="BJ51" s="54"/>
@@ -8983,7 +8995,9 @@
       <c r="BL51" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BM51" s="18"/>
+      <c r="BM51" s="82">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="BN51" s="18"/>
       <c r="BO51" s="18"/>
       <c r="BP51" s="54"/>
@@ -8991,7 +9005,9 @@
       <c r="BR51" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BS51" s="18"/>
+      <c r="BS51" s="82">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="BT51" s="18"/>
       <c r="BU51" s="18"/>
       <c r="BV51" s="54"/>
@@ -8999,7 +9015,9 @@
       <c r="BX51" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BY51" s="18"/>
+      <c r="BY51" s="82">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="BZ51" s="18"/>
       <c r="CA51" s="18"/>
       <c r="CB51" s="54"/>
@@ -9138,7 +9156,7 @@
       <c r="BF52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BG52" s="90">
+      <c r="BG52" s="82">
         <v>0</v>
       </c>
       <c r="BH52" s="18"/>
@@ -9148,7 +9166,7 @@
       <c r="BL52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BM52" s="90">
+      <c r="BM52" s="82">
         <v>0</v>
       </c>
       <c r="BN52" s="18"/>
@@ -9158,7 +9176,7 @@
       <c r="BR52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BS52" s="90">
+      <c r="BS52" s="82">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="BT52" s="18"/>
@@ -9168,7 +9186,7 @@
       <c r="BX52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BY52" s="90">
+      <c r="BY52" s="82">
         <v>6.25E-2</v>
       </c>
       <c r="BZ52" s="18"/>
@@ -9249,7 +9267,7 @@
       <c r="B53" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="85" t="s">
+      <c r="C53" s="86" t="s">
         <v>20</v>
       </c>
       <c r="D53" s="14"/>
@@ -9392,7 +9410,7 @@
       <c r="B54" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="85"/>
+      <c r="C54" s="86"/>
       <c r="D54" s="14"/>
       <c r="E54" s="18"/>
       <c r="F54" s="8"/>
@@ -10248,7 +10266,7 @@
       <c r="B60" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="85" t="s">
+      <c r="C60" s="86" t="s">
         <v>30</v>
       </c>
       <c r="D60" s="14"/>
@@ -10391,7 +10409,7 @@
       <c r="B61" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C61" s="85"/>
+      <c r="C61" s="86"/>
       <c r="D61" s="14"/>
       <c r="E61" s="18"/>
       <c r="F61" s="18"/>
@@ -10532,7 +10550,7 @@
       <c r="B62" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="85"/>
+      <c r="C62" s="86"/>
       <c r="D62" s="14"/>
       <c r="E62" s="18"/>
       <c r="F62" s="18"/>
@@ -11343,11 +11361,11 @@
       <c r="AX66" s="31"/>
       <c r="AZ66" s="28">
         <f>SUM(AZ3:AZ63)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="BA66" s="29">
         <f>SUM(BA3:BA63)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="BB66" s="30" t="s">
         <v>37</v>
@@ -11363,7 +11381,7 @@
       </c>
       <c r="BG66" s="29">
         <f>SUM(BG3:BG63)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="BH66" s="30" t="s">
         <v>37</v>
@@ -11379,7 +11397,7 @@
       </c>
       <c r="BM66" s="29">
         <f>SUM(BM3:BM63)</f>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="BN66" s="30" t="s">
         <v>37</v>
@@ -11395,7 +11413,7 @@
       </c>
       <c r="BS66" s="29">
         <f>SUM(BS3:BS63)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="BT66" s="30" t="s">
         <v>37</v>
@@ -11411,7 +11429,7 @@
       </c>
       <c r="BY66" s="29">
         <f>SUM(BY3:BY63)</f>
-        <v>6.25E-2</v>
+        <v>0.10416666666666666</v>
       </c>
       <c r="BZ66" s="30" t="s">
         <v>37</v>
@@ -11634,25 +11652,25 @@
       <c r="AZ67" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="BA67" s="33" t="e">
+      <c r="BA67" s="33">
         <f>BC66/BA66</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="BD67" s="34"/>
       <c r="BF67" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="BG67" s="33" t="e">
+      <c r="BG67" s="33">
         <f>BI66/BG66</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="BJ67" s="34"/>
       <c r="BL67" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="BM67" s="33" t="e">
+      <c r="BM67" s="33">
         <f>BO66/BM66</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="BP67" s="34"/>
       <c r="BR67" s="32" t="s">
@@ -11990,25 +12008,25 @@
       <c r="AZ69" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="BA69" s="35" t="e">
+      <c r="BA69" s="35">
         <f>1-BA67</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="BD69" s="34"/>
       <c r="BF69" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="BG69" s="35" t="e">
+      <c r="BG69" s="35">
         <f>1-BG67</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="BJ69" s="34"/>
       <c r="BL69" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="BM69" s="35" t="e">
+      <c r="BM69" s="35">
         <f>1-BM67</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="BP69" s="34"/>
       <c r="BR69" s="32" t="s">
@@ -12660,6 +12678,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CP1:CT1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DB1:DF1"/>
+    <mergeCell ref="DH1:DL1"/>
     <mergeCell ref="AT1:AX1"/>
     <mergeCell ref="AZ1:BD1"/>
     <mergeCell ref="DN1:DR1"/>
@@ -12672,24 +12708,6 @@
     <mergeCell ref="BX1:CB1"/>
     <mergeCell ref="CD1:CH1"/>
     <mergeCell ref="AB1:AF1"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CP1:CT1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DB1:DF1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="AN1:AR1"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -12770,18 +12788,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="90" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="89"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
+      <c r="A2" s="90"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="38" t="s">

</xml_diff>

<commit_message>
Readicionado importacao da fipe
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -798,17 +798,14 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -824,6 +821,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1191,10 +1191,10 @@
   <dimension ref="A1:EE78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AW45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AS3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="CE46" sqref="CE46"/>
+      <selection pane="bottomRight" activeCell="BA4" sqref="BA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2642,7 +2642,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="85" t="s">
+      <c r="C8" s="82" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="14">
@@ -2792,7 +2792,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="85"/>
+      <c r="C9" s="82"/>
       <c r="D9" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -2942,7 +2942,7 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="87" t="s">
+      <c r="C10" s="86" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="6">
@@ -3092,7 +3092,7 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="85"/>
+      <c r="C11" s="82"/>
       <c r="D11" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3240,7 +3240,7 @@
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="87" t="s">
+      <c r="C12" s="86" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="6">
@@ -3402,7 +3402,7 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="85"/>
+      <c r="C13" s="82"/>
       <c r="D13" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3556,7 +3556,7 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="85"/>
+      <c r="C14" s="82"/>
       <c r="D14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -5293,7 +5293,7 @@
       <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="88" t="s">
+      <c r="C26" s="87" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="6"/>
@@ -5438,7 +5438,7 @@
       <c r="B27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="89"/>
+      <c r="C27" s="88"/>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
       <c r="F27" s="8"/>
@@ -5869,7 +5869,7 @@
       <c r="B30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="85" t="s">
+      <c r="C30" s="82" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="6"/>
@@ -6014,7 +6014,7 @@
       <c r="B31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="85"/>
+      <c r="C31" s="82"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -6157,7 +6157,7 @@
       <c r="B32" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="85"/>
+      <c r="C32" s="82"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
@@ -7027,7 +7027,7 @@
       <c r="B38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="85" t="s">
+      <c r="C38" s="82" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="6"/>
@@ -7170,7 +7170,7 @@
       <c r="B39" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="85"/>
+      <c r="C39" s="82"/>
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
@@ -8108,9 +8108,7 @@
       <c r="CD45" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="CE45" s="7">
-        <v>0</v>
-      </c>
+      <c r="CE45" s="7"/>
       <c r="CF45" s="8"/>
       <c r="CG45" s="9"/>
       <c r="CH45" s="54"/>
@@ -8805,20 +8803,16 @@
       <c r="AW50" s="18"/>
       <c r="AX50" s="10"/>
       <c r="AY50" s="12"/>
-      <c r="AZ50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="BA50" s="82">
-        <v>0.125</v>
-      </c>
+      <c r="AZ50" s="14"/>
+      <c r="BA50" s="18"/>
       <c r="BB50" s="18"/>
       <c r="BC50" s="18"/>
-      <c r="BD50" s="54"/>
+      <c r="BD50" s="10"/>
       <c r="BE50" s="12"/>
       <c r="BF50" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BG50" s="82"/>
+      <c r="BG50" s="18"/>
       <c r="BH50" s="18"/>
       <c r="BI50" s="18"/>
       <c r="BJ50" s="52"/>
@@ -8972,22 +8966,16 @@
       <c r="AW51" s="18"/>
       <c r="AX51" s="10"/>
       <c r="AY51" s="12"/>
-      <c r="AZ51" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="BA51" s="82">
-        <v>0.125</v>
-      </c>
+      <c r="AZ51" s="14"/>
+      <c r="BA51" s="18"/>
       <c r="BB51" s="18"/>
       <c r="BC51" s="18"/>
-      <c r="BD51" s="54"/>
+      <c r="BD51" s="10"/>
       <c r="BE51" s="12"/>
       <c r="BF51" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BG51" s="82">
-        <v>0.125</v>
-      </c>
+      <c r="BG51" s="18"/>
       <c r="BH51" s="18"/>
       <c r="BI51" s="18"/>
       <c r="BJ51" s="54"/>
@@ -8995,9 +8983,7 @@
       <c r="BL51" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BM51" s="82">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="BM51" s="18"/>
       <c r="BN51" s="18"/>
       <c r="BO51" s="18"/>
       <c r="BP51" s="54"/>
@@ -9005,9 +8991,7 @@
       <c r="BR51" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BS51" s="82">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="BS51" s="18"/>
       <c r="BT51" s="18"/>
       <c r="BU51" s="18"/>
       <c r="BV51" s="54"/>
@@ -9015,9 +8999,7 @@
       <c r="BX51" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BY51" s="82">
-        <v>4.1666666666666664E-2</v>
-      </c>
+      <c r="BY51" s="18"/>
       <c r="BZ51" s="18"/>
       <c r="CA51" s="18"/>
       <c r="CB51" s="54"/>
@@ -9156,7 +9138,7 @@
       <c r="BF52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BG52" s="82">
+      <c r="BG52" s="90">
         <v>0</v>
       </c>
       <c r="BH52" s="18"/>
@@ -9166,7 +9148,7 @@
       <c r="BL52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BM52" s="82">
+      <c r="BM52" s="90">
         <v>0</v>
       </c>
       <c r="BN52" s="18"/>
@@ -9176,7 +9158,7 @@
       <c r="BR52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BS52" s="82">
+      <c r="BS52" s="90">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="BT52" s="18"/>
@@ -9186,7 +9168,7 @@
       <c r="BX52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BY52" s="82">
+      <c r="BY52" s="90">
         <v>6.25E-2</v>
       </c>
       <c r="BZ52" s="18"/>
@@ -9267,7 +9249,7 @@
       <c r="B53" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="86" t="s">
+      <c r="C53" s="85" t="s">
         <v>20</v>
       </c>
       <c r="D53" s="14"/>
@@ -9410,7 +9392,7 @@
       <c r="B54" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="86"/>
+      <c r="C54" s="85"/>
       <c r="D54" s="14"/>
       <c r="E54" s="18"/>
       <c r="F54" s="8"/>
@@ -10266,7 +10248,7 @@
       <c r="B60" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="86" t="s">
+      <c r="C60" s="85" t="s">
         <v>30</v>
       </c>
       <c r="D60" s="14"/>
@@ -10409,7 +10391,7 @@
       <c r="B61" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C61" s="86"/>
+      <c r="C61" s="85"/>
       <c r="D61" s="14"/>
       <c r="E61" s="18"/>
       <c r="F61" s="18"/>
@@ -10550,7 +10532,7 @@
       <c r="B62" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="86"/>
+      <c r="C62" s="85"/>
       <c r="D62" s="14"/>
       <c r="E62" s="18"/>
       <c r="F62" s="18"/>
@@ -11361,11 +11343,11 @@
       <c r="AX66" s="31"/>
       <c r="AZ66" s="28">
         <f>SUM(AZ3:AZ63)</f>
-        <v>0.20833333333333331</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="BA66" s="29">
         <f>SUM(BA3:BA63)</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="BB66" s="30" t="s">
         <v>37</v>
@@ -11381,7 +11363,7 @@
       </c>
       <c r="BG66" s="29">
         <f>SUM(BG3:BG63)</f>
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="BH66" s="30" t="s">
         <v>37</v>
@@ -11397,7 +11379,7 @@
       </c>
       <c r="BM66" s="29">
         <f>SUM(BM3:BM63)</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0</v>
       </c>
       <c r="BN66" s="30" t="s">
         <v>37</v>
@@ -11413,7 +11395,7 @@
       </c>
       <c r="BS66" s="29">
         <f>SUM(BS3:BS63)</f>
-        <v>6.25E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="BT66" s="30" t="s">
         <v>37</v>
@@ -11429,7 +11411,7 @@
       </c>
       <c r="BY66" s="29">
         <f>SUM(BY3:BY63)</f>
-        <v>0.10416666666666666</v>
+        <v>6.25E-2</v>
       </c>
       <c r="BZ66" s="30" t="s">
         <v>37</v>
@@ -11652,25 +11634,25 @@
       <c r="AZ67" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="BA67" s="33">
+      <c r="BA67" s="33" t="e">
         <f>BC66/BA66</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="BD67" s="34"/>
       <c r="BF67" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="BG67" s="33">
+      <c r="BG67" s="33" t="e">
         <f>BI66/BG66</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="BJ67" s="34"/>
       <c r="BL67" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="BM67" s="33">
+      <c r="BM67" s="33" t="e">
         <f>BO66/BM66</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="BP67" s="34"/>
       <c r="BR67" s="32" t="s">
@@ -12008,25 +11990,25 @@
       <c r="AZ69" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="BA69" s="35">
+      <c r="BA69" s="35" t="e">
         <f>1-BA67</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="BD69" s="34"/>
       <c r="BF69" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="BG69" s="35">
+      <c r="BG69" s="35" t="e">
         <f>1-BG67</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="BJ69" s="34"/>
       <c r="BL69" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="BM69" s="35">
+      <c r="BM69" s="35" t="e">
         <f>1-BM67</f>
-        <v>1</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="BP69" s="34"/>
       <c r="BR69" s="32" t="s">
@@ -12678,6 +12660,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="DN1:DR1"/>
+    <mergeCell ref="DT1:DX1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BL1:BP1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BX1:CB1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CP1:CT1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DB1:DF1"/>
+    <mergeCell ref="DH1:DL1"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="AH1:AL1"/>
     <mergeCell ref="AN1:AR1"/>
@@ -12690,24 +12690,6 @@
     <mergeCell ref="P1:T1"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CP1:CT1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DB1:DF1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="DN1:DR1"/>
-    <mergeCell ref="DT1:DX1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BL1:BP1"/>
-    <mergeCell ref="BR1:BV1"/>
-    <mergeCell ref="BX1:CB1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="AB1:AF1"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -12788,18 +12770,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="90"/>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
+      <c r="A2" s="89"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="38" t="s">

</xml_diff>

<commit_message>
Atualização da planilha de atividades
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -807,14 +807,20 @@
     <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -830,12 +836,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1203,10 +1203,10 @@
   <dimension ref="A1:EE80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="DJ3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="CZ3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="DV3" sqref="DV3"/>
+      <selection pane="bottomRight" activeCell="DL51" sqref="DL51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1298,181 +1298,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="84">
+      <c r="D1" s="87">
         <v>42322</v>
       </c>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="84">
+      <c r="J1" s="87">
         <v>42323</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="84">
+      <c r="P1" s="87">
         <v>42324</v>
       </c>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
+      <c r="T1" s="88"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="84">
+      <c r="V1" s="87">
         <v>42325</v>
       </c>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="85"/>
-      <c r="Z1" s="85"/>
+      <c r="W1" s="88"/>
+      <c r="X1" s="88"/>
+      <c r="Y1" s="88"/>
+      <c r="Z1" s="88"/>
       <c r="AA1" s="12"/>
-      <c r="AB1" s="84">
+      <c r="AB1" s="87">
         <v>42326</v>
       </c>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="85"/>
-      <c r="AF1" s="85"/>
+      <c r="AC1" s="88"/>
+      <c r="AD1" s="88"/>
+      <c r="AE1" s="88"/>
+      <c r="AF1" s="88"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="84">
+      <c r="AH1" s="87">
         <v>42327</v>
       </c>
-      <c r="AI1" s="85"/>
-      <c r="AJ1" s="85"/>
-      <c r="AK1" s="85"/>
-      <c r="AL1" s="85"/>
+      <c r="AI1" s="88"/>
+      <c r="AJ1" s="88"/>
+      <c r="AK1" s="88"/>
+      <c r="AL1" s="88"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="84">
+      <c r="AN1" s="87">
         <v>42328</v>
       </c>
-      <c r="AO1" s="85"/>
-      <c r="AP1" s="85"/>
-      <c r="AQ1" s="85"/>
-      <c r="AR1" s="85"/>
+      <c r="AO1" s="88"/>
+      <c r="AP1" s="88"/>
+      <c r="AQ1" s="88"/>
+      <c r="AR1" s="88"/>
       <c r="AS1" s="12"/>
-      <c r="AT1" s="84">
+      <c r="AT1" s="87">
         <v>42329</v>
       </c>
-      <c r="AU1" s="85"/>
-      <c r="AV1" s="85"/>
-      <c r="AW1" s="85"/>
-      <c r="AX1" s="85"/>
+      <c r="AU1" s="88"/>
+      <c r="AV1" s="88"/>
+      <c r="AW1" s="88"/>
+      <c r="AX1" s="88"/>
       <c r="AY1" s="12"/>
-      <c r="AZ1" s="84">
+      <c r="AZ1" s="87">
         <v>42330</v>
       </c>
-      <c r="BA1" s="85"/>
-      <c r="BB1" s="85"/>
-      <c r="BC1" s="85"/>
-      <c r="BD1" s="85"/>
+      <c r="BA1" s="88"/>
+      <c r="BB1" s="88"/>
+      <c r="BC1" s="88"/>
+      <c r="BD1" s="88"/>
       <c r="BE1" s="12"/>
-      <c r="BF1" s="84">
+      <c r="BF1" s="87">
         <v>42331</v>
       </c>
-      <c r="BG1" s="85"/>
-      <c r="BH1" s="85"/>
-      <c r="BI1" s="85"/>
-      <c r="BJ1" s="85"/>
+      <c r="BG1" s="88"/>
+      <c r="BH1" s="88"/>
+      <c r="BI1" s="88"/>
+      <c r="BJ1" s="88"/>
       <c r="BK1" s="12"/>
-      <c r="BL1" s="84">
+      <c r="BL1" s="87">
         <v>42332</v>
       </c>
-      <c r="BM1" s="85"/>
-      <c r="BN1" s="85"/>
-      <c r="BO1" s="85"/>
-      <c r="BP1" s="85"/>
+      <c r="BM1" s="88"/>
+      <c r="BN1" s="88"/>
+      <c r="BO1" s="88"/>
+      <c r="BP1" s="88"/>
       <c r="BQ1" s="12"/>
-      <c r="BR1" s="84">
+      <c r="BR1" s="87">
         <v>42333</v>
       </c>
-      <c r="BS1" s="85"/>
-      <c r="BT1" s="85"/>
-      <c r="BU1" s="85"/>
-      <c r="BV1" s="85"/>
+      <c r="BS1" s="88"/>
+      <c r="BT1" s="88"/>
+      <c r="BU1" s="88"/>
+      <c r="BV1" s="88"/>
       <c r="BW1" s="12"/>
-      <c r="BX1" s="84">
+      <c r="BX1" s="87">
         <v>42334</v>
       </c>
-      <c r="BY1" s="85"/>
-      <c r="BZ1" s="85"/>
-      <c r="CA1" s="85"/>
-      <c r="CB1" s="85"/>
+      <c r="BY1" s="88"/>
+      <c r="BZ1" s="88"/>
+      <c r="CA1" s="88"/>
+      <c r="CB1" s="88"/>
       <c r="CC1" s="12"/>
-      <c r="CD1" s="84">
+      <c r="CD1" s="87">
         <v>42335</v>
       </c>
-      <c r="CE1" s="85"/>
-      <c r="CF1" s="85"/>
-      <c r="CG1" s="85"/>
-      <c r="CH1" s="85"/>
+      <c r="CE1" s="88"/>
+      <c r="CF1" s="88"/>
+      <c r="CG1" s="88"/>
+      <c r="CH1" s="88"/>
       <c r="CI1" s="12"/>
-      <c r="CJ1" s="84">
+      <c r="CJ1" s="87">
         <v>42336</v>
       </c>
-      <c r="CK1" s="85"/>
-      <c r="CL1" s="85"/>
-      <c r="CM1" s="85"/>
-      <c r="CN1" s="85"/>
+      <c r="CK1" s="88"/>
+      <c r="CL1" s="88"/>
+      <c r="CM1" s="88"/>
+      <c r="CN1" s="88"/>
       <c r="CO1" s="12"/>
-      <c r="CP1" s="84">
+      <c r="CP1" s="87">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="85"/>
-      <c r="CR1" s="85"/>
-      <c r="CS1" s="85"/>
-      <c r="CT1" s="85"/>
+      <c r="CQ1" s="88"/>
+      <c r="CR1" s="88"/>
+      <c r="CS1" s="88"/>
+      <c r="CT1" s="88"/>
       <c r="CU1" s="12"/>
-      <c r="CV1" s="84">
+      <c r="CV1" s="87">
         <v>42338</v>
       </c>
-      <c r="CW1" s="85"/>
-      <c r="CX1" s="85"/>
-      <c r="CY1" s="85"/>
-      <c r="CZ1" s="85"/>
+      <c r="CW1" s="88"/>
+      <c r="CX1" s="88"/>
+      <c r="CY1" s="88"/>
+      <c r="CZ1" s="88"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="84">
+      <c r="DB1" s="87">
         <v>42339</v>
       </c>
-      <c r="DC1" s="85"/>
-      <c r="DD1" s="85"/>
-      <c r="DE1" s="85"/>
-      <c r="DF1" s="85"/>
+      <c r="DC1" s="88"/>
+      <c r="DD1" s="88"/>
+      <c r="DE1" s="88"/>
+      <c r="DF1" s="88"/>
       <c r="DG1" s="12"/>
-      <c r="DH1" s="84">
+      <c r="DH1" s="87">
         <v>42340</v>
       </c>
-      <c r="DI1" s="85"/>
-      <c r="DJ1" s="85"/>
-      <c r="DK1" s="85"/>
-      <c r="DL1" s="85"/>
+      <c r="DI1" s="88"/>
+      <c r="DJ1" s="88"/>
+      <c r="DK1" s="88"/>
+      <c r="DL1" s="88"/>
       <c r="DM1" s="12"/>
-      <c r="DN1" s="84">
+      <c r="DN1" s="87">
         <v>42341</v>
       </c>
-      <c r="DO1" s="85"/>
-      <c r="DP1" s="85"/>
-      <c r="DQ1" s="85"/>
-      <c r="DR1" s="85"/>
+      <c r="DO1" s="88"/>
+      <c r="DP1" s="88"/>
+      <c r="DQ1" s="88"/>
+      <c r="DR1" s="88"/>
       <c r="DS1" s="12"/>
-      <c r="DT1" s="84">
+      <c r="DT1" s="87">
         <v>42342</v>
       </c>
-      <c r="DU1" s="85"/>
-      <c r="DV1" s="85"/>
-      <c r="DW1" s="85"/>
-      <c r="DX1" s="85"/>
+      <c r="DU1" s="88"/>
+      <c r="DV1" s="88"/>
+      <c r="DW1" s="88"/>
+      <c r="DX1" s="88"/>
       <c r="DY1" s="12"/>
-      <c r="DZ1" s="84">
+      <c r="DZ1" s="87">
         <v>42343</v>
       </c>
-      <c r="EA1" s="85"/>
-      <c r="EB1" s="85"/>
-      <c r="EC1" s="85"/>
-      <c r="ED1" s="85"/>
+      <c r="EA1" s="88"/>
+      <c r="EB1" s="88"/>
+      <c r="EC1" s="88"/>
+      <c r="ED1" s="88"/>
       <c r="EE1" s="12"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -2025,7 +2025,9 @@
       <c r="DH3" s="71">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="DI3" s="77"/>
+      <c r="DI3" s="72">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="DJ3" s="74"/>
       <c r="DK3" s="74"/>
       <c r="DL3" s="75"/>
@@ -2962,7 +2964,7 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="88" t="s">
+      <c r="C10" s="90" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="6">
@@ -3260,7 +3262,7 @@
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="90" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="6">
@@ -5313,7 +5315,7 @@
       <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="89" t="s">
+      <c r="C26" s="91" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="6"/>
@@ -5458,7 +5460,7 @@
       <c r="B27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="90"/>
+      <c r="C27" s="92"/>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
       <c r="F27" s="8"/>
@@ -8910,7 +8912,9 @@
       <c r="DH50" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DI50" s="18"/>
+      <c r="DI50" s="83">
+        <v>0</v>
+      </c>
       <c r="DJ50" s="18"/>
       <c r="DK50" s="18"/>
       <c r="DL50" s="52"/>
@@ -9429,7 +9433,9 @@
       <c r="DH53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DI53" s="18"/>
+      <c r="DI53" s="83">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="DJ53" s="18"/>
       <c r="DK53" s="18"/>
       <c r="DL53" s="53"/>
@@ -9462,7 +9468,7 @@
       <c r="B54" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="87" t="s">
+      <c r="C54" s="89" t="s">
         <v>20</v>
       </c>
       <c r="D54" s="14"/>
@@ -9605,7 +9611,7 @@
       <c r="B55" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="87"/>
+      <c r="C55" s="89"/>
       <c r="D55" s="14"/>
       <c r="E55" s="18"/>
       <c r="F55" s="8"/>
@@ -9887,112 +9893,112 @@
       <c r="B57" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C57" s="93" t="s">
+      <c r="C57" s="85" t="s">
         <v>90</v>
       </c>
-      <c r="D57" s="92"/>
+      <c r="D57" s="84"/>
       <c r="E57" s="18"/>
       <c r="F57" s="8"/>
       <c r="G57" s="18"/>
       <c r="H57" s="10"/>
       <c r="I57" s="12"/>
-      <c r="J57" s="92"/>
+      <c r="J57" s="84"/>
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
       <c r="M57" s="18"/>
       <c r="N57" s="10"/>
       <c r="O57" s="12"/>
-      <c r="P57" s="92"/>
+      <c r="P57" s="84"/>
       <c r="Q57" s="18"/>
       <c r="R57" s="18"/>
       <c r="S57" s="18"/>
       <c r="T57" s="10"/>
       <c r="U57" s="12"/>
-      <c r="V57" s="92"/>
+      <c r="V57" s="84"/>
       <c r="W57" s="18"/>
       <c r="X57" s="18"/>
       <c r="Y57" s="18"/>
       <c r="Z57" s="10"/>
       <c r="AA57" s="12"/>
-      <c r="AB57" s="92"/>
+      <c r="AB57" s="84"/>
       <c r="AC57" s="18"/>
       <c r="AD57" s="18"/>
       <c r="AE57" s="18"/>
       <c r="AF57" s="10"/>
       <c r="AG57" s="12"/>
-      <c r="AH57" s="92"/>
+      <c r="AH57" s="84"/>
       <c r="AI57" s="18"/>
       <c r="AJ57" s="18"/>
       <c r="AK57" s="18"/>
       <c r="AL57" s="10"/>
       <c r="AM57" s="12"/>
-      <c r="AN57" s="92"/>
+      <c r="AN57" s="84"/>
       <c r="AO57" s="18"/>
       <c r="AP57" s="18"/>
       <c r="AQ57" s="18"/>
       <c r="AR57" s="10"/>
       <c r="AS57" s="12"/>
-      <c r="AT57" s="92"/>
+      <c r="AT57" s="84"/>
       <c r="AU57" s="18"/>
       <c r="AV57" s="18"/>
       <c r="AW57" s="18"/>
       <c r="AX57" s="10"/>
       <c r="AY57" s="12"/>
-      <c r="AZ57" s="92"/>
+      <c r="AZ57" s="84"/>
       <c r="BA57" s="18"/>
       <c r="BB57" s="18"/>
       <c r="BC57" s="18"/>
       <c r="BD57" s="10"/>
       <c r="BE57" s="12"/>
-      <c r="BF57" s="92"/>
+      <c r="BF57" s="84"/>
       <c r="BG57" s="18"/>
       <c r="BH57" s="18"/>
       <c r="BI57" s="18"/>
       <c r="BJ57" s="10"/>
       <c r="BK57" s="12"/>
-      <c r="BL57" s="92"/>
+      <c r="BL57" s="84"/>
       <c r="BM57" s="18"/>
       <c r="BN57" s="18"/>
       <c r="BO57" s="18"/>
       <c r="BP57" s="10"/>
       <c r="BQ57" s="12"/>
-      <c r="BR57" s="92"/>
+      <c r="BR57" s="84"/>
       <c r="BS57" s="18"/>
       <c r="BT57" s="18"/>
       <c r="BU57" s="18"/>
       <c r="BV57" s="10"/>
       <c r="BW57" s="12"/>
-      <c r="BX57" s="92"/>
+      <c r="BX57" s="84"/>
       <c r="BY57" s="18"/>
       <c r="BZ57" s="18"/>
       <c r="CA57" s="18"/>
       <c r="CB57" s="10"/>
       <c r="CC57" s="12"/>
-      <c r="CD57" s="92"/>
+      <c r="CD57" s="84"/>
       <c r="CE57" s="18"/>
       <c r="CF57" s="18"/>
       <c r="CG57" s="18"/>
       <c r="CH57" s="10"/>
       <c r="CI57" s="12"/>
-      <c r="CJ57" s="92"/>
+      <c r="CJ57" s="84"/>
       <c r="CK57" s="18"/>
       <c r="CL57" s="18"/>
       <c r="CM57" s="18"/>
       <c r="CN57" s="10"/>
       <c r="CO57" s="12"/>
-      <c r="CP57" s="92"/>
+      <c r="CP57" s="84"/>
       <c r="CQ57" s="18"/>
       <c r="CR57" s="18"/>
       <c r="CS57" s="18"/>
       <c r="CT57" s="10"/>
       <c r="CU57" s="12"/>
-      <c r="CV57" s="92"/>
+      <c r="CV57" s="84"/>
       <c r="CW57" s="18"/>
       <c r="CX57" s="18"/>
       <c r="CY57" s="18"/>
       <c r="CZ57" s="10"/>
       <c r="DA57" s="12"/>
-      <c r="DB57" s="92">
+      <c r="DB57" s="84">
         <v>0</v>
       </c>
       <c r="DC57" s="83">
@@ -10002,25 +10008,25 @@
       <c r="DE57" s="18"/>
       <c r="DF57" s="53"/>
       <c r="DG57" s="12"/>
-      <c r="DH57" s="92"/>
+      <c r="DH57" s="84"/>
       <c r="DI57" s="18"/>
       <c r="DJ57" s="18"/>
       <c r="DK57" s="18"/>
       <c r="DL57" s="10"/>
       <c r="DM57" s="12"/>
-      <c r="DN57" s="92"/>
+      <c r="DN57" s="84"/>
       <c r="DO57" s="18"/>
       <c r="DP57" s="18"/>
       <c r="DQ57" s="18"/>
       <c r="DR57" s="10"/>
       <c r="DS57" s="12"/>
-      <c r="DT57" s="92"/>
+      <c r="DT57" s="84"/>
       <c r="DU57" s="18"/>
       <c r="DV57" s="18"/>
       <c r="DW57" s="18"/>
       <c r="DX57" s="10"/>
       <c r="DY57" s="12"/>
-      <c r="DZ57" s="92"/>
+      <c r="DZ57" s="84"/>
       <c r="EA57" s="18"/>
       <c r="EB57" s="18"/>
       <c r="EC57" s="18"/>
@@ -10606,7 +10612,7 @@
       <c r="B62" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="87" t="s">
+      <c r="C62" s="89" t="s">
         <v>30</v>
       </c>
       <c r="D62" s="14"/>
@@ -10749,7 +10755,7 @@
       <c r="B63" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C63" s="87"/>
+      <c r="C63" s="89"/>
       <c r="D63" s="14"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
@@ -10890,7 +10896,7 @@
       <c r="B64" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C64" s="87"/>
+      <c r="C64" s="89"/>
       <c r="D64" s="14"/>
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
@@ -11865,7 +11871,7 @@
       </c>
       <c r="DI68" s="29">
         <f>SUM(DI3:DI65)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="DJ68" s="30" t="s">
         <v>37</v>
@@ -12072,9 +12078,9 @@
       <c r="DH69" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="DI69" s="33" t="e">
+      <c r="DI69" s="33">
         <f>DK68/DI68</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="DL69" s="34"/>
       <c r="DN69" s="32" t="s">
@@ -12428,9 +12434,9 @@
       <c r="DH71" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="DI71" s="35" t="e">
+      <c r="DI71" s="35">
         <f>1-DI69</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="DL71" s="34"/>
       <c r="DN71" s="32" t="s">
@@ -13018,6 +13024,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="DN1:DR1"/>
+    <mergeCell ref="DT1:DX1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BL1:BP1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BX1:CB1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CP1:CT1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DB1:DF1"/>
+    <mergeCell ref="DH1:DL1"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="AH1:AL1"/>
     <mergeCell ref="AN1:AR1"/>
@@ -13030,24 +13054,6 @@
     <mergeCell ref="P1:T1"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CP1:CT1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DB1:DF1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="DN1:DR1"/>
-    <mergeCell ref="DT1:DX1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BL1:BP1"/>
-    <mergeCell ref="BR1:BV1"/>
-    <mergeCell ref="BX1:CB1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="AB1:AF1"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -13128,18 +13134,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="91"/>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="38" t="s">

</xml_diff>

<commit_message>
Atualização da planilha de atividades (horas do dia 02/12 do Ricardo)
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -813,14 +813,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1203,10 +1203,10 @@
   <dimension ref="A1:EE80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="CZ3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="CZ46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="DL51" sqref="DL51"/>
+      <selection pane="bottomRight" activeCell="DI61" sqref="DI61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1298,181 +1298,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="87">
+      <c r="D1" s="86">
         <v>42322</v>
       </c>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="87">
+      <c r="J1" s="86">
         <v>42323</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="87">
+      <c r="P1" s="86">
         <v>42324</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-      <c r="T1" s="88"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="S1" s="87"/>
+      <c r="T1" s="87"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="87">
+      <c r="V1" s="86">
         <v>42325</v>
       </c>
-      <c r="W1" s="88"/>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="88"/>
+      <c r="W1" s="87"/>
+      <c r="X1" s="87"/>
+      <c r="Y1" s="87"/>
+      <c r="Z1" s="87"/>
       <c r="AA1" s="12"/>
-      <c r="AB1" s="87">
+      <c r="AB1" s="86">
         <v>42326</v>
       </c>
-      <c r="AC1" s="88"/>
-      <c r="AD1" s="88"/>
-      <c r="AE1" s="88"/>
-      <c r="AF1" s="88"/>
+      <c r="AC1" s="87"/>
+      <c r="AD1" s="87"/>
+      <c r="AE1" s="87"/>
+      <c r="AF1" s="87"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="87">
+      <c r="AH1" s="86">
         <v>42327</v>
       </c>
-      <c r="AI1" s="88"/>
-      <c r="AJ1" s="88"/>
-      <c r="AK1" s="88"/>
-      <c r="AL1" s="88"/>
+      <c r="AI1" s="87"/>
+      <c r="AJ1" s="87"/>
+      <c r="AK1" s="87"/>
+      <c r="AL1" s="87"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="87">
+      <c r="AN1" s="86">
         <v>42328</v>
       </c>
-      <c r="AO1" s="88"/>
-      <c r="AP1" s="88"/>
-      <c r="AQ1" s="88"/>
-      <c r="AR1" s="88"/>
+      <c r="AO1" s="87"/>
+      <c r="AP1" s="87"/>
+      <c r="AQ1" s="87"/>
+      <c r="AR1" s="87"/>
       <c r="AS1" s="12"/>
-      <c r="AT1" s="87">
+      <c r="AT1" s="86">
         <v>42329</v>
       </c>
-      <c r="AU1" s="88"/>
-      <c r="AV1" s="88"/>
-      <c r="AW1" s="88"/>
-      <c r="AX1" s="88"/>
+      <c r="AU1" s="87"/>
+      <c r="AV1" s="87"/>
+      <c r="AW1" s="87"/>
+      <c r="AX1" s="87"/>
       <c r="AY1" s="12"/>
-      <c r="AZ1" s="87">
+      <c r="AZ1" s="86">
         <v>42330</v>
       </c>
-      <c r="BA1" s="88"/>
-      <c r="BB1" s="88"/>
-      <c r="BC1" s="88"/>
-      <c r="BD1" s="88"/>
+      <c r="BA1" s="87"/>
+      <c r="BB1" s="87"/>
+      <c r="BC1" s="87"/>
+      <c r="BD1" s="87"/>
       <c r="BE1" s="12"/>
-      <c r="BF1" s="87">
+      <c r="BF1" s="86">
         <v>42331</v>
       </c>
-      <c r="BG1" s="88"/>
-      <c r="BH1" s="88"/>
-      <c r="BI1" s="88"/>
-      <c r="BJ1" s="88"/>
+      <c r="BG1" s="87"/>
+      <c r="BH1" s="87"/>
+      <c r="BI1" s="87"/>
+      <c r="BJ1" s="87"/>
       <c r="BK1" s="12"/>
-      <c r="BL1" s="87">
+      <c r="BL1" s="86">
         <v>42332</v>
       </c>
-      <c r="BM1" s="88"/>
-      <c r="BN1" s="88"/>
-      <c r="BO1" s="88"/>
-      <c r="BP1" s="88"/>
+      <c r="BM1" s="87"/>
+      <c r="BN1" s="87"/>
+      <c r="BO1" s="87"/>
+      <c r="BP1" s="87"/>
       <c r="BQ1" s="12"/>
-      <c r="BR1" s="87">
+      <c r="BR1" s="86">
         <v>42333</v>
       </c>
-      <c r="BS1" s="88"/>
-      <c r="BT1" s="88"/>
-      <c r="BU1" s="88"/>
-      <c r="BV1" s="88"/>
+      <c r="BS1" s="87"/>
+      <c r="BT1" s="87"/>
+      <c r="BU1" s="87"/>
+      <c r="BV1" s="87"/>
       <c r="BW1" s="12"/>
-      <c r="BX1" s="87">
+      <c r="BX1" s="86">
         <v>42334</v>
       </c>
-      <c r="BY1" s="88"/>
-      <c r="BZ1" s="88"/>
-      <c r="CA1" s="88"/>
-      <c r="CB1" s="88"/>
+      <c r="BY1" s="87"/>
+      <c r="BZ1" s="87"/>
+      <c r="CA1" s="87"/>
+      <c r="CB1" s="87"/>
       <c r="CC1" s="12"/>
-      <c r="CD1" s="87">
+      <c r="CD1" s="86">
         <v>42335</v>
       </c>
-      <c r="CE1" s="88"/>
-      <c r="CF1" s="88"/>
-      <c r="CG1" s="88"/>
-      <c r="CH1" s="88"/>
+      <c r="CE1" s="87"/>
+      <c r="CF1" s="87"/>
+      <c r="CG1" s="87"/>
+      <c r="CH1" s="87"/>
       <c r="CI1" s="12"/>
-      <c r="CJ1" s="87">
+      <c r="CJ1" s="86">
         <v>42336</v>
       </c>
-      <c r="CK1" s="88"/>
-      <c r="CL1" s="88"/>
-      <c r="CM1" s="88"/>
-      <c r="CN1" s="88"/>
+      <c r="CK1" s="87"/>
+      <c r="CL1" s="87"/>
+      <c r="CM1" s="87"/>
+      <c r="CN1" s="87"/>
       <c r="CO1" s="12"/>
-      <c r="CP1" s="87">
+      <c r="CP1" s="86">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="88"/>
-      <c r="CR1" s="88"/>
-      <c r="CS1" s="88"/>
-      <c r="CT1" s="88"/>
+      <c r="CQ1" s="87"/>
+      <c r="CR1" s="87"/>
+      <c r="CS1" s="87"/>
+      <c r="CT1" s="87"/>
       <c r="CU1" s="12"/>
-      <c r="CV1" s="87">
+      <c r="CV1" s="86">
         <v>42338</v>
       </c>
-      <c r="CW1" s="88"/>
-      <c r="CX1" s="88"/>
-      <c r="CY1" s="88"/>
-      <c r="CZ1" s="88"/>
+      <c r="CW1" s="87"/>
+      <c r="CX1" s="87"/>
+      <c r="CY1" s="87"/>
+      <c r="CZ1" s="87"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="87">
+      <c r="DB1" s="86">
         <v>42339</v>
       </c>
-      <c r="DC1" s="88"/>
-      <c r="DD1" s="88"/>
-      <c r="DE1" s="88"/>
-      <c r="DF1" s="88"/>
+      <c r="DC1" s="87"/>
+      <c r="DD1" s="87"/>
+      <c r="DE1" s="87"/>
+      <c r="DF1" s="87"/>
       <c r="DG1" s="12"/>
-      <c r="DH1" s="87">
+      <c r="DH1" s="86">
         <v>42340</v>
       </c>
-      <c r="DI1" s="88"/>
-      <c r="DJ1" s="88"/>
-      <c r="DK1" s="88"/>
-      <c r="DL1" s="88"/>
+      <c r="DI1" s="87"/>
+      <c r="DJ1" s="87"/>
+      <c r="DK1" s="87"/>
+      <c r="DL1" s="87"/>
       <c r="DM1" s="12"/>
-      <c r="DN1" s="87">
+      <c r="DN1" s="86">
         <v>42341</v>
       </c>
-      <c r="DO1" s="88"/>
-      <c r="DP1" s="88"/>
-      <c r="DQ1" s="88"/>
-      <c r="DR1" s="88"/>
+      <c r="DO1" s="87"/>
+      <c r="DP1" s="87"/>
+      <c r="DQ1" s="87"/>
+      <c r="DR1" s="87"/>
       <c r="DS1" s="12"/>
-      <c r="DT1" s="87">
+      <c r="DT1" s="86">
         <v>42342</v>
       </c>
-      <c r="DU1" s="88"/>
-      <c r="DV1" s="88"/>
-      <c r="DW1" s="88"/>
-      <c r="DX1" s="88"/>
+      <c r="DU1" s="87"/>
+      <c r="DV1" s="87"/>
+      <c r="DW1" s="87"/>
+      <c r="DX1" s="87"/>
       <c r="DY1" s="12"/>
-      <c r="DZ1" s="87">
+      <c r="DZ1" s="86">
         <v>42343</v>
       </c>
-      <c r="EA1" s="88"/>
-      <c r="EB1" s="88"/>
-      <c r="EC1" s="88"/>
-      <c r="ED1" s="88"/>
+      <c r="EA1" s="87"/>
+      <c r="EB1" s="87"/>
+      <c r="EC1" s="87"/>
+      <c r="ED1" s="87"/>
       <c r="EE1" s="12"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -2664,7 +2664,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="88" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="14">
@@ -2814,7 +2814,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="86"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3114,7 +3114,7 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="86"/>
+      <c r="C11" s="88"/>
       <c r="D11" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3424,7 +3424,7 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="86"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3578,7 +3578,7 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="86"/>
+      <c r="C14" s="88"/>
       <c r="D14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -5891,7 +5891,7 @@
       <c r="B30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="86" t="s">
+      <c r="C30" s="88" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="6"/>
@@ -6036,7 +6036,7 @@
       <c r="B31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="86"/>
+      <c r="C31" s="88"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -6179,7 +6179,7 @@
       <c r="B32" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="86"/>
+      <c r="C32" s="88"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
@@ -7049,7 +7049,7 @@
       <c r="B38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="86" t="s">
+      <c r="C38" s="88" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="6"/>
@@ -7192,7 +7192,7 @@
       <c r="B39" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="86"/>
+      <c r="C39" s="88"/>
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
@@ -9256,7 +9256,9 @@
       <c r="DH52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DI52" s="18"/>
+      <c r="DI52" s="83">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="DJ52" s="18"/>
       <c r="DK52" s="18"/>
       <c r="DL52" s="54"/>
@@ -11871,7 +11873,7 @@
       </c>
       <c r="DI68" s="29">
         <f>SUM(DI3:DI65)</f>
-        <v>0.125</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="DJ68" s="30" t="s">
         <v>37</v>
@@ -13024,6 +13026,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CP1:CT1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DB1:DF1"/>
+    <mergeCell ref="DH1:DL1"/>
     <mergeCell ref="AT1:AX1"/>
     <mergeCell ref="AZ1:BD1"/>
     <mergeCell ref="DN1:DR1"/>
@@ -13036,24 +13056,6 @@
     <mergeCell ref="BX1:CB1"/>
     <mergeCell ref="CD1:CH1"/>
     <mergeCell ref="AB1:AF1"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CP1:CT1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DB1:DF1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="AN1:AR1"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualização planilha de atividades 03/12
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -264,9 +264,6 @@
     <t>Criar arquivo de apresentacao PPT</t>
   </si>
   <si>
-    <t>Criar arquivo sprintbacklog.pdf</t>
-  </si>
-  <si>
     <t>Criar arquivo sprintbacklog INICIAL.pdf</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
   </si>
   <si>
     <t>Entregar dia 21/11 os arquivos do projeto seguro.eap</t>
-  </si>
-  <si>
-    <t>Copia do Seguro.eap da sprint 2</t>
   </si>
   <si>
     <t>1.0</t>
@@ -292,6 +286,12 @@
   </si>
   <si>
     <t>Alterações de projeto</t>
+  </si>
+  <si>
+    <t>Criar arquivo sprint_backlog_2.pdf</t>
+  </si>
+  <si>
+    <t>Criar do Seguro_v2.eap da sprint 2</t>
   </si>
 </sst>
 </file>
@@ -813,14 +813,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1203,10 +1203,10 @@
   <dimension ref="A1:EE80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="CZ46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="DH39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="DI61" sqref="DI61"/>
+      <selection pane="bottomRight" activeCell="DR34" sqref="DR34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1298,181 +1298,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="86">
+      <c r="D1" s="87">
         <v>42322</v>
       </c>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="88"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="86">
+      <c r="J1" s="87">
         <v>42323</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
+      <c r="K1" s="88"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="88"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="86">
+      <c r="P1" s="87">
         <v>42324</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
+      <c r="Q1" s="88"/>
+      <c r="R1" s="88"/>
+      <c r="S1" s="88"/>
+      <c r="T1" s="88"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="86">
+      <c r="V1" s="87">
         <v>42325</v>
       </c>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
+      <c r="W1" s="88"/>
+      <c r="X1" s="88"/>
+      <c r="Y1" s="88"/>
+      <c r="Z1" s="88"/>
       <c r="AA1" s="12"/>
-      <c r="AB1" s="86">
+      <c r="AB1" s="87">
         <v>42326</v>
       </c>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="87"/>
-      <c r="AF1" s="87"/>
+      <c r="AC1" s="88"/>
+      <c r="AD1" s="88"/>
+      <c r="AE1" s="88"/>
+      <c r="AF1" s="88"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="86">
+      <c r="AH1" s="87">
         <v>42327</v>
       </c>
-      <c r="AI1" s="87"/>
-      <c r="AJ1" s="87"/>
-      <c r="AK1" s="87"/>
-      <c r="AL1" s="87"/>
+      <c r="AI1" s="88"/>
+      <c r="AJ1" s="88"/>
+      <c r="AK1" s="88"/>
+      <c r="AL1" s="88"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="86">
+      <c r="AN1" s="87">
         <v>42328</v>
       </c>
-      <c r="AO1" s="87"/>
-      <c r="AP1" s="87"/>
-      <c r="AQ1" s="87"/>
-      <c r="AR1" s="87"/>
+      <c r="AO1" s="88"/>
+      <c r="AP1" s="88"/>
+      <c r="AQ1" s="88"/>
+      <c r="AR1" s="88"/>
       <c r="AS1" s="12"/>
-      <c r="AT1" s="86">
+      <c r="AT1" s="87">
         <v>42329</v>
       </c>
-      <c r="AU1" s="87"/>
-      <c r="AV1" s="87"/>
-      <c r="AW1" s="87"/>
-      <c r="AX1" s="87"/>
+      <c r="AU1" s="88"/>
+      <c r="AV1" s="88"/>
+      <c r="AW1" s="88"/>
+      <c r="AX1" s="88"/>
       <c r="AY1" s="12"/>
-      <c r="AZ1" s="86">
+      <c r="AZ1" s="87">
         <v>42330</v>
       </c>
-      <c r="BA1" s="87"/>
-      <c r="BB1" s="87"/>
-      <c r="BC1" s="87"/>
-      <c r="BD1" s="87"/>
+      <c r="BA1" s="88"/>
+      <c r="BB1" s="88"/>
+      <c r="BC1" s="88"/>
+      <c r="BD1" s="88"/>
       <c r="BE1" s="12"/>
-      <c r="BF1" s="86">
+      <c r="BF1" s="87">
         <v>42331</v>
       </c>
-      <c r="BG1" s="87"/>
-      <c r="BH1" s="87"/>
-      <c r="BI1" s="87"/>
-      <c r="BJ1" s="87"/>
+      <c r="BG1" s="88"/>
+      <c r="BH1" s="88"/>
+      <c r="BI1" s="88"/>
+      <c r="BJ1" s="88"/>
       <c r="BK1" s="12"/>
-      <c r="BL1" s="86">
+      <c r="BL1" s="87">
         <v>42332</v>
       </c>
-      <c r="BM1" s="87"/>
-      <c r="BN1" s="87"/>
-      <c r="BO1" s="87"/>
-      <c r="BP1" s="87"/>
+      <c r="BM1" s="88"/>
+      <c r="BN1" s="88"/>
+      <c r="BO1" s="88"/>
+      <c r="BP1" s="88"/>
       <c r="BQ1" s="12"/>
-      <c r="BR1" s="86">
+      <c r="BR1" s="87">
         <v>42333</v>
       </c>
-      <c r="BS1" s="87"/>
-      <c r="BT1" s="87"/>
-      <c r="BU1" s="87"/>
-      <c r="BV1" s="87"/>
+      <c r="BS1" s="88"/>
+      <c r="BT1" s="88"/>
+      <c r="BU1" s="88"/>
+      <c r="BV1" s="88"/>
       <c r="BW1" s="12"/>
-      <c r="BX1" s="86">
+      <c r="BX1" s="87">
         <v>42334</v>
       </c>
-      <c r="BY1" s="87"/>
-      <c r="BZ1" s="87"/>
-      <c r="CA1" s="87"/>
-      <c r="CB1" s="87"/>
+      <c r="BY1" s="88"/>
+      <c r="BZ1" s="88"/>
+      <c r="CA1" s="88"/>
+      <c r="CB1" s="88"/>
       <c r="CC1" s="12"/>
-      <c r="CD1" s="86">
+      <c r="CD1" s="87">
         <v>42335</v>
       </c>
-      <c r="CE1" s="87"/>
-      <c r="CF1" s="87"/>
-      <c r="CG1" s="87"/>
-      <c r="CH1" s="87"/>
+      <c r="CE1" s="88"/>
+      <c r="CF1" s="88"/>
+      <c r="CG1" s="88"/>
+      <c r="CH1" s="88"/>
       <c r="CI1" s="12"/>
-      <c r="CJ1" s="86">
+      <c r="CJ1" s="87">
         <v>42336</v>
       </c>
-      <c r="CK1" s="87"/>
-      <c r="CL1" s="87"/>
-      <c r="CM1" s="87"/>
-      <c r="CN1" s="87"/>
+      <c r="CK1" s="88"/>
+      <c r="CL1" s="88"/>
+      <c r="CM1" s="88"/>
+      <c r="CN1" s="88"/>
       <c r="CO1" s="12"/>
-      <c r="CP1" s="86">
+      <c r="CP1" s="87">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="87"/>
-      <c r="CR1" s="87"/>
-      <c r="CS1" s="87"/>
-      <c r="CT1" s="87"/>
+      <c r="CQ1" s="88"/>
+      <c r="CR1" s="88"/>
+      <c r="CS1" s="88"/>
+      <c r="CT1" s="88"/>
       <c r="CU1" s="12"/>
-      <c r="CV1" s="86">
+      <c r="CV1" s="87">
         <v>42338</v>
       </c>
-      <c r="CW1" s="87"/>
-      <c r="CX1" s="87"/>
-      <c r="CY1" s="87"/>
-      <c r="CZ1" s="87"/>
+      <c r="CW1" s="88"/>
+      <c r="CX1" s="88"/>
+      <c r="CY1" s="88"/>
+      <c r="CZ1" s="88"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="86">
+      <c r="DB1" s="87">
         <v>42339</v>
       </c>
-      <c r="DC1" s="87"/>
-      <c r="DD1" s="87"/>
-      <c r="DE1" s="87"/>
-      <c r="DF1" s="87"/>
+      <c r="DC1" s="88"/>
+      <c r="DD1" s="88"/>
+      <c r="DE1" s="88"/>
+      <c r="DF1" s="88"/>
       <c r="DG1" s="12"/>
-      <c r="DH1" s="86">
+      <c r="DH1" s="87">
         <v>42340</v>
       </c>
-      <c r="DI1" s="87"/>
-      <c r="DJ1" s="87"/>
-      <c r="DK1" s="87"/>
-      <c r="DL1" s="87"/>
+      <c r="DI1" s="88"/>
+      <c r="DJ1" s="88"/>
+      <c r="DK1" s="88"/>
+      <c r="DL1" s="88"/>
       <c r="DM1" s="12"/>
-      <c r="DN1" s="86">
+      <c r="DN1" s="87">
         <v>42341</v>
       </c>
-      <c r="DO1" s="87"/>
-      <c r="DP1" s="87"/>
-      <c r="DQ1" s="87"/>
-      <c r="DR1" s="87"/>
+      <c r="DO1" s="88"/>
+      <c r="DP1" s="88"/>
+      <c r="DQ1" s="88"/>
+      <c r="DR1" s="88"/>
       <c r="DS1" s="12"/>
-      <c r="DT1" s="86">
+      <c r="DT1" s="87">
         <v>42342</v>
       </c>
-      <c r="DU1" s="87"/>
-      <c r="DV1" s="87"/>
-      <c r="DW1" s="87"/>
-      <c r="DX1" s="87"/>
+      <c r="DU1" s="88"/>
+      <c r="DV1" s="88"/>
+      <c r="DW1" s="88"/>
+      <c r="DX1" s="88"/>
       <c r="DY1" s="12"/>
-      <c r="DZ1" s="86">
+      <c r="DZ1" s="87">
         <v>42343</v>
       </c>
-      <c r="EA1" s="87"/>
-      <c r="EB1" s="87"/>
-      <c r="EC1" s="87"/>
-      <c r="ED1" s="87"/>
+      <c r="EA1" s="88"/>
+      <c r="EB1" s="88"/>
+      <c r="EC1" s="88"/>
+      <c r="ED1" s="88"/>
       <c r="EE1" s="12"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -2035,7 +2035,9 @@
       <c r="DN3" s="71">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="DO3" s="77"/>
+      <c r="DO3" s="72">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="DP3" s="74"/>
       <c r="DQ3" s="74"/>
       <c r="DR3" s="75"/>
@@ -2664,7 +2666,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="86" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="14">
@@ -2814,7 +2816,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="88"/>
+      <c r="C9" s="86"/>
       <c r="D9" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3114,7 +3116,7 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="88"/>
+      <c r="C11" s="86"/>
       <c r="D11" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3424,7 +3426,7 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="88"/>
+      <c r="C13" s="86"/>
       <c r="D13" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3578,7 +3580,7 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="88"/>
+      <c r="C14" s="86"/>
       <c r="D14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -4158,7 +4160,7 @@
         <v>66</v>
       </c>
       <c r="C18" s="67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
@@ -4305,7 +4307,7 @@
         <v>66</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
@@ -4448,7 +4450,7 @@
         <v>66</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
@@ -5024,7 +5026,7 @@
         <v>68</v>
       </c>
       <c r="C24" s="67" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
@@ -5169,7 +5171,7 @@
         <v>68</v>
       </c>
       <c r="C25" s="67" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="7"/>
@@ -5891,7 +5893,7 @@
       <c r="B30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="88" t="s">
+      <c r="C30" s="86" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="6"/>
@@ -6036,7 +6038,7 @@
       <c r="B31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="88"/>
+      <c r="C31" s="86"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -6179,7 +6181,7 @@
       <c r="B32" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="88"/>
+      <c r="C32" s="86"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
@@ -6321,7 +6323,7 @@
         <v>69</v>
       </c>
       <c r="C33" s="68" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="7"/>
@@ -6437,11 +6439,15 @@
       <c r="DK33" s="9"/>
       <c r="DL33" s="10"/>
       <c r="DM33" s="12"/>
-      <c r="DN33" s="6"/>
-      <c r="DO33" s="7"/>
+      <c r="DN33" s="6">
+        <v>0</v>
+      </c>
+      <c r="DO33" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="DP33" s="8"/>
       <c r="DQ33" s="9"/>
-      <c r="DR33" s="10"/>
+      <c r="DR33" s="53"/>
       <c r="DS33" s="12"/>
       <c r="DT33" s="6">
         <v>4.1666666666666664E-2</v>
@@ -6464,7 +6470,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="67" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="7"/>
@@ -6582,11 +6588,15 @@
       <c r="DK34" s="9"/>
       <c r="DL34" s="10"/>
       <c r="DM34" s="12"/>
-      <c r="DN34" s="6"/>
-      <c r="DO34" s="7"/>
+      <c r="DN34" s="6">
+        <v>0</v>
+      </c>
+      <c r="DO34" s="7">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="DP34" s="8"/>
       <c r="DQ34" s="9"/>
-      <c r="DR34" s="10"/>
+      <c r="DR34" s="53"/>
       <c r="DS34" s="12"/>
       <c r="DT34" s="6">
         <v>8.3333333333333329E-2</v>
@@ -7049,7 +7059,7 @@
       <c r="B38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="88" t="s">
+      <c r="C38" s="86" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="6"/>
@@ -7192,7 +7202,7 @@
       <c r="B39" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="88"/>
+      <c r="C39" s="86"/>
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
@@ -7479,7 +7489,7 @@
         <v>77</v>
       </c>
       <c r="C41" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
@@ -7902,7 +7912,7 @@
         <v>79</v>
       </c>
       <c r="C44" s="46" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="7"/>
@@ -8047,7 +8057,7 @@
         <v>79</v>
       </c>
       <c r="C45" s="46" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="7"/>
@@ -8190,7 +8200,7 @@
         <v>79</v>
       </c>
       <c r="C46" s="46" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="7"/>
@@ -8306,11 +8316,15 @@
       <c r="DK46" s="9"/>
       <c r="DL46" s="10"/>
       <c r="DM46" s="12"/>
-      <c r="DN46" s="6"/>
-      <c r="DO46" s="7"/>
+      <c r="DN46" s="6">
+        <v>0</v>
+      </c>
+      <c r="DO46" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="DP46" s="8"/>
       <c r="DQ46" s="9"/>
-      <c r="DR46" s="10"/>
+      <c r="DR46" s="53"/>
       <c r="DS46" s="12"/>
       <c r="DT46" s="6">
         <v>4.1666666666666664E-2</v>
@@ -8630,7 +8644,7 @@
         <v>16</v>
       </c>
       <c r="C49" s="46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="7"/>
@@ -9445,7 +9459,9 @@
       <c r="DN53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DO53" s="18"/>
+      <c r="DO53" s="83">
+        <v>0</v>
+      </c>
       <c r="DP53" s="18"/>
       <c r="DQ53" s="18"/>
       <c r="DR53" s="53"/>
@@ -9896,7 +9912,7 @@
         <v>21</v>
       </c>
       <c r="C57" s="85" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D57" s="84"/>
       <c r="E57" s="18"/>
@@ -11889,7 +11905,7 @@
       </c>
       <c r="DO68" s="29">
         <f>SUM(DO3:DO65)</f>
-        <v>0</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="DP68" s="30" t="s">
         <v>37</v>
@@ -12088,9 +12104,9 @@
       <c r="DN69" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="DO69" s="33" t="e">
+      <c r="DO69" s="33">
         <f>DQ68/DO68</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="DR69" s="34"/>
       <c r="DT69" s="32" t="s">
@@ -12444,9 +12460,9 @@
       <c r="DN71" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="DO71" s="35" t="e">
+      <c r="DO71" s="35">
         <f>1-DO69</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="DR71" s="34"/>
       <c r="DT71" s="32" t="s">
@@ -13026,6 +13042,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="DN1:DR1"/>
+    <mergeCell ref="DT1:DX1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BL1:BP1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BX1:CB1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CP1:CT1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DB1:DF1"/>
+    <mergeCell ref="DH1:DL1"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="AH1:AL1"/>
     <mergeCell ref="AN1:AR1"/>
@@ -13038,24 +13072,6 @@
     <mergeCell ref="P1:T1"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CP1:CT1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DB1:DF1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="DN1:DR1"/>
-    <mergeCell ref="DT1:DX1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BL1:BP1"/>
-    <mergeCell ref="BR1:BV1"/>
-    <mergeCell ref="BX1:CB1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="AB1:AF1"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -13171,7 +13187,7 @@
         <v>42322</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4" s="39" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Apontamento de horas da semana
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="701"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="701"/>
   </bookViews>
   <sheets>
     <sheet name="Atividades" sheetId="1" r:id="rId1"/>
@@ -813,14 +813,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1203,89 +1203,89 @@
   <dimension ref="A1:EE80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="DH39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="DK48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="DR34" sqref="DR34"/>
+      <selection pane="bottomRight" activeCell="DV51" sqref="DV51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.42578125"/>
-    <col min="2" max="2" width="29.42578125"/>
-    <col min="3" max="3" width="33.5703125"/>
-    <col min="4" max="5" width="11.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625"/>
+    <col min="2" max="2" width="29.44140625"/>
+    <col min="3" max="3" width="33.5546875"/>
+    <col min="4" max="5" width="11.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="3.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="1"/>
-    <col min="14" max="14" width="8.7109375" customWidth="1"/>
-    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="12" max="13" width="9.109375" style="1"/>
+    <col min="14" max="14" width="8.6640625" customWidth="1"/>
+    <col min="15" max="15" width="3.44140625" customWidth="1"/>
     <col min="16" max="16" width="12" style="1" customWidth="1"/>
-    <col min="17" max="19" width="9.140625" style="1"/>
-    <col min="20" max="20" width="8.7109375" customWidth="1"/>
-    <col min="21" max="21" width="3.42578125" customWidth="1"/>
-    <col min="22" max="25" width="9.140625" style="1"/>
-    <col min="26" max="26" width="8.7109375" customWidth="1"/>
-    <col min="27" max="27" width="3.85546875" customWidth="1"/>
-    <col min="28" max="31" width="9.140625" style="1"/>
-    <col min="32" max="32" width="8.7109375" customWidth="1"/>
-    <col min="33" max="33" width="3.85546875" customWidth="1"/>
-    <col min="34" max="37" width="9.140625" style="1"/>
-    <col min="38" max="38" width="8.7109375" customWidth="1"/>
-    <col min="39" max="39" width="3.85546875" customWidth="1"/>
-    <col min="40" max="43" width="9.140625" style="1"/>
-    <col min="44" max="44" width="8.7109375" customWidth="1"/>
-    <col min="45" max="45" width="3.85546875" customWidth="1"/>
-    <col min="46" max="49" width="9.140625" style="1"/>
-    <col min="50" max="50" width="8.7109375" customWidth="1"/>
-    <col min="51" max="51" width="3.85546875" customWidth="1"/>
-    <col min="52" max="55" width="9.140625" style="1"/>
-    <col min="56" max="56" width="8.7109375" customWidth="1"/>
-    <col min="57" max="57" width="3.85546875" customWidth="1"/>
-    <col min="58" max="61" width="9.140625" style="1"/>
-    <col min="62" max="62" width="8.7109375" customWidth="1"/>
-    <col min="63" max="63" width="3.85546875" customWidth="1"/>
-    <col min="64" max="67" width="9.140625" style="1"/>
-    <col min="68" max="68" width="8.7109375" customWidth="1"/>
-    <col min="69" max="69" width="3.85546875" customWidth="1"/>
-    <col min="70" max="73" width="9.140625" style="1"/>
-    <col min="74" max="74" width="8.7109375" customWidth="1"/>
-    <col min="75" max="75" width="3.85546875" customWidth="1"/>
-    <col min="76" max="79" width="9.140625" style="1"/>
-    <col min="80" max="80" width="8.7109375" customWidth="1"/>
-    <col min="81" max="81" width="3.85546875" customWidth="1"/>
-    <col min="82" max="85" width="9.140625" style="1"/>
-    <col min="86" max="86" width="8.7109375" customWidth="1"/>
-    <col min="87" max="87" width="3.85546875" customWidth="1"/>
-    <col min="88" max="91" width="9.140625" style="1"/>
-    <col min="92" max="92" width="8.7109375" customWidth="1"/>
-    <col min="93" max="93" width="3.85546875" customWidth="1"/>
-    <col min="94" max="97" width="9.140625" style="1"/>
-    <col min="98" max="98" width="8.7109375" customWidth="1"/>
-    <col min="99" max="99" width="3.85546875" customWidth="1"/>
-    <col min="100" max="103" width="9.140625" style="1"/>
-    <col min="104" max="104" width="8.7109375" customWidth="1"/>
-    <col min="105" max="105" width="3.85546875" customWidth="1"/>
-    <col min="106" max="109" width="9.140625" style="1"/>
-    <col min="110" max="110" width="8.7109375" customWidth="1"/>
-    <col min="111" max="111" width="3.85546875" customWidth="1"/>
-    <col min="112" max="115" width="9.140625" style="1"/>
-    <col min="116" max="116" width="8.7109375" customWidth="1"/>
-    <col min="117" max="117" width="3.85546875" customWidth="1"/>
-    <col min="118" max="121" width="9.140625" style="1"/>
-    <col min="122" max="122" width="8.7109375" customWidth="1"/>
-    <col min="123" max="123" width="3.85546875" customWidth="1"/>
-    <col min="124" max="127" width="9.140625" style="1"/>
-    <col min="128" max="128" width="8.7109375" customWidth="1"/>
-    <col min="129" max="129" width="3.85546875" customWidth="1"/>
-    <col min="130" max="132" width="9.140625" style="1"/>
-    <col min="133" max="133" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="8.7109375" customWidth="1"/>
-    <col min="135" max="135" width="3.85546875" customWidth="1"/>
+    <col min="17" max="19" width="9.109375" style="1"/>
+    <col min="20" max="20" width="8.6640625" customWidth="1"/>
+    <col min="21" max="21" width="3.44140625" customWidth="1"/>
+    <col min="22" max="25" width="9.109375" style="1"/>
+    <col min="26" max="26" width="8.6640625" customWidth="1"/>
+    <col min="27" max="27" width="3.88671875" customWidth="1"/>
+    <col min="28" max="31" width="9.109375" style="1"/>
+    <col min="32" max="32" width="8.6640625" customWidth="1"/>
+    <col min="33" max="33" width="3.88671875" customWidth="1"/>
+    <col min="34" max="37" width="9.109375" style="1"/>
+    <col min="38" max="38" width="8.6640625" customWidth="1"/>
+    <col min="39" max="39" width="3.88671875" customWidth="1"/>
+    <col min="40" max="43" width="9.109375" style="1"/>
+    <col min="44" max="44" width="8.6640625" customWidth="1"/>
+    <col min="45" max="45" width="3.88671875" customWidth="1"/>
+    <col min="46" max="49" width="9.109375" style="1"/>
+    <col min="50" max="50" width="8.6640625" customWidth="1"/>
+    <col min="51" max="51" width="3.88671875" customWidth="1"/>
+    <col min="52" max="55" width="9.109375" style="1"/>
+    <col min="56" max="56" width="8.6640625" customWidth="1"/>
+    <col min="57" max="57" width="3.88671875" customWidth="1"/>
+    <col min="58" max="61" width="9.109375" style="1"/>
+    <col min="62" max="62" width="8.6640625" customWidth="1"/>
+    <col min="63" max="63" width="3.88671875" customWidth="1"/>
+    <col min="64" max="67" width="9.109375" style="1"/>
+    <col min="68" max="68" width="8.6640625" customWidth="1"/>
+    <col min="69" max="69" width="3.88671875" customWidth="1"/>
+    <col min="70" max="73" width="9.109375" style="1"/>
+    <col min="74" max="74" width="8.6640625" customWidth="1"/>
+    <col min="75" max="75" width="3.88671875" customWidth="1"/>
+    <col min="76" max="79" width="9.109375" style="1"/>
+    <col min="80" max="80" width="8.6640625" customWidth="1"/>
+    <col min="81" max="81" width="3.88671875" customWidth="1"/>
+    <col min="82" max="85" width="9.109375" style="1"/>
+    <col min="86" max="86" width="8.6640625" customWidth="1"/>
+    <col min="87" max="87" width="3.88671875" customWidth="1"/>
+    <col min="88" max="91" width="9.109375" style="1"/>
+    <col min="92" max="92" width="8.6640625" customWidth="1"/>
+    <col min="93" max="93" width="3.88671875" customWidth="1"/>
+    <col min="94" max="97" width="9.109375" style="1"/>
+    <col min="98" max="98" width="8.6640625" customWidth="1"/>
+    <col min="99" max="99" width="3.88671875" customWidth="1"/>
+    <col min="100" max="103" width="9.109375" style="1"/>
+    <col min="104" max="104" width="8.6640625" customWidth="1"/>
+    <col min="105" max="105" width="3.88671875" customWidth="1"/>
+    <col min="106" max="109" width="9.109375" style="1"/>
+    <col min="110" max="110" width="8.6640625" customWidth="1"/>
+    <col min="111" max="111" width="3.88671875" customWidth="1"/>
+    <col min="112" max="115" width="9.109375" style="1"/>
+    <col min="116" max="116" width="8.6640625" customWidth="1"/>
+    <col min="117" max="117" width="3.88671875" customWidth="1"/>
+    <col min="118" max="121" width="9.109375" style="1"/>
+    <col min="122" max="122" width="8.6640625" customWidth="1"/>
+    <col min="123" max="123" width="3.88671875" customWidth="1"/>
+    <col min="124" max="127" width="9.109375" style="1"/>
+    <col min="128" max="128" width="8.6640625" customWidth="1"/>
+    <col min="129" max="129" width="3.88671875" customWidth="1"/>
+    <col min="130" max="132" width="9.109375" style="1"/>
+    <col min="133" max="133" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="8.6640625" customWidth="1"/>
+    <col min="135" max="135" width="3.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:135">
@@ -1298,181 +1298,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="87">
+      <c r="D1" s="86">
         <v>42322</v>
       </c>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="87">
+      <c r="J1" s="86">
         <v>42323</v>
       </c>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="87">
+      <c r="P1" s="86">
         <v>42324</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-      <c r="T1" s="88"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="S1" s="87"/>
+      <c r="T1" s="87"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="87">
+      <c r="V1" s="86">
         <v>42325</v>
       </c>
-      <c r="W1" s="88"/>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="88"/>
+      <c r="W1" s="87"/>
+      <c r="X1" s="87"/>
+      <c r="Y1" s="87"/>
+      <c r="Z1" s="87"/>
       <c r="AA1" s="12"/>
-      <c r="AB1" s="87">
+      <c r="AB1" s="86">
         <v>42326</v>
       </c>
-      <c r="AC1" s="88"/>
-      <c r="AD1" s="88"/>
-      <c r="AE1" s="88"/>
-      <c r="AF1" s="88"/>
+      <c r="AC1" s="87"/>
+      <c r="AD1" s="87"/>
+      <c r="AE1" s="87"/>
+      <c r="AF1" s="87"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="87">
+      <c r="AH1" s="86">
         <v>42327</v>
       </c>
-      <c r="AI1" s="88"/>
-      <c r="AJ1" s="88"/>
-      <c r="AK1" s="88"/>
-      <c r="AL1" s="88"/>
+      <c r="AI1" s="87"/>
+      <c r="AJ1" s="87"/>
+      <c r="AK1" s="87"/>
+      <c r="AL1" s="87"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="87">
+      <c r="AN1" s="86">
         <v>42328</v>
       </c>
-      <c r="AO1" s="88"/>
-      <c r="AP1" s="88"/>
-      <c r="AQ1" s="88"/>
-      <c r="AR1" s="88"/>
+      <c r="AO1" s="87"/>
+      <c r="AP1" s="87"/>
+      <c r="AQ1" s="87"/>
+      <c r="AR1" s="87"/>
       <c r="AS1" s="12"/>
-      <c r="AT1" s="87">
+      <c r="AT1" s="86">
         <v>42329</v>
       </c>
-      <c r="AU1" s="88"/>
-      <c r="AV1" s="88"/>
-      <c r="AW1" s="88"/>
-      <c r="AX1" s="88"/>
+      <c r="AU1" s="87"/>
+      <c r="AV1" s="87"/>
+      <c r="AW1" s="87"/>
+      <c r="AX1" s="87"/>
       <c r="AY1" s="12"/>
-      <c r="AZ1" s="87">
+      <c r="AZ1" s="86">
         <v>42330</v>
       </c>
-      <c r="BA1" s="88"/>
-      <c r="BB1" s="88"/>
-      <c r="BC1" s="88"/>
-      <c r="BD1" s="88"/>
+      <c r="BA1" s="87"/>
+      <c r="BB1" s="87"/>
+      <c r="BC1" s="87"/>
+      <c r="BD1" s="87"/>
       <c r="BE1" s="12"/>
-      <c r="BF1" s="87">
+      <c r="BF1" s="86">
         <v>42331</v>
       </c>
-      <c r="BG1" s="88"/>
-      <c r="BH1" s="88"/>
-      <c r="BI1" s="88"/>
-      <c r="BJ1" s="88"/>
+      <c r="BG1" s="87"/>
+      <c r="BH1" s="87"/>
+      <c r="BI1" s="87"/>
+      <c r="BJ1" s="87"/>
       <c r="BK1" s="12"/>
-      <c r="BL1" s="87">
+      <c r="BL1" s="86">
         <v>42332</v>
       </c>
-      <c r="BM1" s="88"/>
-      <c r="BN1" s="88"/>
-      <c r="BO1" s="88"/>
-      <c r="BP1" s="88"/>
+      <c r="BM1" s="87"/>
+      <c r="BN1" s="87"/>
+      <c r="BO1" s="87"/>
+      <c r="BP1" s="87"/>
       <c r="BQ1" s="12"/>
-      <c r="BR1" s="87">
+      <c r="BR1" s="86">
         <v>42333</v>
       </c>
-      <c r="BS1" s="88"/>
-      <c r="BT1" s="88"/>
-      <c r="BU1" s="88"/>
-      <c r="BV1" s="88"/>
+      <c r="BS1" s="87"/>
+      <c r="BT1" s="87"/>
+      <c r="BU1" s="87"/>
+      <c r="BV1" s="87"/>
       <c r="BW1" s="12"/>
-      <c r="BX1" s="87">
+      <c r="BX1" s="86">
         <v>42334</v>
       </c>
-      <c r="BY1" s="88"/>
-      <c r="BZ1" s="88"/>
-      <c r="CA1" s="88"/>
-      <c r="CB1" s="88"/>
+      <c r="BY1" s="87"/>
+      <c r="BZ1" s="87"/>
+      <c r="CA1" s="87"/>
+      <c r="CB1" s="87"/>
       <c r="CC1" s="12"/>
-      <c r="CD1" s="87">
+      <c r="CD1" s="86">
         <v>42335</v>
       </c>
-      <c r="CE1" s="88"/>
-      <c r="CF1" s="88"/>
-      <c r="CG1" s="88"/>
-      <c r="CH1" s="88"/>
+      <c r="CE1" s="87"/>
+      <c r="CF1" s="87"/>
+      <c r="CG1" s="87"/>
+      <c r="CH1" s="87"/>
       <c r="CI1" s="12"/>
-      <c r="CJ1" s="87">
+      <c r="CJ1" s="86">
         <v>42336</v>
       </c>
-      <c r="CK1" s="88"/>
-      <c r="CL1" s="88"/>
-      <c r="CM1" s="88"/>
-      <c r="CN1" s="88"/>
+      <c r="CK1" s="87"/>
+      <c r="CL1" s="87"/>
+      <c r="CM1" s="87"/>
+      <c r="CN1" s="87"/>
       <c r="CO1" s="12"/>
-      <c r="CP1" s="87">
+      <c r="CP1" s="86">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="88"/>
-      <c r="CR1" s="88"/>
-      <c r="CS1" s="88"/>
-      <c r="CT1" s="88"/>
+      <c r="CQ1" s="87"/>
+      <c r="CR1" s="87"/>
+      <c r="CS1" s="87"/>
+      <c r="CT1" s="87"/>
       <c r="CU1" s="12"/>
-      <c r="CV1" s="87">
+      <c r="CV1" s="86">
         <v>42338</v>
       </c>
-      <c r="CW1" s="88"/>
-      <c r="CX1" s="88"/>
-      <c r="CY1" s="88"/>
-      <c r="CZ1" s="88"/>
+      <c r="CW1" s="87"/>
+      <c r="CX1" s="87"/>
+      <c r="CY1" s="87"/>
+      <c r="CZ1" s="87"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="87">
+      <c r="DB1" s="86">
         <v>42339</v>
       </c>
-      <c r="DC1" s="88"/>
-      <c r="DD1" s="88"/>
-      <c r="DE1" s="88"/>
-      <c r="DF1" s="88"/>
+      <c r="DC1" s="87"/>
+      <c r="DD1" s="87"/>
+      <c r="DE1" s="87"/>
+      <c r="DF1" s="87"/>
       <c r="DG1" s="12"/>
-      <c r="DH1" s="87">
+      <c r="DH1" s="86">
         <v>42340</v>
       </c>
-      <c r="DI1" s="88"/>
-      <c r="DJ1" s="88"/>
-      <c r="DK1" s="88"/>
-      <c r="DL1" s="88"/>
+      <c r="DI1" s="87"/>
+      <c r="DJ1" s="87"/>
+      <c r="DK1" s="87"/>
+      <c r="DL1" s="87"/>
       <c r="DM1" s="12"/>
-      <c r="DN1" s="87">
+      <c r="DN1" s="86">
         <v>42341</v>
       </c>
-      <c r="DO1" s="88"/>
-      <c r="DP1" s="88"/>
-      <c r="DQ1" s="88"/>
-      <c r="DR1" s="88"/>
+      <c r="DO1" s="87"/>
+      <c r="DP1" s="87"/>
+      <c r="DQ1" s="87"/>
+      <c r="DR1" s="87"/>
       <c r="DS1" s="12"/>
-      <c r="DT1" s="87">
+      <c r="DT1" s="86">
         <v>42342</v>
       </c>
-      <c r="DU1" s="88"/>
-      <c r="DV1" s="88"/>
-      <c r="DW1" s="88"/>
-      <c r="DX1" s="88"/>
+      <c r="DU1" s="87"/>
+      <c r="DV1" s="87"/>
+      <c r="DW1" s="87"/>
+      <c r="DX1" s="87"/>
       <c r="DY1" s="12"/>
-      <c r="DZ1" s="87">
+      <c r="DZ1" s="86">
         <v>42343</v>
       </c>
-      <c r="EA1" s="88"/>
-      <c r="EB1" s="88"/>
-      <c r="EC1" s="88"/>
-      <c r="ED1" s="88"/>
+      <c r="EA1" s="87"/>
+      <c r="EB1" s="87"/>
+      <c r="EC1" s="87"/>
+      <c r="ED1" s="87"/>
       <c r="EE1" s="12"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -2666,7 +2666,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="88" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="14">
@@ -2816,7 +2816,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="86"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3116,7 +3116,7 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="86"/>
+      <c r="C11" s="88"/>
       <c r="D11" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3426,7 +3426,7 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="86"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3580,7 +3580,7 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="86"/>
+      <c r="C14" s="88"/>
       <c r="D14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -4154,7 +4154,7 @@
       <c r="ED17" s="10"/>
       <c r="EE17" s="12"/>
     </row>
-    <row r="18" spans="1:135" ht="30">
+    <row r="18" spans="1:135">
       <c r="A18" s="2"/>
       <c r="B18" s="4" t="s">
         <v>66</v>
@@ -4301,7 +4301,7 @@
       <c r="ED18" s="10"/>
       <c r="EE18" s="12"/>
     </row>
-    <row r="19" spans="1:135" ht="30">
+    <row r="19" spans="1:135">
       <c r="A19" s="2"/>
       <c r="B19" s="4" t="s">
         <v>66</v>
@@ -4444,7 +4444,7 @@
       <c r="ED19" s="10"/>
       <c r="EE19" s="12"/>
     </row>
-    <row r="20" spans="1:135" ht="30">
+    <row r="20" spans="1:135">
       <c r="A20" s="2"/>
       <c r="B20" s="4" t="s">
         <v>66</v>
@@ -5893,7 +5893,7 @@
       <c r="B30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="86" t="s">
+      <c r="C30" s="88" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="6"/>
@@ -6038,7 +6038,7 @@
       <c r="B31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="86"/>
+      <c r="C31" s="88"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -6181,7 +6181,7 @@
       <c r="B32" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="86"/>
+      <c r="C32" s="88"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
@@ -7059,7 +7059,7 @@
       <c r="B38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="86" t="s">
+      <c r="C38" s="88" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="6"/>
@@ -7202,7 +7202,7 @@
       <c r="B39" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="86"/>
+      <c r="C39" s="88"/>
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
@@ -7483,7 +7483,7 @@
       <c r="ED40" s="10"/>
       <c r="EE40" s="12"/>
     </row>
-    <row r="41" spans="1:135" ht="30">
+    <row r="41" spans="1:135" ht="28.8">
       <c r="A41" s="2"/>
       <c r="B41" s="17" t="s">
         <v>77</v>
@@ -7626,7 +7626,7 @@
       <c r="ED41" s="10"/>
       <c r="EE41" s="12"/>
     </row>
-    <row r="42" spans="1:135" ht="30">
+    <row r="42" spans="1:135" ht="28.8">
       <c r="A42" s="2"/>
       <c r="B42" s="17" t="s">
         <v>77</v>
@@ -9079,31 +9079,41 @@
       <c r="CT51" s="52"/>
       <c r="CU51" s="12"/>
       <c r="CV51" s="14"/>
-      <c r="CW51" s="18"/>
+      <c r="CW51" s="83">
+        <v>0.125</v>
+      </c>
       <c r="CX51" s="18"/>
       <c r="CY51" s="18"/>
       <c r="CZ51" s="52"/>
       <c r="DA51" s="12"/>
       <c r="DB51" s="14"/>
-      <c r="DC51" s="18"/>
+      <c r="DC51" s="83">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="DD51" s="18"/>
       <c r="DE51" s="18"/>
       <c r="DF51" s="52"/>
       <c r="DG51" s="12"/>
       <c r="DH51" s="14"/>
-      <c r="DI51" s="18"/>
+      <c r="DI51" s="83">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="DJ51" s="18"/>
       <c r="DK51" s="18"/>
       <c r="DL51" s="52"/>
       <c r="DM51" s="12"/>
       <c r="DN51" s="14"/>
-      <c r="DO51" s="18"/>
+      <c r="DO51" s="83">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="DP51" s="18"/>
       <c r="DQ51" s="18"/>
       <c r="DR51" s="52"/>
       <c r="DS51" s="12"/>
       <c r="DT51" s="14"/>
-      <c r="DU51" s="18"/>
+      <c r="DU51" s="83">
+        <v>0.10416666666666667</v>
+      </c>
       <c r="DV51" s="18"/>
       <c r="DW51" s="18"/>
       <c r="DX51" s="10"/>
@@ -11591,7 +11601,7 @@
       </c>
       <c r="ED67" s="16"/>
     </row>
-    <row r="68" spans="1:135" ht="15.75" thickBot="1">
+    <row r="68" spans="1:135" ht="15" thickBot="1">
       <c r="C68" s="27" t="s">
         <v>36</v>
       </c>
@@ -11857,7 +11867,7 @@
       </c>
       <c r="CW68" s="29">
         <f>SUM(CW3:CW65)</f>
-        <v>0.14583333333333334</v>
+        <v>0.27083333333333337</v>
       </c>
       <c r="CX68" s="30" t="s">
         <v>37</v>
@@ -11873,7 +11883,7 @@
       </c>
       <c r="DC68" s="29">
         <f>SUM(DC3:DC65)</f>
-        <v>0.29166666666666663</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="DD68" s="30" t="s">
         <v>37</v>
@@ -11889,7 +11899,7 @@
       </c>
       <c r="DI68" s="29">
         <f>SUM(DI3:DI65)</f>
-        <v>0.29166666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="DJ68" s="30" t="s">
         <v>37</v>
@@ -11905,7 +11915,7 @@
       </c>
       <c r="DO68" s="29">
         <f>SUM(DO3:DO65)</f>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="DP68" s="30" t="s">
         <v>37</v>
@@ -11921,7 +11931,7 @@
       </c>
       <c r="DU68" s="29">
         <f>SUM(DU3:DU65)</f>
-        <v>0</v>
+        <v>0.10416666666666667</v>
       </c>
       <c r="DV68" s="30" t="s">
         <v>37</v>
@@ -12112,9 +12122,9 @@
       <c r="DT69" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="DU69" s="33" t="e">
+      <c r="DU69" s="33">
         <f>DW68/DU68</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="DX69" s="34"/>
       <c r="DZ69" s="32" t="s">
@@ -12468,9 +12478,9 @@
       <c r="DT71" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="DU71" s="35" t="e">
+      <c r="DU71" s="35">
         <f>1-DU69</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="DX71" s="34"/>
       <c r="DZ71" s="32" t="s">
@@ -13042,6 +13052,24 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CP1:CT1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DB1:DF1"/>
+    <mergeCell ref="DH1:DL1"/>
     <mergeCell ref="AT1:AX1"/>
     <mergeCell ref="AZ1:BD1"/>
     <mergeCell ref="DN1:DR1"/>
@@ -13054,24 +13082,6 @@
     <mergeCell ref="BX1:CB1"/>
     <mergeCell ref="CD1:CH1"/>
     <mergeCell ref="AB1:AF1"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CP1:CT1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DB1:DF1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="AN1:AR1"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -13087,19 +13097,19 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.42578125"/>
-    <col min="2" max="2" width="10.28515625"/>
+    <col min="1" max="1" width="33.44140625"/>
+    <col min="2" max="2" width="10.33203125"/>
     <col min="3" max="3" width="32"/>
     <col min="4" max="4" width="16"/>
-    <col min="5" max="5" width="12.85546875"/>
-    <col min="6" max="6" width="14.28515625"/>
-    <col min="7" max="7" width="18.7109375"/>
+    <col min="5" max="5" width="12.88671875"/>
+    <col min="6" max="6" width="14.33203125"/>
+    <col min="7" max="7" width="18.6640625"/>
     <col min="8" max="8" width="21"/>
-    <col min="9" max="9" width="14.42578125"/>
-    <col min="10" max="10" width="19.42578125"/>
-    <col min="11" max="11" width="23.42578125"/>
+    <col min="9" max="9" width="14.44140625"/>
+    <col min="10" max="10" width="19.44140625"/>
+    <col min="11" max="11" width="23.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -13142,13 +13152,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.5703125"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125"/>
-    <col min="4" max="4" width="56.85546875"/>
-    <col min="5" max="1025" width="10.5703125"/>
+    <col min="1" max="1" width="10.5546875"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875"/>
+    <col min="4" max="4" width="56.88671875"/>
+    <col min="5" max="1025" width="10.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>

<commit_message>
Conteúdo da atualização: * preenchimento do documento "alterações do projeto" com as alterações da sprint 2; * atualização da planilha de atividades
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="701"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="701"/>
   </bookViews>
   <sheets>
     <sheet name="Atividades" sheetId="1" r:id="rId1"/>
@@ -614,7 +614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -791,9 +791,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1203,89 +1200,89 @@
   <dimension ref="A1:EE80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="DK48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="DT3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="DV51" sqref="DV51"/>
+      <selection pane="bottomRight" activeCell="EA4" sqref="EA4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.44140625"/>
-    <col min="2" max="2" width="29.44140625"/>
-    <col min="3" max="3" width="33.5546875"/>
-    <col min="4" max="5" width="11.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125"/>
+    <col min="2" max="2" width="29.42578125"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="4" max="5" width="11.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="9" width="3.44140625" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" customWidth="1"/>
-    <col min="12" max="13" width="9.109375" style="1"/>
-    <col min="14" max="14" width="8.6640625" customWidth="1"/>
-    <col min="15" max="15" width="3.44140625" customWidth="1"/>
+    <col min="12" max="13" width="9.140625" style="1"/>
+    <col min="14" max="14" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
     <col min="16" max="16" width="12" style="1" customWidth="1"/>
-    <col min="17" max="19" width="9.109375" style="1"/>
-    <col min="20" max="20" width="8.6640625" customWidth="1"/>
-    <col min="21" max="21" width="3.44140625" customWidth="1"/>
-    <col min="22" max="25" width="9.109375" style="1"/>
-    <col min="26" max="26" width="8.6640625" customWidth="1"/>
-    <col min="27" max="27" width="3.88671875" customWidth="1"/>
-    <col min="28" max="31" width="9.109375" style="1"/>
-    <col min="32" max="32" width="8.6640625" customWidth="1"/>
-    <col min="33" max="33" width="3.88671875" customWidth="1"/>
-    <col min="34" max="37" width="9.109375" style="1"/>
-    <col min="38" max="38" width="8.6640625" customWidth="1"/>
-    <col min="39" max="39" width="3.88671875" customWidth="1"/>
-    <col min="40" max="43" width="9.109375" style="1"/>
-    <col min="44" max="44" width="8.6640625" customWidth="1"/>
-    <col min="45" max="45" width="3.88671875" customWidth="1"/>
-    <col min="46" max="49" width="9.109375" style="1"/>
-    <col min="50" max="50" width="8.6640625" customWidth="1"/>
-    <col min="51" max="51" width="3.88671875" customWidth="1"/>
-    <col min="52" max="55" width="9.109375" style="1"/>
-    <col min="56" max="56" width="8.6640625" customWidth="1"/>
-    <col min="57" max="57" width="3.88671875" customWidth="1"/>
-    <col min="58" max="61" width="9.109375" style="1"/>
-    <col min="62" max="62" width="8.6640625" customWidth="1"/>
-    <col min="63" max="63" width="3.88671875" customWidth="1"/>
-    <col min="64" max="67" width="9.109375" style="1"/>
-    <col min="68" max="68" width="8.6640625" customWidth="1"/>
-    <col min="69" max="69" width="3.88671875" customWidth="1"/>
-    <col min="70" max="73" width="9.109375" style="1"/>
-    <col min="74" max="74" width="8.6640625" customWidth="1"/>
-    <col min="75" max="75" width="3.88671875" customWidth="1"/>
-    <col min="76" max="79" width="9.109375" style="1"/>
-    <col min="80" max="80" width="8.6640625" customWidth="1"/>
-    <col min="81" max="81" width="3.88671875" customWidth="1"/>
-    <col min="82" max="85" width="9.109375" style="1"/>
-    <col min="86" max="86" width="8.6640625" customWidth="1"/>
-    <col min="87" max="87" width="3.88671875" customWidth="1"/>
-    <col min="88" max="91" width="9.109375" style="1"/>
-    <col min="92" max="92" width="8.6640625" customWidth="1"/>
-    <col min="93" max="93" width="3.88671875" customWidth="1"/>
-    <col min="94" max="97" width="9.109375" style="1"/>
-    <col min="98" max="98" width="8.6640625" customWidth="1"/>
-    <col min="99" max="99" width="3.88671875" customWidth="1"/>
-    <col min="100" max="103" width="9.109375" style="1"/>
-    <col min="104" max="104" width="8.6640625" customWidth="1"/>
-    <col min="105" max="105" width="3.88671875" customWidth="1"/>
-    <col min="106" max="109" width="9.109375" style="1"/>
-    <col min="110" max="110" width="8.6640625" customWidth="1"/>
-    <col min="111" max="111" width="3.88671875" customWidth="1"/>
-    <col min="112" max="115" width="9.109375" style="1"/>
-    <col min="116" max="116" width="8.6640625" customWidth="1"/>
-    <col min="117" max="117" width="3.88671875" customWidth="1"/>
-    <col min="118" max="121" width="9.109375" style="1"/>
-    <col min="122" max="122" width="8.6640625" customWidth="1"/>
-    <col min="123" max="123" width="3.88671875" customWidth="1"/>
-    <col min="124" max="127" width="9.109375" style="1"/>
-    <col min="128" max="128" width="8.6640625" customWidth="1"/>
-    <col min="129" max="129" width="3.88671875" customWidth="1"/>
-    <col min="130" max="132" width="9.109375" style="1"/>
-    <col min="133" max="133" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="8.6640625" customWidth="1"/>
-    <col min="135" max="135" width="3.88671875" customWidth="1"/>
+    <col min="17" max="19" width="9.140625" style="1"/>
+    <col min="20" max="20" width="8.7109375" customWidth="1"/>
+    <col min="21" max="21" width="3.42578125" customWidth="1"/>
+    <col min="22" max="25" width="9.140625" style="1"/>
+    <col min="26" max="26" width="8.7109375" customWidth="1"/>
+    <col min="27" max="27" width="3.85546875" customWidth="1"/>
+    <col min="28" max="31" width="9.140625" style="1"/>
+    <col min="32" max="32" width="8.7109375" customWidth="1"/>
+    <col min="33" max="33" width="3.85546875" customWidth="1"/>
+    <col min="34" max="37" width="9.140625" style="1"/>
+    <col min="38" max="38" width="8.7109375" customWidth="1"/>
+    <col min="39" max="39" width="3.85546875" customWidth="1"/>
+    <col min="40" max="43" width="9.140625" style="1"/>
+    <col min="44" max="44" width="8.7109375" customWidth="1"/>
+    <col min="45" max="45" width="3.85546875" customWidth="1"/>
+    <col min="46" max="49" width="9.140625" style="1"/>
+    <col min="50" max="50" width="8.7109375" customWidth="1"/>
+    <col min="51" max="51" width="3.85546875" customWidth="1"/>
+    <col min="52" max="55" width="9.140625" style="1"/>
+    <col min="56" max="56" width="8.7109375" customWidth="1"/>
+    <col min="57" max="57" width="3.85546875" customWidth="1"/>
+    <col min="58" max="61" width="9.140625" style="1"/>
+    <col min="62" max="62" width="8.7109375" customWidth="1"/>
+    <col min="63" max="63" width="3.85546875" customWidth="1"/>
+    <col min="64" max="67" width="9.140625" style="1"/>
+    <col min="68" max="68" width="8.7109375" customWidth="1"/>
+    <col min="69" max="69" width="3.85546875" customWidth="1"/>
+    <col min="70" max="73" width="9.140625" style="1"/>
+    <col min="74" max="74" width="8.7109375" customWidth="1"/>
+    <col min="75" max="75" width="3.85546875" customWidth="1"/>
+    <col min="76" max="79" width="9.140625" style="1"/>
+    <col min="80" max="80" width="8.7109375" customWidth="1"/>
+    <col min="81" max="81" width="3.85546875" customWidth="1"/>
+    <col min="82" max="85" width="9.140625" style="1"/>
+    <col min="86" max="86" width="8.7109375" customWidth="1"/>
+    <col min="87" max="87" width="3.85546875" customWidth="1"/>
+    <col min="88" max="91" width="9.140625" style="1"/>
+    <col min="92" max="92" width="8.7109375" customWidth="1"/>
+    <col min="93" max="93" width="3.85546875" customWidth="1"/>
+    <col min="94" max="97" width="9.140625" style="1"/>
+    <col min="98" max="98" width="8.7109375" customWidth="1"/>
+    <col min="99" max="99" width="3.85546875" customWidth="1"/>
+    <col min="100" max="103" width="9.140625" style="1"/>
+    <col min="104" max="104" width="8.7109375" customWidth="1"/>
+    <col min="105" max="105" width="3.85546875" customWidth="1"/>
+    <col min="106" max="109" width="9.140625" style="1"/>
+    <col min="110" max="110" width="8.7109375" customWidth="1"/>
+    <col min="111" max="111" width="3.85546875" customWidth="1"/>
+    <col min="112" max="115" width="9.140625" style="1"/>
+    <col min="116" max="116" width="8.7109375" customWidth="1"/>
+    <col min="117" max="117" width="3.85546875" customWidth="1"/>
+    <col min="118" max="121" width="9.140625" style="1"/>
+    <col min="122" max="122" width="8.7109375" customWidth="1"/>
+    <col min="123" max="123" width="3.85546875" customWidth="1"/>
+    <col min="124" max="127" width="9.140625" style="1"/>
+    <col min="128" max="128" width="8.7109375" customWidth="1"/>
+    <col min="129" max="129" width="3.85546875" customWidth="1"/>
+    <col min="130" max="132" width="9.140625" style="1"/>
+    <col min="133" max="133" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="8.7109375" customWidth="1"/>
+    <col min="135" max="135" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:135">
@@ -1298,181 +1295,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="86">
+      <c r="D1" s="85">
         <v>42322</v>
       </c>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="86">
+      <c r="J1" s="85">
         <v>42323</v>
       </c>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="86">
+      <c r="P1" s="85">
         <v>42324</v>
       </c>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="86">
+      <c r="V1" s="85">
         <v>42325</v>
       </c>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+      <c r="Z1" s="86"/>
       <c r="AA1" s="12"/>
-      <c r="AB1" s="86">
+      <c r="AB1" s="85">
         <v>42326</v>
       </c>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="87"/>
-      <c r="AF1" s="87"/>
+      <c r="AC1" s="86"/>
+      <c r="AD1" s="86"/>
+      <c r="AE1" s="86"/>
+      <c r="AF1" s="86"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="86">
+      <c r="AH1" s="85">
         <v>42327</v>
       </c>
-      <c r="AI1" s="87"/>
-      <c r="AJ1" s="87"/>
-      <c r="AK1" s="87"/>
-      <c r="AL1" s="87"/>
+      <c r="AI1" s="86"/>
+      <c r="AJ1" s="86"/>
+      <c r="AK1" s="86"/>
+      <c r="AL1" s="86"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="86">
+      <c r="AN1" s="85">
         <v>42328</v>
       </c>
-      <c r="AO1" s="87"/>
-      <c r="AP1" s="87"/>
-      <c r="AQ1" s="87"/>
-      <c r="AR1" s="87"/>
+      <c r="AO1" s="86"/>
+      <c r="AP1" s="86"/>
+      <c r="AQ1" s="86"/>
+      <c r="AR1" s="86"/>
       <c r="AS1" s="12"/>
-      <c r="AT1" s="86">
+      <c r="AT1" s="85">
         <v>42329</v>
       </c>
-      <c r="AU1" s="87"/>
-      <c r="AV1" s="87"/>
-      <c r="AW1" s="87"/>
-      <c r="AX1" s="87"/>
+      <c r="AU1" s="86"/>
+      <c r="AV1" s="86"/>
+      <c r="AW1" s="86"/>
+      <c r="AX1" s="86"/>
       <c r="AY1" s="12"/>
-      <c r="AZ1" s="86">
+      <c r="AZ1" s="85">
         <v>42330</v>
       </c>
-      <c r="BA1" s="87"/>
-      <c r="BB1" s="87"/>
-      <c r="BC1" s="87"/>
-      <c r="BD1" s="87"/>
+      <c r="BA1" s="86"/>
+      <c r="BB1" s="86"/>
+      <c r="BC1" s="86"/>
+      <c r="BD1" s="86"/>
       <c r="BE1" s="12"/>
-      <c r="BF1" s="86">
+      <c r="BF1" s="85">
         <v>42331</v>
       </c>
-      <c r="BG1" s="87"/>
-      <c r="BH1" s="87"/>
-      <c r="BI1" s="87"/>
-      <c r="BJ1" s="87"/>
+      <c r="BG1" s="86"/>
+      <c r="BH1" s="86"/>
+      <c r="BI1" s="86"/>
+      <c r="BJ1" s="86"/>
       <c r="BK1" s="12"/>
-      <c r="BL1" s="86">
+      <c r="BL1" s="85">
         <v>42332</v>
       </c>
-      <c r="BM1" s="87"/>
-      <c r="BN1" s="87"/>
-      <c r="BO1" s="87"/>
-      <c r="BP1" s="87"/>
+      <c r="BM1" s="86"/>
+      <c r="BN1" s="86"/>
+      <c r="BO1" s="86"/>
+      <c r="BP1" s="86"/>
       <c r="BQ1" s="12"/>
-      <c r="BR1" s="86">
+      <c r="BR1" s="85">
         <v>42333</v>
       </c>
-      <c r="BS1" s="87"/>
-      <c r="BT1" s="87"/>
-      <c r="BU1" s="87"/>
-      <c r="BV1" s="87"/>
+      <c r="BS1" s="86"/>
+      <c r="BT1" s="86"/>
+      <c r="BU1" s="86"/>
+      <c r="BV1" s="86"/>
       <c r="BW1" s="12"/>
-      <c r="BX1" s="86">
+      <c r="BX1" s="85">
         <v>42334</v>
       </c>
-      <c r="BY1" s="87"/>
-      <c r="BZ1" s="87"/>
-      <c r="CA1" s="87"/>
-      <c r="CB1" s="87"/>
+      <c r="BY1" s="86"/>
+      <c r="BZ1" s="86"/>
+      <c r="CA1" s="86"/>
+      <c r="CB1" s="86"/>
       <c r="CC1" s="12"/>
-      <c r="CD1" s="86">
+      <c r="CD1" s="85">
         <v>42335</v>
       </c>
-      <c r="CE1" s="87"/>
-      <c r="CF1" s="87"/>
-      <c r="CG1" s="87"/>
-      <c r="CH1" s="87"/>
+      <c r="CE1" s="86"/>
+      <c r="CF1" s="86"/>
+      <c r="CG1" s="86"/>
+      <c r="CH1" s="86"/>
       <c r="CI1" s="12"/>
-      <c r="CJ1" s="86">
+      <c r="CJ1" s="85">
         <v>42336</v>
       </c>
-      <c r="CK1" s="87"/>
-      <c r="CL1" s="87"/>
-      <c r="CM1" s="87"/>
-      <c r="CN1" s="87"/>
+      <c r="CK1" s="86"/>
+      <c r="CL1" s="86"/>
+      <c r="CM1" s="86"/>
+      <c r="CN1" s="86"/>
       <c r="CO1" s="12"/>
-      <c r="CP1" s="86">
+      <c r="CP1" s="85">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="87"/>
-      <c r="CR1" s="87"/>
-      <c r="CS1" s="87"/>
-      <c r="CT1" s="87"/>
+      <c r="CQ1" s="86"/>
+      <c r="CR1" s="86"/>
+      <c r="CS1" s="86"/>
+      <c r="CT1" s="86"/>
       <c r="CU1" s="12"/>
-      <c r="CV1" s="86">
+      <c r="CV1" s="85">
         <v>42338</v>
       </c>
-      <c r="CW1" s="87"/>
-      <c r="CX1" s="87"/>
-      <c r="CY1" s="87"/>
-      <c r="CZ1" s="87"/>
+      <c r="CW1" s="86"/>
+      <c r="CX1" s="86"/>
+      <c r="CY1" s="86"/>
+      <c r="CZ1" s="86"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="86">
+      <c r="DB1" s="85">
         <v>42339</v>
       </c>
-      <c r="DC1" s="87"/>
-      <c r="DD1" s="87"/>
-      <c r="DE1" s="87"/>
-      <c r="DF1" s="87"/>
+      <c r="DC1" s="86"/>
+      <c r="DD1" s="86"/>
+      <c r="DE1" s="86"/>
+      <c r="DF1" s="86"/>
       <c r="DG1" s="12"/>
-      <c r="DH1" s="86">
+      <c r="DH1" s="85">
         <v>42340</v>
       </c>
-      <c r="DI1" s="87"/>
-      <c r="DJ1" s="87"/>
-      <c r="DK1" s="87"/>
-      <c r="DL1" s="87"/>
+      <c r="DI1" s="86"/>
+      <c r="DJ1" s="86"/>
+      <c r="DK1" s="86"/>
+      <c r="DL1" s="86"/>
       <c r="DM1" s="12"/>
-      <c r="DN1" s="86">
+      <c r="DN1" s="85">
         <v>42341</v>
       </c>
-      <c r="DO1" s="87"/>
-      <c r="DP1" s="87"/>
-      <c r="DQ1" s="87"/>
-      <c r="DR1" s="87"/>
+      <c r="DO1" s="86"/>
+      <c r="DP1" s="86"/>
+      <c r="DQ1" s="86"/>
+      <c r="DR1" s="86"/>
       <c r="DS1" s="12"/>
-      <c r="DT1" s="86">
+      <c r="DT1" s="85">
         <v>42342</v>
       </c>
-      <c r="DU1" s="87"/>
-      <c r="DV1" s="87"/>
-      <c r="DW1" s="87"/>
-      <c r="DX1" s="87"/>
+      <c r="DU1" s="86"/>
+      <c r="DV1" s="86"/>
+      <c r="DW1" s="86"/>
+      <c r="DX1" s="86"/>
       <c r="DY1" s="12"/>
-      <c r="DZ1" s="86">
+      <c r="DZ1" s="85">
         <v>42343</v>
       </c>
-      <c r="EA1" s="87"/>
-      <c r="EB1" s="87"/>
-      <c r="EC1" s="87"/>
-      <c r="ED1" s="87"/>
+      <c r="EA1" s="86"/>
+      <c r="EB1" s="86"/>
+      <c r="EC1" s="86"/>
+      <c r="ED1" s="86"/>
       <c r="EE1" s="12"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -1834,7 +1831,7 @@
       </c>
       <c r="EE2" s="12"/>
     </row>
-    <row r="3" spans="1:135" s="78" customFormat="1">
+    <row r="3" spans="1:135" s="77" customFormat="1">
       <c r="A3" s="73">
         <v>2</v>
       </c>
@@ -1907,7 +1904,9 @@
       <c r="AN3" s="71">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AO3" s="77"/>
+      <c r="AO3" s="72">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="AP3" s="74"/>
       <c r="AQ3" s="74"/>
       <c r="AR3" s="75"/>
@@ -2045,7 +2044,9 @@
       <c r="DT3" s="71">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="DU3" s="77"/>
+      <c r="DU3" s="72">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="DV3" s="74"/>
       <c r="DW3" s="74"/>
       <c r="DX3" s="75"/>
@@ -2053,7 +2054,9 @@
       <c r="DZ3" s="71">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="EA3" s="77"/>
+      <c r="EA3" s="72">
+        <v>0</v>
+      </c>
       <c r="EB3" s="74"/>
       <c r="EC3" s="74"/>
       <c r="ED3" s="75"/>
@@ -2519,7 +2522,9 @@
       <c r="D7" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F7" s="8">
         <v>1</v>
       </c>
@@ -2666,13 +2671,15 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="87" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E8" s="7"/>
+      <c r="E8" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F8" s="8">
         <v>0</v>
       </c>
@@ -2816,7 +2823,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="88"/>
+      <c r="C9" s="87"/>
       <c r="D9" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -2966,13 +2973,15 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="90" t="s">
+      <c r="C10" s="89" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F10" s="8">
         <v>0</v>
       </c>
@@ -3116,11 +3125,13 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="88"/>
+      <c r="C11" s="87"/>
       <c r="D11" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="F11" s="8">
         <v>0</v>
       </c>
@@ -3264,13 +3275,15 @@
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="90" t="s">
+      <c r="C12" s="89" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
       <c r="F12" s="8">
         <v>0</v>
       </c>
@@ -3426,11 +3439,13 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="88"/>
+      <c r="C13" s="87"/>
       <c r="D13" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
       <c r="F13" s="8">
         <v>0</v>
       </c>
@@ -3456,13 +3471,11 @@
       <c r="S13" s="9"/>
       <c r="T13" s="54"/>
       <c r="U13" s="12"/>
-      <c r="V13" s="6">
-        <v>0</v>
-      </c>
+      <c r="V13" s="6"/>
       <c r="W13" s="7"/>
       <c r="X13" s="8"/>
       <c r="Y13" s="9"/>
-      <c r="Z13" s="54"/>
+      <c r="Z13" s="69"/>
       <c r="AA13" s="12"/>
       <c r="AB13" s="6"/>
       <c r="AC13" s="7"/>
@@ -3580,11 +3593,13 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="88"/>
+      <c r="C14" s="87"/>
       <c r="D14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
       <c r="F14" s="8">
         <v>0</v>
       </c>
@@ -3768,7 +3783,9 @@
       <c r="AN15" s="56">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AO15" s="7"/>
+      <c r="AO15" s="7">
+        <v>0</v>
+      </c>
       <c r="AP15" s="8"/>
       <c r="AQ15" s="9"/>
       <c r="AR15" s="53"/>
@@ -3915,7 +3932,9 @@
       <c r="AN16" s="56">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AO16" s="7"/>
+      <c r="AO16" s="7">
+        <v>0</v>
+      </c>
       <c r="AP16" s="8"/>
       <c r="AQ16" s="9"/>
       <c r="AR16" s="62"/>
@@ -4058,7 +4077,9 @@
       <c r="AN17" s="56">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AO17" s="7"/>
+      <c r="AO17" s="7">
+        <v>0</v>
+      </c>
       <c r="AP17" s="8"/>
       <c r="AQ17" s="9"/>
       <c r="AR17" s="63"/>
@@ -4201,10 +4222,12 @@
       <c r="AN18" s="56">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="AO18" s="7"/>
+      <c r="AO18" s="7">
+        <v>0</v>
+      </c>
       <c r="AP18" s="8"/>
       <c r="AQ18" s="9"/>
-      <c r="AR18" s="81"/>
+      <c r="AR18" s="80"/>
       <c r="AS18" s="12"/>
       <c r="AT18" s="6"/>
       <c r="AU18" s="7"/>
@@ -4390,7 +4413,9 @@
       <c r="CD19" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="CE19" s="7"/>
+      <c r="CE19" s="7">
+        <v>0</v>
+      </c>
       <c r="CF19" s="8"/>
       <c r="CG19" s="9"/>
       <c r="CH19" s="52"/>
@@ -4533,7 +4558,9 @@
       <c r="CD20" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="CE20" s="7"/>
+      <c r="CE20" s="7">
+        <v>0</v>
+      </c>
       <c r="CF20" s="8"/>
       <c r="CG20" s="9"/>
       <c r="CH20" s="54"/>
@@ -4634,7 +4661,9 @@
       <c r="AN21" s="66">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AO21" s="7"/>
+      <c r="AO21" s="7">
+        <v>0</v>
+      </c>
       <c r="AP21" s="8"/>
       <c r="AQ21" s="9"/>
       <c r="AR21" s="53"/>
@@ -4777,7 +4806,9 @@
       <c r="AN22" s="66">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AO22" s="7"/>
+      <c r="AO22" s="7">
+        <v>0</v>
+      </c>
       <c r="AP22" s="8"/>
       <c r="AQ22" s="9"/>
       <c r="AR22" s="62"/>
@@ -4924,7 +4955,9 @@
       <c r="AN23" s="66">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AO23" s="7"/>
+      <c r="AO23" s="7">
+        <v>0</v>
+      </c>
       <c r="AP23" s="8"/>
       <c r="AQ23" s="9"/>
       <c r="AR23" s="63"/>
@@ -5212,10 +5245,12 @@
       <c r="AN25" s="56">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="AO25" s="7"/>
+      <c r="AO25" s="7">
+        <v>0</v>
+      </c>
       <c r="AP25" s="8"/>
       <c r="AQ25" s="9"/>
-      <c r="AR25" s="80"/>
+      <c r="AR25" s="79"/>
       <c r="AS25" s="12"/>
       <c r="AT25" s="6"/>
       <c r="AU25" s="7"/>
@@ -5256,7 +5291,9 @@
       <c r="CD25" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="CE25" s="7"/>
+      <c r="CE25" s="7">
+        <v>0</v>
+      </c>
       <c r="CF25" s="8"/>
       <c r="CG25" s="9"/>
       <c r="CH25" s="52"/>
@@ -5317,7 +5354,7 @@
       <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="91" t="s">
+      <c r="C26" s="90" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="6"/>
@@ -5407,7 +5444,9 @@
       <c r="CJ26" s="6">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="CK26" s="7"/>
+      <c r="CK26" s="7">
+        <v>0</v>
+      </c>
       <c r="CL26" s="8"/>
       <c r="CM26" s="9"/>
       <c r="CN26" s="52"/>
@@ -5462,7 +5501,7 @@
       <c r="B27" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="92"/>
+      <c r="C27" s="91"/>
       <c r="D27" s="6"/>
       <c r="E27" s="7"/>
       <c r="F27" s="8"/>
@@ -5550,7 +5589,9 @@
       <c r="CJ27" s="6">
         <v>2.0833333333333332E-2</v>
       </c>
-      <c r="CK27" s="7"/>
+      <c r="CK27" s="7">
+        <v>0</v>
+      </c>
       <c r="CL27" s="8"/>
       <c r="CM27" s="9"/>
       <c r="CN27" s="54"/>
@@ -5893,7 +5934,7 @@
       <c r="B30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="88" t="s">
+      <c r="C30" s="87" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="6"/>
@@ -6025,7 +6066,9 @@
       <c r="DZ30" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="EA30" s="7"/>
+      <c r="EA30" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="EB30" s="8"/>
       <c r="EC30" s="8"/>
       <c r="ED30" s="53"/>
@@ -6038,7 +6081,7 @@
       <c r="B31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="88"/>
+      <c r="C31" s="87"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -6168,7 +6211,9 @@
       <c r="DZ31" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="EA31" s="7"/>
+      <c r="EA31" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="EB31" s="8"/>
       <c r="EC31" s="9"/>
       <c r="ED31" s="52"/>
@@ -6181,7 +6226,7 @@
       <c r="B32" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="88"/>
+      <c r="C32" s="87"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
@@ -6311,7 +6356,9 @@
       <c r="DZ32" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="EA32" s="7"/>
+      <c r="EA32" s="7">
+        <v>0</v>
+      </c>
       <c r="EB32" s="8"/>
       <c r="EC32" s="9"/>
       <c r="ED32" s="54"/>
@@ -6452,7 +6499,9 @@
       <c r="DT33" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="DU33" s="7"/>
+      <c r="DU33" s="7">
+        <v>0</v>
+      </c>
       <c r="DV33" s="8"/>
       <c r="DW33" s="9"/>
       <c r="DX33" s="54"/>
@@ -6461,7 +6510,7 @@
       <c r="EA33" s="7"/>
       <c r="EB33" s="8"/>
       <c r="EC33" s="9"/>
-      <c r="ED33" s="54"/>
+      <c r="ED33" s="69"/>
       <c r="EE33" s="12"/>
     </row>
     <row r="34" spans="1:135">
@@ -6553,7 +6602,9 @@
       <c r="CD34" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="CE34" s="7"/>
+      <c r="CE34" s="7">
+        <v>0</v>
+      </c>
       <c r="CF34" s="8"/>
       <c r="CG34" s="9"/>
       <c r="CH34" s="52"/>
@@ -6601,7 +6652,9 @@
       <c r="DT34" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DU34" s="7"/>
+      <c r="DU34" s="7">
+        <v>0</v>
+      </c>
       <c r="DV34" s="8"/>
       <c r="DW34" s="9"/>
       <c r="DX34" s="52"/>
@@ -6709,7 +6762,7 @@
       <c r="CK35" s="7"/>
       <c r="CL35" s="8"/>
       <c r="CM35" s="9"/>
-      <c r="CN35" s="54"/>
+      <c r="CN35" s="69"/>
       <c r="CO35" s="12"/>
       <c r="CP35" s="6"/>
       <c r="CQ35" s="7"/>
@@ -6744,7 +6797,9 @@
       <c r="DT35" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DU35" s="7"/>
+      <c r="DU35" s="7">
+        <v>0</v>
+      </c>
       <c r="DV35" s="8"/>
       <c r="DW35" s="9"/>
       <c r="DX35" s="53"/>
@@ -6947,7 +7002,9 @@
       <c r="AE37" s="9"/>
       <c r="AF37" s="10"/>
       <c r="AG37" s="12"/>
-      <c r="AH37" s="6"/>
+      <c r="AH37" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="AI37" s="7">
         <v>0.10416666666666667</v>
       </c>
@@ -7059,7 +7116,7 @@
       <c r="B38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="88" t="s">
+      <c r="C38" s="87" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="6"/>
@@ -7202,7 +7259,7 @@
       <c r="B39" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="88"/>
+      <c r="C39" s="87"/>
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
@@ -7483,7 +7540,7 @@
       <c r="ED40" s="10"/>
       <c r="EE40" s="12"/>
     </row>
-    <row r="41" spans="1:135" ht="28.8">
+    <row r="41" spans="1:135" ht="30">
       <c r="A41" s="2"/>
       <c r="B41" s="17" t="s">
         <v>77</v>
@@ -7536,7 +7593,9 @@
       <c r="AT41" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="AU41" s="7"/>
+      <c r="AU41" s="7">
+        <v>0</v>
+      </c>
       <c r="AV41" s="8"/>
       <c r="AW41" s="9"/>
       <c r="AX41" s="54"/>
@@ -7626,7 +7685,7 @@
       <c r="ED41" s="10"/>
       <c r="EE41" s="12"/>
     </row>
-    <row r="42" spans="1:135" ht="28.8">
+    <row r="42" spans="1:135" ht="30">
       <c r="A42" s="2"/>
       <c r="B42" s="17" t="s">
         <v>77</v>
@@ -7721,7 +7780,9 @@
       <c r="CJ42" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="CK42" s="7"/>
+      <c r="CK42" s="7">
+        <v>0</v>
+      </c>
       <c r="CL42" s="8"/>
       <c r="CM42" s="9"/>
       <c r="CN42" s="54"/>
@@ -7861,7 +7922,7 @@
       <c r="CK43" s="7"/>
       <c r="CL43" s="8"/>
       <c r="CM43" s="9"/>
-      <c r="CN43" s="54"/>
+      <c r="CN43" s="69"/>
       <c r="CO43" s="12"/>
       <c r="CP43" s="6"/>
       <c r="CQ43" s="7"/>
@@ -8006,7 +8067,7 @@
       <c r="CK44" s="7"/>
       <c r="CL44" s="8"/>
       <c r="CM44" s="9"/>
-      <c r="CN44" s="54"/>
+      <c r="CN44" s="69"/>
       <c r="CO44" s="12"/>
       <c r="CP44" s="6"/>
       <c r="CQ44" s="7"/>
@@ -8140,7 +8201,9 @@
       <c r="CD45" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="CE45" s="7"/>
+      <c r="CE45" s="7">
+        <v>0</v>
+      </c>
       <c r="CF45" s="8"/>
       <c r="CG45" s="9"/>
       <c r="CH45" s="54"/>
@@ -8149,7 +8212,7 @@
       <c r="CK45" s="7"/>
       <c r="CL45" s="8"/>
       <c r="CM45" s="9"/>
-      <c r="CN45" s="54"/>
+      <c r="CN45" s="69"/>
       <c r="CO45" s="12"/>
       <c r="CP45" s="6"/>
       <c r="CQ45" s="7"/>
@@ -8290,7 +8353,7 @@
       <c r="CK46" s="7"/>
       <c r="CL46" s="8"/>
       <c r="CM46" s="9"/>
-      <c r="CN46" s="54"/>
+      <c r="CN46" s="69"/>
       <c r="CO46" s="12"/>
       <c r="CP46" s="6"/>
       <c r="CQ46" s="7"/>
@@ -8329,7 +8392,9 @@
       <c r="DT46" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="DU46" s="7"/>
+      <c r="DU46" s="7">
+        <v>0</v>
+      </c>
       <c r="DV46" s="8"/>
       <c r="DW46" s="9"/>
       <c r="DX46" s="54"/>
@@ -8393,7 +8458,7 @@
       </c>
       <c r="AJ47" s="59"/>
       <c r="AK47" s="60"/>
-      <c r="AL47" s="79"/>
+      <c r="AL47" s="78"/>
       <c r="AM47" s="12"/>
       <c r="AN47" s="6"/>
       <c r="AO47" s="7"/>
@@ -8685,7 +8750,9 @@
       <c r="AN49" s="6">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="AO49" s="7"/>
+      <c r="AO49" s="7">
+        <v>6.25E-2</v>
+      </c>
       <c r="AP49" s="8"/>
       <c r="AQ49" s="9"/>
       <c r="AR49" s="53"/>
@@ -8845,45 +8912,29 @@
       <c r="BC50" s="18"/>
       <c r="BD50" s="10"/>
       <c r="BE50" s="12"/>
-      <c r="BF50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="BG50" s="83">
-        <v>0</v>
-      </c>
+      <c r="BF50" s="14"/>
+      <c r="BG50" s="82"/>
       <c r="BH50" s="18"/>
       <c r="BI50" s="18"/>
-      <c r="BJ50" s="52"/>
+      <c r="BJ50" s="69"/>
       <c r="BK50" s="12"/>
-      <c r="BL50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="BM50" s="18">
-        <v>0</v>
-      </c>
+      <c r="BL50" s="14"/>
+      <c r="BM50" s="18"/>
       <c r="BN50" s="18"/>
       <c r="BO50" s="18"/>
-      <c r="BP50" s="52"/>
+      <c r="BP50" s="69"/>
       <c r="BQ50" s="12"/>
-      <c r="BR50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="BS50" s="83">
-        <v>0</v>
-      </c>
+      <c r="BR50" s="14"/>
+      <c r="BS50" s="82"/>
       <c r="BT50" s="18"/>
       <c r="BU50" s="18"/>
-      <c r="BV50" s="52"/>
+      <c r="BV50" s="69"/>
       <c r="BW50" s="12"/>
-      <c r="BX50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="BY50" s="83">
-        <v>0</v>
-      </c>
+      <c r="BX50" s="14"/>
+      <c r="BY50" s="82"/>
       <c r="BZ50" s="18"/>
       <c r="CA50" s="18"/>
-      <c r="CB50" s="52"/>
+      <c r="CB50" s="69"/>
       <c r="CC50" s="12"/>
       <c r="CD50" s="14"/>
       <c r="CE50" s="18"/>
@@ -8891,55 +8942,40 @@
       <c r="CG50" s="18"/>
       <c r="CH50" s="10"/>
       <c r="CI50" s="12"/>
-      <c r="CJ50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
       <c r="CK50" s="18"/>
       <c r="CL50" s="18"/>
       <c r="CM50" s="18"/>
-      <c r="CN50" s="52"/>
+      <c r="CN50" s="69"/>
       <c r="CO50" s="12"/>
-      <c r="CP50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="CP50" s="14"/>
       <c r="CQ50" s="18"/>
       <c r="CR50" s="18"/>
       <c r="CS50" s="18"/>
-      <c r="CT50" s="52"/>
+      <c r="CT50" s="69"/>
       <c r="CU50" s="12"/>
-      <c r="CV50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="CV50" s="14"/>
       <c r="CW50" s="18"/>
       <c r="CX50" s="18"/>
       <c r="CY50" s="18"/>
-      <c r="CZ50" s="52"/>
+      <c r="CZ50" s="69"/>
       <c r="DA50" s="12"/>
-      <c r="DB50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="DB50" s="14"/>
       <c r="DC50" s="18"/>
       <c r="DD50" s="18"/>
       <c r="DE50" s="18"/>
-      <c r="DF50" s="52"/>
+      <c r="DF50" s="69"/>
       <c r="DG50" s="12"/>
-      <c r="DH50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="DI50" s="83">
-        <v>0</v>
-      </c>
+      <c r="DH50" s="14"/>
+      <c r="DI50" s="82"/>
       <c r="DJ50" s="18"/>
       <c r="DK50" s="18"/>
-      <c r="DL50" s="52"/>
+      <c r="DL50" s="69"/>
       <c r="DM50" s="12"/>
-      <c r="DN50" s="14">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="DN50" s="14"/>
       <c r="DO50" s="18"/>
       <c r="DP50" s="18"/>
       <c r="DQ50" s="18"/>
-      <c r="DR50" s="52"/>
+      <c r="DR50" s="69"/>
       <c r="DS50" s="12"/>
       <c r="DT50" s="14"/>
       <c r="DU50" s="18"/>
@@ -8959,7 +8995,7 @@
       <c r="B51" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C51" s="82" t="s">
+      <c r="C51" s="81" t="s">
         <v>64</v>
       </c>
       <c r="D51" s="14"/>
@@ -9013,7 +9049,7 @@
       <c r="AZ51" s="14">
         <v>0</v>
       </c>
-      <c r="BA51" s="83">
+      <c r="BA51" s="82">
         <v>0.33333333333333331</v>
       </c>
       <c r="BB51" s="18"/>
@@ -9021,9 +9057,9 @@
       <c r="BD51" s="52"/>
       <c r="BE51" s="12"/>
       <c r="BF51" s="14">
-        <v>0</v>
-      </c>
-      <c r="BG51" s="83">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="BG51" s="82">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="BH51" s="18"/>
@@ -9031,9 +9067,9 @@
       <c r="BJ51" s="52"/>
       <c r="BK51" s="12"/>
       <c r="BL51" s="14">
-        <v>0</v>
-      </c>
-      <c r="BM51" s="83">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="BM51" s="82">
         <v>0.20833333333333334</v>
       </c>
       <c r="BN51" s="18"/>
@@ -9041,9 +9077,9 @@
       <c r="BP51" s="52"/>
       <c r="BQ51" s="12"/>
       <c r="BR51" s="14">
-        <v>0</v>
-      </c>
-      <c r="BS51" s="83">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="BS51" s="82">
         <v>0.125</v>
       </c>
       <c r="BT51" s="18"/>
@@ -9051,9 +9087,9 @@
       <c r="BV51" s="52"/>
       <c r="BW51" s="12"/>
       <c r="BX51" s="14">
-        <v>0</v>
-      </c>
-      <c r="BY51" s="83">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="BY51" s="82">
         <v>0.16666666666666666</v>
       </c>
       <c r="BZ51" s="18"/>
@@ -9066,57 +9102,75 @@
       <c r="CG51" s="18"/>
       <c r="CH51" s="10"/>
       <c r="CI51" s="12"/>
-      <c r="CJ51" s="14"/>
-      <c r="CK51" s="18"/>
+      <c r="CJ51" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="CK51" s="82">
+        <v>0</v>
+      </c>
       <c r="CL51" s="18"/>
       <c r="CM51" s="18"/>
       <c r="CN51" s="52"/>
       <c r="CO51" s="12"/>
-      <c r="CP51" s="14"/>
-      <c r="CQ51" s="18"/>
+      <c r="CP51" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="CQ51" s="82">
+        <v>0</v>
+      </c>
       <c r="CR51" s="18"/>
       <c r="CS51" s="18"/>
       <c r="CT51" s="52"/>
       <c r="CU51" s="12"/>
-      <c r="CV51" s="14"/>
-      <c r="CW51" s="83">
+      <c r="CV51" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="CW51" s="82">
         <v>0.125</v>
       </c>
       <c r="CX51" s="18"/>
       <c r="CY51" s="18"/>
       <c r="CZ51" s="52"/>
       <c r="DA51" s="12"/>
-      <c r="DB51" s="14"/>
-      <c r="DC51" s="83">
+      <c r="DB51" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="DC51" s="82">
         <v>0.16666666666666666</v>
       </c>
       <c r="DD51" s="18"/>
       <c r="DE51" s="18"/>
       <c r="DF51" s="52"/>
       <c r="DG51" s="12"/>
-      <c r="DH51" s="14"/>
-      <c r="DI51" s="83">
+      <c r="DH51" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="DI51" s="82">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="DJ51" s="18"/>
       <c r="DK51" s="18"/>
       <c r="DL51" s="52"/>
       <c r="DM51" s="12"/>
-      <c r="DN51" s="14"/>
-      <c r="DO51" s="83">
+      <c r="DN51" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="DO51" s="82">
         <v>0.16666666666666666</v>
       </c>
       <c r="DP51" s="18"/>
       <c r="DQ51" s="18"/>
       <c r="DR51" s="52"/>
       <c r="DS51" s="12"/>
-      <c r="DT51" s="14"/>
-      <c r="DU51" s="83">
-        <v>0.10416666666666667</v>
+      <c r="DT51" s="14">
+        <v>0</v>
+      </c>
+      <c r="DU51" s="82">
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="DV51" s="18"/>
       <c r="DW51" s="18"/>
-      <c r="DX51" s="10"/>
+      <c r="DX51" s="52"/>
       <c r="DY51" s="12"/>
       <c r="DZ51" s="14"/>
       <c r="EA51" s="18"/>
@@ -9186,7 +9240,7 @@
       <c r="AZ52" s="14">
         <v>0</v>
       </c>
-      <c r="BA52" s="83">
+      <c r="BA52" s="82">
         <v>0.20833333333333334</v>
       </c>
       <c r="BB52" s="18"/>
@@ -9196,7 +9250,7 @@
       <c r="BF52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BG52" s="83">
+      <c r="BG52" s="82">
         <v>0.14583333333333334</v>
       </c>
       <c r="BH52" s="18"/>
@@ -9206,7 +9260,7 @@
       <c r="BL52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BM52" s="83">
+      <c r="BM52" s="82">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="BN52" s="18"/>
@@ -9216,7 +9270,7 @@
       <c r="BR52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BS52" s="83">
+      <c r="BS52" s="82">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="BT52" s="18"/>
@@ -9226,7 +9280,7 @@
       <c r="BX52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BY52" s="83">
+      <c r="BY52" s="82">
         <v>6.25E-2</v>
       </c>
       <c r="BZ52" s="18"/>
@@ -9242,7 +9296,9 @@
       <c r="CJ52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="CK52" s="18"/>
+      <c r="CK52" s="82">
+        <v>4.1666666666666699E-2</v>
+      </c>
       <c r="CL52" s="18"/>
       <c r="CM52" s="18"/>
       <c r="CN52" s="54"/>
@@ -9250,7 +9306,7 @@
       <c r="CP52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="CQ52" s="83">
+      <c r="CQ52" s="82">
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="CR52" s="18"/>
@@ -9260,7 +9316,7 @@
       <c r="CV52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="CW52" s="83">
+      <c r="CW52" s="82">
         <v>0.14583333333333334</v>
       </c>
       <c r="CX52" s="18"/>
@@ -9270,7 +9326,7 @@
       <c r="DB52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DC52" s="83">
+      <c r="DC52" s="82">
         <v>0.125</v>
       </c>
       <c r="DD52" s="18"/>
@@ -9280,7 +9336,7 @@
       <c r="DH52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DI52" s="83">
+      <c r="DI52" s="82">
         <v>0.16666666666666666</v>
       </c>
       <c r="DJ52" s="18"/>
@@ -9290,7 +9346,9 @@
       <c r="DN52" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DO52" s="18"/>
+      <c r="DO52" s="82">
+        <v>0.125</v>
+      </c>
       <c r="DP52" s="18"/>
       <c r="DQ52" s="18"/>
       <c r="DR52" s="54"/>
@@ -9375,7 +9433,7 @@
       <c r="BF53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BG53" s="83">
+      <c r="BG53" s="82">
         <v>0</v>
       </c>
       <c r="BH53" s="18"/>
@@ -9385,7 +9443,7 @@
       <c r="BL53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BM53" s="83">
+      <c r="BM53" s="82">
         <v>0</v>
       </c>
       <c r="BN53" s="18"/>
@@ -9395,7 +9453,7 @@
       <c r="BR53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BS53" s="83">
+      <c r="BS53" s="82">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="BT53" s="18"/>
@@ -9405,7 +9463,7 @@
       <c r="BX53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="BY53" s="83">
+      <c r="BY53" s="82">
         <v>6.25E-2</v>
       </c>
       <c r="BZ53" s="18"/>
@@ -9421,7 +9479,9 @@
       <c r="CJ53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="CK53" s="18"/>
+      <c r="CK53" s="82">
+        <v>8.3333333333333301E-2</v>
+      </c>
       <c r="CL53" s="18"/>
       <c r="CM53" s="18"/>
       <c r="CN53" s="53"/>
@@ -9429,7 +9489,7 @@
       <c r="CP53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="CQ53" s="83">
+      <c r="CQ53" s="82">
         <v>0</v>
       </c>
       <c r="CR53" s="18"/>
@@ -9439,7 +9499,7 @@
       <c r="CV53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="CW53" s="83">
+      <c r="CW53" s="82">
         <v>0</v>
       </c>
       <c r="CX53" s="18"/>
@@ -9449,7 +9509,7 @@
       <c r="DB53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DC53" s="83">
+      <c r="DC53" s="82">
         <v>6.25E-2</v>
       </c>
       <c r="DD53" s="18"/>
@@ -9459,7 +9519,7 @@
       <c r="DH53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DI53" s="83">
+      <c r="DI53" s="82">
         <v>0.10416666666666667</v>
       </c>
       <c r="DJ53" s="18"/>
@@ -9469,7 +9529,7 @@
       <c r="DN53" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="DO53" s="83">
+      <c r="DO53" s="82">
         <v>0</v>
       </c>
       <c r="DP53" s="18"/>
@@ -9496,7 +9556,7 @@
       <c r="B54" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="89" t="s">
+      <c r="C54" s="88" t="s">
         <v>20</v>
       </c>
       <c r="D54" s="14"/>
@@ -9639,7 +9699,7 @@
       <c r="B55" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="89"/>
+      <c r="C55" s="88"/>
       <c r="D55" s="14"/>
       <c r="E55" s="18"/>
       <c r="F55" s="8"/>
@@ -9921,140 +9981,144 @@
       <c r="B57" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C57" s="85" t="s">
+      <c r="C57" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="D57" s="84"/>
+      <c r="D57" s="83"/>
       <c r="E57" s="18"/>
       <c r="F57" s="8"/>
       <c r="G57" s="18"/>
       <c r="H57" s="10"/>
       <c r="I57" s="12"/>
-      <c r="J57" s="84"/>
+      <c r="J57" s="83"/>
       <c r="K57" s="18"/>
       <c r="L57" s="18"/>
       <c r="M57" s="18"/>
       <c r="N57" s="10"/>
       <c r="O57" s="12"/>
-      <c r="P57" s="84"/>
+      <c r="P57" s="83"/>
       <c r="Q57" s="18"/>
       <c r="R57" s="18"/>
       <c r="S57" s="18"/>
       <c r="T57" s="10"/>
       <c r="U57" s="12"/>
-      <c r="V57" s="84"/>
+      <c r="V57" s="83"/>
       <c r="W57" s="18"/>
       <c r="X57" s="18"/>
       <c r="Y57" s="18"/>
       <c r="Z57" s="10"/>
       <c r="AA57" s="12"/>
-      <c r="AB57" s="84"/>
+      <c r="AB57" s="83"/>
       <c r="AC57" s="18"/>
       <c r="AD57" s="18"/>
       <c r="AE57" s="18"/>
       <c r="AF57" s="10"/>
       <c r="AG57" s="12"/>
-      <c r="AH57" s="84"/>
+      <c r="AH57" s="83"/>
       <c r="AI57" s="18"/>
       <c r="AJ57" s="18"/>
       <c r="AK57" s="18"/>
       <c r="AL57" s="10"/>
       <c r="AM57" s="12"/>
-      <c r="AN57" s="84"/>
+      <c r="AN57" s="83"/>
       <c r="AO57" s="18"/>
       <c r="AP57" s="18"/>
       <c r="AQ57" s="18"/>
       <c r="AR57" s="10"/>
       <c r="AS57" s="12"/>
-      <c r="AT57" s="84"/>
+      <c r="AT57" s="83"/>
       <c r="AU57" s="18"/>
       <c r="AV57" s="18"/>
       <c r="AW57" s="18"/>
       <c r="AX57" s="10"/>
       <c r="AY57" s="12"/>
-      <c r="AZ57" s="84"/>
+      <c r="AZ57" s="83"/>
       <c r="BA57" s="18"/>
       <c r="BB57" s="18"/>
       <c r="BC57" s="18"/>
       <c r="BD57" s="10"/>
       <c r="BE57" s="12"/>
-      <c r="BF57" s="84"/>
+      <c r="BF57" s="83"/>
       <c r="BG57" s="18"/>
       <c r="BH57" s="18"/>
       <c r="BI57" s="18"/>
       <c r="BJ57" s="10"/>
       <c r="BK57" s="12"/>
-      <c r="BL57" s="84"/>
+      <c r="BL57" s="83"/>
       <c r="BM57" s="18"/>
       <c r="BN57" s="18"/>
       <c r="BO57" s="18"/>
       <c r="BP57" s="10"/>
       <c r="BQ57" s="12"/>
-      <c r="BR57" s="84"/>
+      <c r="BR57" s="83"/>
       <c r="BS57" s="18"/>
       <c r="BT57" s="18"/>
       <c r="BU57" s="18"/>
       <c r="BV57" s="10"/>
       <c r="BW57" s="12"/>
-      <c r="BX57" s="84"/>
+      <c r="BX57" s="83"/>
       <c r="BY57" s="18"/>
       <c r="BZ57" s="18"/>
       <c r="CA57" s="18"/>
       <c r="CB57" s="10"/>
       <c r="CC57" s="12"/>
-      <c r="CD57" s="84"/>
+      <c r="CD57" s="83"/>
       <c r="CE57" s="18"/>
       <c r="CF57" s="18"/>
       <c r="CG57" s="18"/>
       <c r="CH57" s="10"/>
       <c r="CI57" s="12"/>
-      <c r="CJ57" s="84"/>
+      <c r="CJ57" s="83"/>
       <c r="CK57" s="18"/>
       <c r="CL57" s="18"/>
       <c r="CM57" s="18"/>
       <c r="CN57" s="10"/>
       <c r="CO57" s="12"/>
-      <c r="CP57" s="84"/>
+      <c r="CP57" s="83"/>
       <c r="CQ57" s="18"/>
       <c r="CR57" s="18"/>
       <c r="CS57" s="18"/>
       <c r="CT57" s="10"/>
       <c r="CU57" s="12"/>
-      <c r="CV57" s="84"/>
+      <c r="CV57" s="83"/>
       <c r="CW57" s="18"/>
       <c r="CX57" s="18"/>
       <c r="CY57" s="18"/>
       <c r="CZ57" s="10"/>
       <c r="DA57" s="12"/>
-      <c r="DB57" s="84">
-        <v>0</v>
-      </c>
-      <c r="DC57" s="83">
+      <c r="DB57" s="83">
+        <v>0</v>
+      </c>
+      <c r="DC57" s="82">
         <v>6.25E-2</v>
       </c>
       <c r="DD57" s="18"/>
       <c r="DE57" s="18"/>
       <c r="DF57" s="53"/>
       <c r="DG57" s="12"/>
-      <c r="DH57" s="84"/>
+      <c r="DH57" s="83"/>
       <c r="DI57" s="18"/>
       <c r="DJ57" s="18"/>
       <c r="DK57" s="18"/>
       <c r="DL57" s="10"/>
       <c r="DM57" s="12"/>
-      <c r="DN57" s="84"/>
+      <c r="DN57" s="83"/>
       <c r="DO57" s="18"/>
       <c r="DP57" s="18"/>
       <c r="DQ57" s="18"/>
       <c r="DR57" s="10"/>
       <c r="DS57" s="12"/>
-      <c r="DT57" s="84"/>
-      <c r="DU57" s="18"/>
+      <c r="DT57" s="83">
+        <v>0</v>
+      </c>
+      <c r="DU57" s="82">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="DV57" s="18"/>
       <c r="DW57" s="18"/>
-      <c r="DX57" s="10"/>
+      <c r="DX57" s="53"/>
       <c r="DY57" s="12"/>
-      <c r="DZ57" s="84"/>
+      <c r="DZ57" s="83"/>
       <c r="EA57" s="18"/>
       <c r="EB57" s="18"/>
       <c r="EC57" s="18"/>
@@ -10640,7 +10704,7 @@
       <c r="B62" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="89" t="s">
+      <c r="C62" s="88" t="s">
         <v>30</v>
       </c>
       <c r="D62" s="14"/>
@@ -10783,7 +10847,7 @@
       <c r="B63" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C63" s="89"/>
+      <c r="C63" s="88"/>
       <c r="D63" s="14"/>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
@@ -10924,7 +10988,7 @@
       <c r="B64" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C64" s="89"/>
+      <c r="C64" s="88"/>
       <c r="D64" s="14"/>
       <c r="E64" s="18"/>
       <c r="F64" s="18"/>
@@ -11601,7 +11665,7 @@
       </c>
       <c r="ED67" s="16"/>
     </row>
-    <row r="68" spans="1:135" ht="15" thickBot="1">
+    <row r="68" spans="1:135" ht="15.75" thickBot="1">
       <c r="C68" s="27" t="s">
         <v>36</v>
       </c>
@@ -11611,7 +11675,7 @@
       </c>
       <c r="E68" s="29">
         <f>SUM(E3:E65)</f>
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F68" s="30" t="s">
         <v>37</v>
@@ -11687,7 +11751,7 @@
       <c r="AF68" s="31"/>
       <c r="AH68" s="28">
         <f>SUM(AH3:AH65)</f>
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AI68" s="29">
         <f>SUM(AI3:AI65)</f>
@@ -11707,7 +11771,7 @@
       </c>
       <c r="AO68" s="29">
         <f>SUM(AO3:AO65)</f>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="AP68" s="30" t="s">
         <v>37</v>
@@ -11835,7 +11899,7 @@
       </c>
       <c r="CK68" s="29">
         <f>SUM(CK3:CK65)</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="CL68" s="30" t="s">
         <v>37</v>
@@ -11915,7 +11979,7 @@
       </c>
       <c r="DO68" s="29">
         <f>SUM(DO3:DO65)</f>
-        <v>0.33333333333333331</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="DP68" s="30" t="s">
         <v>37</v>
@@ -11931,7 +11995,7 @@
       </c>
       <c r="DU68" s="29">
         <f>SUM(DU3:DU65)</f>
-        <v>0.10416666666666667</v>
+        <v>0.20833333333333331</v>
       </c>
       <c r="DV68" s="30" t="s">
         <v>37</v>
@@ -11947,7 +12011,7 @@
       </c>
       <c r="EA68" s="29">
         <f>SUM(EA3:EA65)</f>
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="EB68" s="30" t="s">
         <v>37</v>
@@ -11964,7 +12028,7 @@
       </c>
       <c r="E69" s="33">
         <f>G68/E68</f>
-        <v>6.75</v>
+        <v>3.375</v>
       </c>
       <c r="H69" s="34"/>
       <c r="J69" s="32" t="s">
@@ -12010,9 +12074,9 @@
       <c r="AN69" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="AO69" s="33" t="e">
+      <c r="AO69" s="33">
         <f>AQ68/AO68</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="AR69" s="34"/>
       <c r="AT69" s="32" t="s">
@@ -12074,9 +12138,9 @@
       <c r="CJ69" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="CK69" s="33" t="e">
+      <c r="CK69" s="33">
         <f>CM68/CK68</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="CN69" s="34"/>
       <c r="CP69" s="32" t="s">
@@ -12130,9 +12194,9 @@
       <c r="DZ69" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="EA69" s="33" t="e">
+      <c r="EA69" s="33">
         <f>EC68/EA68</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="ED69" s="34"/>
     </row>
@@ -12320,7 +12384,7 @@
       </c>
       <c r="E71" s="35">
         <f>1-E69</f>
-        <v>-5.75</v>
+        <v>-2.375</v>
       </c>
       <c r="H71" s="34"/>
       <c r="J71" s="32" t="s">
@@ -12366,9 +12430,9 @@
       <c r="AN71" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AO71" s="35" t="e">
+      <c r="AO71" s="35">
         <f>1-AO69</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="AR71" s="34"/>
       <c r="AT71" s="32" t="s">
@@ -12430,9 +12494,9 @@
       <c r="CJ71" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="CK71" s="35" t="e">
+      <c r="CK71" s="35">
         <f>1-CK69</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="CN71" s="34"/>
       <c r="CP71" s="32" t="s">
@@ -12486,9 +12550,9 @@
       <c r="DZ71" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="EA71" s="35" t="e">
+      <c r="EA71" s="35">
         <f>1-EA69</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="ED71" s="34"/>
     </row>
@@ -13097,19 +13161,19 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.44140625"/>
-    <col min="2" max="2" width="10.33203125"/>
+    <col min="1" max="1" width="33.42578125"/>
+    <col min="2" max="2" width="10.28515625"/>
     <col min="3" max="3" width="32"/>
     <col min="4" max="4" width="16"/>
-    <col min="5" max="5" width="12.88671875"/>
-    <col min="6" max="6" width="14.33203125"/>
-    <col min="7" max="7" width="18.6640625"/>
+    <col min="5" max="5" width="12.85546875"/>
+    <col min="6" max="6" width="14.28515625"/>
+    <col min="7" max="7" width="18.7109375"/>
     <col min="8" max="8" width="21"/>
-    <col min="9" max="9" width="14.44140625"/>
-    <col min="10" max="10" width="19.44140625"/>
-    <col min="11" max="11" width="23.44140625"/>
+    <col min="9" max="9" width="14.42578125"/>
+    <col min="10" max="10" width="19.42578125"/>
+    <col min="11" max="11" width="23.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -13152,28 +13216,28 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5546875"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875"/>
-    <col min="4" max="4" width="56.88671875"/>
-    <col min="5" max="1025" width="10.5546875"/>
+    <col min="1" max="1" width="10.5703125"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125"/>
+    <col min="4" max="4" width="56.85546875"/>
+    <col min="5" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="93"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
+      <c r="A2" s="92"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="38" t="s">

</xml_diff>

<commit_message>
Conteúdo da atualização: * adicionado alteraçõe sde projeto; * criado totalizaçãod e esforço na planilha de atividades
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_v1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="96">
   <si>
     <t>Cód.</t>
   </si>
@@ -145,18 +145,6 @@
   </si>
   <si>
     <t>Percentual atrasado do tempo estimado:</t>
-  </si>
-  <si>
-    <t>Total de horas do projeto =</t>
-  </si>
-  <si>
-    <t>Realizado =</t>
-  </si>
-  <si>
-    <t>Restantes =</t>
-  </si>
-  <si>
-    <t>Percentual concluído =</t>
   </si>
   <si>
     <t>Recurso</t>
@@ -293,6 +281,33 @@
   <si>
     <t>Criar do Seguro_v2.eap da sprint 2</t>
   </si>
+  <si>
+    <t>Horas orçadas sprint 1</t>
+  </si>
+  <si>
+    <t>Horas trabalhadas sprint 1</t>
+  </si>
+  <si>
+    <t>Horas orçadas sprint 2</t>
+  </si>
+  <si>
+    <t>Horas trabalhadas sprint 2</t>
+  </si>
+  <si>
+    <t>Horas orçadas documentação</t>
+  </si>
+  <si>
+    <t>Horas trabalhadas documentação</t>
+  </si>
+  <si>
+    <t>Horas orçadas total</t>
+  </si>
+  <si>
+    <t>Horas trabalhadas total</t>
+  </si>
+  <si>
+    <t>Esforço (Horas)</t>
+  </si>
 </sst>
 </file>
 
@@ -304,7 +319,7 @@
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="h:mm:ss"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -349,6 +364,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -614,7 +636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -810,14 +832,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -832,6 +854,21 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1197,19 +1234,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:EE80"/>
+  <dimension ref="A1:EE81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="DT3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="DT69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="EA4" sqref="EA4"/>
+      <selection pane="bottomRight" activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.42578125"/>
-    <col min="2" max="2" width="29.42578125"/>
+    <col min="2" max="2" width="31.140625" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
     <col min="4" max="5" width="11.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1295,181 +1332,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="85">
+      <c r="D1" s="86">
         <v>42322</v>
       </c>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
       <c r="I1" s="12"/>
-      <c r="J1" s="85">
+      <c r="J1" s="86">
         <v>42323</v>
       </c>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
       <c r="O1" s="12"/>
-      <c r="P1" s="85">
+      <c r="P1" s="86">
         <v>42324</v>
       </c>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="S1" s="87"/>
+      <c r="T1" s="87"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="85">
+      <c r="V1" s="86">
         <v>42325</v>
       </c>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
+      <c r="W1" s="87"/>
+      <c r="X1" s="87"/>
+      <c r="Y1" s="87"/>
+      <c r="Z1" s="87"/>
       <c r="AA1" s="12"/>
-      <c r="AB1" s="85">
+      <c r="AB1" s="86">
         <v>42326</v>
       </c>
-      <c r="AC1" s="86"/>
-      <c r="AD1" s="86"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="86"/>
+      <c r="AC1" s="87"/>
+      <c r="AD1" s="87"/>
+      <c r="AE1" s="87"/>
+      <c r="AF1" s="87"/>
       <c r="AG1" s="12"/>
-      <c r="AH1" s="85">
+      <c r="AH1" s="86">
         <v>42327</v>
       </c>
-      <c r="AI1" s="86"/>
-      <c r="AJ1" s="86"/>
-      <c r="AK1" s="86"/>
-      <c r="AL1" s="86"/>
+      <c r="AI1" s="87"/>
+      <c r="AJ1" s="87"/>
+      <c r="AK1" s="87"/>
+      <c r="AL1" s="87"/>
       <c r="AM1" s="12"/>
-      <c r="AN1" s="85">
+      <c r="AN1" s="86">
         <v>42328</v>
       </c>
-      <c r="AO1" s="86"/>
-      <c r="AP1" s="86"/>
-      <c r="AQ1" s="86"/>
-      <c r="AR1" s="86"/>
+      <c r="AO1" s="87"/>
+      <c r="AP1" s="87"/>
+      <c r="AQ1" s="87"/>
+      <c r="AR1" s="87"/>
       <c r="AS1" s="12"/>
-      <c r="AT1" s="85">
+      <c r="AT1" s="86">
         <v>42329</v>
       </c>
-      <c r="AU1" s="86"/>
-      <c r="AV1" s="86"/>
-      <c r="AW1" s="86"/>
-      <c r="AX1" s="86"/>
+      <c r="AU1" s="87"/>
+      <c r="AV1" s="87"/>
+      <c r="AW1" s="87"/>
+      <c r="AX1" s="87"/>
       <c r="AY1" s="12"/>
-      <c r="AZ1" s="85">
+      <c r="AZ1" s="86">
         <v>42330</v>
       </c>
-      <c r="BA1" s="86"/>
-      <c r="BB1" s="86"/>
-      <c r="BC1" s="86"/>
-      <c r="BD1" s="86"/>
+      <c r="BA1" s="87"/>
+      <c r="BB1" s="87"/>
+      <c r="BC1" s="87"/>
+      <c r="BD1" s="87"/>
       <c r="BE1" s="12"/>
-      <c r="BF1" s="85">
+      <c r="BF1" s="86">
         <v>42331</v>
       </c>
-      <c r="BG1" s="86"/>
-      <c r="BH1" s="86"/>
-      <c r="BI1" s="86"/>
-      <c r="BJ1" s="86"/>
+      <c r="BG1" s="87"/>
+      <c r="BH1" s="87"/>
+      <c r="BI1" s="87"/>
+      <c r="BJ1" s="87"/>
       <c r="BK1" s="12"/>
-      <c r="BL1" s="85">
+      <c r="BL1" s="86">
         <v>42332</v>
       </c>
-      <c r="BM1" s="86"/>
-      <c r="BN1" s="86"/>
-      <c r="BO1" s="86"/>
-      <c r="BP1" s="86"/>
+      <c r="BM1" s="87"/>
+      <c r="BN1" s="87"/>
+      <c r="BO1" s="87"/>
+      <c r="BP1" s="87"/>
       <c r="BQ1" s="12"/>
-      <c r="BR1" s="85">
+      <c r="BR1" s="86">
         <v>42333</v>
       </c>
-      <c r="BS1" s="86"/>
-      <c r="BT1" s="86"/>
-      <c r="BU1" s="86"/>
-      <c r="BV1" s="86"/>
+      <c r="BS1" s="87"/>
+      <c r="BT1" s="87"/>
+      <c r="BU1" s="87"/>
+      <c r="BV1" s="87"/>
       <c r="BW1" s="12"/>
-      <c r="BX1" s="85">
+      <c r="BX1" s="86">
         <v>42334</v>
       </c>
-      <c r="BY1" s="86"/>
-      <c r="BZ1" s="86"/>
-      <c r="CA1" s="86"/>
-      <c r="CB1" s="86"/>
+      <c r="BY1" s="87"/>
+      <c r="BZ1" s="87"/>
+      <c r="CA1" s="87"/>
+      <c r="CB1" s="87"/>
       <c r="CC1" s="12"/>
-      <c r="CD1" s="85">
+      <c r="CD1" s="86">
         <v>42335</v>
       </c>
-      <c r="CE1" s="86"/>
-      <c r="CF1" s="86"/>
-      <c r="CG1" s="86"/>
-      <c r="CH1" s="86"/>
+      <c r="CE1" s="87"/>
+      <c r="CF1" s="87"/>
+      <c r="CG1" s="87"/>
+      <c r="CH1" s="87"/>
       <c r="CI1" s="12"/>
-      <c r="CJ1" s="85">
+      <c r="CJ1" s="86">
         <v>42336</v>
       </c>
-      <c r="CK1" s="86"/>
-      <c r="CL1" s="86"/>
-      <c r="CM1" s="86"/>
-      <c r="CN1" s="86"/>
+      <c r="CK1" s="87"/>
+      <c r="CL1" s="87"/>
+      <c r="CM1" s="87"/>
+      <c r="CN1" s="87"/>
       <c r="CO1" s="12"/>
-      <c r="CP1" s="85">
+      <c r="CP1" s="86">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="86"/>
-      <c r="CR1" s="86"/>
-      <c r="CS1" s="86"/>
-      <c r="CT1" s="86"/>
+      <c r="CQ1" s="87"/>
+      <c r="CR1" s="87"/>
+      <c r="CS1" s="87"/>
+      <c r="CT1" s="87"/>
       <c r="CU1" s="12"/>
-      <c r="CV1" s="85">
+      <c r="CV1" s="86">
         <v>42338</v>
       </c>
-      <c r="CW1" s="86"/>
-      <c r="CX1" s="86"/>
-      <c r="CY1" s="86"/>
-      <c r="CZ1" s="86"/>
+      <c r="CW1" s="87"/>
+      <c r="CX1" s="87"/>
+      <c r="CY1" s="87"/>
+      <c r="CZ1" s="87"/>
       <c r="DA1" s="12"/>
-      <c r="DB1" s="85">
+      <c r="DB1" s="86">
         <v>42339</v>
       </c>
-      <c r="DC1" s="86"/>
-      <c r="DD1" s="86"/>
-      <c r="DE1" s="86"/>
-      <c r="DF1" s="86"/>
+      <c r="DC1" s="87"/>
+      <c r="DD1" s="87"/>
+      <c r="DE1" s="87"/>
+      <c r="DF1" s="87"/>
       <c r="DG1" s="12"/>
-      <c r="DH1" s="85">
+      <c r="DH1" s="86">
         <v>42340</v>
       </c>
-      <c r="DI1" s="86"/>
-      <c r="DJ1" s="86"/>
-      <c r="DK1" s="86"/>
-      <c r="DL1" s="86"/>
+      <c r="DI1" s="87"/>
+      <c r="DJ1" s="87"/>
+      <c r="DK1" s="87"/>
+      <c r="DL1" s="87"/>
       <c r="DM1" s="12"/>
-      <c r="DN1" s="85">
+      <c r="DN1" s="86">
         <v>42341</v>
       </c>
-      <c r="DO1" s="86"/>
-      <c r="DP1" s="86"/>
-      <c r="DQ1" s="86"/>
-      <c r="DR1" s="86"/>
+      <c r="DO1" s="87"/>
+      <c r="DP1" s="87"/>
+      <c r="DQ1" s="87"/>
+      <c r="DR1" s="87"/>
       <c r="DS1" s="12"/>
-      <c r="DT1" s="85">
+      <c r="DT1" s="86">
         <v>42342</v>
       </c>
-      <c r="DU1" s="86"/>
-      <c r="DV1" s="86"/>
-      <c r="DW1" s="86"/>
-      <c r="DX1" s="86"/>
+      <c r="DU1" s="87"/>
+      <c r="DV1" s="87"/>
+      <c r="DW1" s="87"/>
+      <c r="DX1" s="87"/>
       <c r="DY1" s="12"/>
-      <c r="DZ1" s="85">
+      <c r="DZ1" s="86">
         <v>42343</v>
       </c>
-      <c r="EA1" s="86"/>
-      <c r="EB1" s="86"/>
-      <c r="EC1" s="86"/>
-      <c r="ED1" s="86"/>
+      <c r="EA1" s="87"/>
+      <c r="EB1" s="87"/>
+      <c r="EC1" s="87"/>
+      <c r="ED1" s="87"/>
       <c r="EE1" s="12"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -1491,7 +1528,7 @@
         <v>6</v>
       </c>
       <c r="H2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="43" t="s">
@@ -1507,7 +1544,7 @@
         <v>6</v>
       </c>
       <c r="N2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="O2" s="12"/>
       <c r="P2" s="43" t="s">
@@ -1523,7 +1560,7 @@
         <v>6</v>
       </c>
       <c r="T2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="U2" s="12"/>
       <c r="V2" s="43" t="s">
@@ -1539,7 +1576,7 @@
         <v>6</v>
       </c>
       <c r="Z2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AA2" s="12"/>
       <c r="AB2" s="43" t="s">
@@ -1555,7 +1592,7 @@
         <v>6</v>
       </c>
       <c r="AF2" s="61" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AG2" s="12"/>
       <c r="AH2" s="43" t="s">
@@ -1571,7 +1608,7 @@
         <v>6</v>
       </c>
       <c r="AL2" s="61" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AM2" s="12"/>
       <c r="AN2" s="43" t="s">
@@ -1587,7 +1624,7 @@
         <v>6</v>
       </c>
       <c r="AR2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AS2" s="12"/>
       <c r="AT2" s="43" t="s">
@@ -1603,7 +1640,7 @@
         <v>6</v>
       </c>
       <c r="AX2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="AY2" s="12"/>
       <c r="AZ2" s="43" t="s">
@@ -1619,7 +1656,7 @@
         <v>6</v>
       </c>
       <c r="BD2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="BE2" s="12"/>
       <c r="BF2" s="43" t="s">
@@ -1635,7 +1672,7 @@
         <v>6</v>
       </c>
       <c r="BJ2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="BK2" s="12"/>
       <c r="BL2" s="43" t="s">
@@ -1651,7 +1688,7 @@
         <v>6</v>
       </c>
       <c r="BP2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="BQ2" s="12"/>
       <c r="BR2" s="43" t="s">
@@ -1667,7 +1704,7 @@
         <v>6</v>
       </c>
       <c r="BV2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="BW2" s="12"/>
       <c r="BX2" s="43" t="s">
@@ -1683,7 +1720,7 @@
         <v>6</v>
       </c>
       <c r="CB2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="CC2" s="12"/>
       <c r="CD2" s="43" t="s">
@@ -1699,7 +1736,7 @@
         <v>6</v>
       </c>
       <c r="CH2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="CI2" s="12"/>
       <c r="CJ2" s="43" t="s">
@@ -1715,7 +1752,7 @@
         <v>6</v>
       </c>
       <c r="CN2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="CO2" s="12"/>
       <c r="CP2" s="43" t="s">
@@ -1731,7 +1768,7 @@
         <v>6</v>
       </c>
       <c r="CT2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="CU2" s="12"/>
       <c r="CV2" s="43" t="s">
@@ -1747,7 +1784,7 @@
         <v>6</v>
       </c>
       <c r="CZ2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="DA2" s="12"/>
       <c r="DB2" s="43" t="s">
@@ -1763,7 +1800,7 @@
         <v>6</v>
       </c>
       <c r="DF2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="DG2" s="12"/>
       <c r="DH2" s="43" t="s">
@@ -1779,7 +1816,7 @@
         <v>6</v>
       </c>
       <c r="DL2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="DM2" s="12"/>
       <c r="DN2" s="43" t="s">
@@ -1795,7 +1832,7 @@
         <v>6</v>
       </c>
       <c r="DR2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="DS2" s="12"/>
       <c r="DT2" s="43" t="s">
@@ -1811,7 +1848,7 @@
         <v>6</v>
       </c>
       <c r="DX2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="DY2" s="12"/>
       <c r="DZ2" s="43" t="s">
@@ -1827,7 +1864,7 @@
         <v>6</v>
       </c>
       <c r="ED2" s="44" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="EE2" s="12"/>
     </row>
@@ -2055,7 +2092,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="EA3" s="72">
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="EB3" s="74"/>
       <c r="EC3" s="74"/>
@@ -2070,7 +2107,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
@@ -2218,7 +2255,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="4"/>
       <c r="C5" s="46" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="7"/>
@@ -2362,10 +2399,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D6" s="14">
         <v>8.3333333333333301E-2</v>
@@ -2514,10 +2551,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C7" s="47" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D7" s="14">
         <v>4.1666666666666664E-2</v>
@@ -2671,7 +2708,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="85" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="14">
@@ -2823,7 +2860,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="87"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -2974,7 +3011,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="89" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D10" s="6">
         <v>4.1666666666666699E-2</v>
@@ -3125,7 +3162,7 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="87"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3276,7 +3313,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="89" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D12" s="6">
         <v>4.1666666666666699E-2</v>
@@ -3439,7 +3476,7 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="87"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3593,7 +3630,7 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="87"/>
+      <c r="C14" s="85"/>
       <c r="D14" s="6">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3739,10 +3776,10 @@
     <row r="15" spans="1:135">
       <c r="A15" s="2"/>
       <c r="B15" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="7"/>
@@ -3886,14 +3923,12 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="6">
-        <v>8.3333333333333329E-2</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D16" s="6"/>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
       <c r="G16" s="45"/>
@@ -4033,10 +4068,10 @@
     <row r="17" spans="1:135">
       <c r="A17" s="2"/>
       <c r="B17" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="7"/>
@@ -4178,10 +4213,10 @@
     <row r="18" spans="1:135">
       <c r="A18" s="2"/>
       <c r="B18" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C18" s="67" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="7"/>
@@ -4327,10 +4362,10 @@
     <row r="19" spans="1:135">
       <c r="A19" s="2"/>
       <c r="B19" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="7"/>
@@ -4472,10 +4507,10 @@
     <row r="20" spans="1:135">
       <c r="A20" s="2"/>
       <c r="B20" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="7"/>
@@ -4617,10 +4652,10 @@
     <row r="21" spans="1:135">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="7"/>
@@ -4762,10 +4797,10 @@
     <row r="22" spans="1:135">
       <c r="A22" s="2"/>
       <c r="B22" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
@@ -4909,14 +4944,12 @@
         <v>15</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="D23" s="6">
-        <v>8.3333333333333329E-2</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D23" s="6"/>
       <c r="E23" s="7"/>
       <c r="F23" s="8"/>
       <c r="G23" s="45"/>
@@ -5056,10 +5089,10 @@
     <row r="24" spans="1:135">
       <c r="A24" s="2"/>
       <c r="B24" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C24" s="67" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="7"/>
@@ -5201,10 +5234,10 @@
     <row r="25" spans="1:135">
       <c r="A25" s="2"/>
       <c r="B25" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C25" s="67" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="7"/>
@@ -5352,7 +5385,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C26" s="90" t="s">
         <v>23</v>
@@ -5499,7 +5532,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C27" s="91"/>
       <c r="D27" s="6"/>
@@ -5642,10 +5675,10 @@
     <row r="28" spans="1:135">
       <c r="A28" s="2"/>
       <c r="B28" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="7"/>
@@ -5789,10 +5822,10 @@
         <v>18</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="46" t="s">
         <v>69</v>
-      </c>
-      <c r="C29" s="46" t="s">
-        <v>73</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="7"/>
@@ -5932,9 +5965,9 @@
         <v>19</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="87" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="85" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="6"/>
@@ -6079,9 +6112,9 @@
         <v>20</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="87"/>
+        <v>65</v>
+      </c>
+      <c r="C31" s="85"/>
       <c r="D31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="8"/>
@@ -6224,9 +6257,9 @@
         <v>21</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="87"/>
+        <v>65</v>
+      </c>
+      <c r="C32" s="85"/>
       <c r="D32" s="6"/>
       <c r="E32" s="7"/>
       <c r="F32" s="8"/>
@@ -6367,10 +6400,10 @@
     <row r="33" spans="1:135">
       <c r="A33" s="2"/>
       <c r="B33" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C33" s="68" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="7"/>
@@ -6516,10 +6549,10 @@
     <row r="34" spans="1:135">
       <c r="A34" s="2"/>
       <c r="B34" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C34" s="67" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="7"/>
@@ -6669,10 +6702,10 @@
     <row r="35" spans="1:135">
       <c r="A35" s="2"/>
       <c r="B35" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C35" s="48" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="7"/>
@@ -6817,7 +6850,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="48" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="7"/>
@@ -6966,7 +6999,7 @@
         <v>13</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="7"/>
@@ -7116,7 +7149,7 @@
       <c r="B38" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="87" t="s">
+      <c r="C38" s="85" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="6"/>
@@ -7259,7 +7292,7 @@
       <c r="B39" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="87"/>
+      <c r="C39" s="85"/>
       <c r="D39" s="6"/>
       <c r="E39" s="7"/>
       <c r="F39" s="8"/>
@@ -7543,10 +7576,10 @@
     <row r="41" spans="1:135" ht="30">
       <c r="A41" s="2"/>
       <c r="B41" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C41" s="46" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="7"/>
@@ -7688,10 +7721,10 @@
     <row r="42" spans="1:135" ht="30">
       <c r="A42" s="2"/>
       <c r="B42" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C42" s="46" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D42" s="6"/>
       <c r="E42" s="7"/>
@@ -7970,10 +8003,10 @@
     <row r="44" spans="1:135">
       <c r="A44" s="2"/>
       <c r="B44" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C44" s="46" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D44" s="6"/>
       <c r="E44" s="7"/>
@@ -8115,10 +8148,10 @@
     <row r="45" spans="1:135">
       <c r="A45" s="2"/>
       <c r="B45" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C45" s="46" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D45" s="6"/>
       <c r="E45" s="7"/>
@@ -8260,10 +8293,10 @@
     <row r="46" spans="1:135">
       <c r="A46" s="2"/>
       <c r="B46" s="17" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C46" s="46" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D46" s="6"/>
       <c r="E46" s="7"/>
@@ -8709,7 +8742,7 @@
         <v>16</v>
       </c>
       <c r="C49" s="46" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D49" s="6"/>
       <c r="E49" s="7"/>
@@ -8853,10 +8886,10 @@
         <v>27</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D50" s="14"/>
       <c r="E50" s="18"/>
@@ -8993,10 +9026,10 @@
     <row r="51" spans="1:135" ht="14.1" customHeight="1">
       <c r="A51" s="2"/>
       <c r="B51" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C51" s="81" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D51" s="14"/>
       <c r="E51" s="18"/>
@@ -9172,11 +9205,15 @@
       <c r="DW51" s="18"/>
       <c r="DX51" s="52"/>
       <c r="DY51" s="12"/>
-      <c r="DZ51" s="14"/>
-      <c r="EA51" s="18"/>
+      <c r="DZ51" s="14">
+        <v>0</v>
+      </c>
+      <c r="EA51" s="82">
+        <v>0.125</v>
+      </c>
       <c r="EB51" s="18"/>
       <c r="EC51" s="18"/>
-      <c r="ED51" s="10"/>
+      <c r="ED51" s="54"/>
       <c r="EE51" s="12"/>
     </row>
     <row r="52" spans="1:135" ht="14.1" customHeight="1">
@@ -9184,10 +9221,10 @@
         <v>28</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C52" s="48" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D52" s="14"/>
       <c r="E52" s="18"/>
@@ -9374,7 +9411,7 @@
         <v>19</v>
       </c>
       <c r="C53" s="46" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D53" s="14"/>
       <c r="E53" s="18"/>
@@ -9542,11 +9579,15 @@
       <c r="DW53" s="18"/>
       <c r="DX53" s="10"/>
       <c r="DY53" s="12"/>
-      <c r="DZ53" s="14"/>
-      <c r="EA53" s="18"/>
+      <c r="DZ53" s="14">
+        <v>0</v>
+      </c>
+      <c r="EA53" s="82">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="EB53" s="18"/>
       <c r="EC53" s="18"/>
-      <c r="ED53" s="10"/>
+      <c r="ED53" s="53"/>
       <c r="EE53" s="12"/>
     </row>
     <row r="54" spans="1:135">
@@ -9982,7 +10023,7 @@
         <v>21</v>
       </c>
       <c r="C57" s="84" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D57" s="83"/>
       <c r="E57" s="18"/>
@@ -11671,7 +11712,7 @@
       </c>
       <c r="D68" s="28">
         <f>SUM(D3:D65)</f>
-        <v>0.62500000000000011</v>
+        <v>0.45833333333333343</v>
       </c>
       <c r="E68" s="29">
         <f>SUM(E3:E65)</f>
@@ -12011,7 +12052,7 @@
       </c>
       <c r="EA68" s="29">
         <f>SUM(EA3:EA65)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>0.27083333333333331</v>
       </c>
       <c r="EB68" s="30" t="s">
         <v>37</v>
@@ -12201,12 +12242,15 @@
       <c r="ED69" s="34"/>
     </row>
     <row r="70" spans="1:135">
+      <c r="B70" s="19" t="s">
+        <v>95</v>
+      </c>
       <c r="D70" s="32" t="s">
         <v>39</v>
       </c>
       <c r="E70" s="33">
         <f>G68/D68</f>
-        <v>1.7999999999999996</v>
+        <v>2.4545454545454541</v>
       </c>
       <c r="H70" s="34"/>
       <c r="J70" s="32" t="s">
@@ -12379,6 +12423,13 @@
       <c r="ED70" s="34"/>
     </row>
     <row r="71" spans="1:135">
+      <c r="B71" s="93" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71" s="96">
+        <f>SUM(D68+J68+P68+V68+AN68+AB68+AH68)</f>
+        <v>2.5000000000000004</v>
+      </c>
       <c r="D71" s="32" t="s">
         <v>40</v>
       </c>
@@ -12557,12 +12608,19 @@
       <c r="ED71" s="34"/>
     </row>
     <row r="72" spans="1:135">
+      <c r="B72" s="93" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" s="96">
+        <f>SUM(E68+K68+Q68+W68+AC68+AI68+AO68)</f>
+        <v>1.8124999999999998</v>
+      </c>
       <c r="D72" s="32" t="s">
         <v>41</v>
       </c>
       <c r="E72" s="35">
         <f>1-E70</f>
-        <v>-0.7999999999999996</v>
+        <v>-1.4545454545454541</v>
       </c>
       <c r="H72" s="34"/>
       <c r="J72" s="32" t="s">
@@ -12735,6 +12793,8 @@
       <c r="ED72" s="34"/>
     </row>
     <row r="73" spans="1:135">
+      <c r="B73" s="22"/>
+      <c r="C73" s="97"/>
       <c r="D73"/>
       <c r="E73"/>
       <c r="J73"/>
@@ -12781,6 +12841,13 @@
       <c r="EA73"/>
     </row>
     <row r="74" spans="1:135">
+      <c r="B74" s="94" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" s="96">
+        <f>SUM(AT68+AZ68+BF68+BR68+BL68+BX68+CD68)</f>
+        <v>1.7499999999999998</v>
+      </c>
       <c r="D74"/>
       <c r="E74"/>
       <c r="J74"/>
@@ -12827,6 +12894,13 @@
       <c r="EA74"/>
     </row>
     <row r="75" spans="1:135">
+      <c r="B75" s="93" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" s="96">
+        <f>SUM(AU68+BA68+BG68+BM68+BS68+BY68+CE68)</f>
+        <v>1.6666666666666667</v>
+      </c>
       <c r="D75"/>
       <c r="E75"/>
       <c r="J75"/>
@@ -12873,6 +12947,8 @@
       <c r="EA75"/>
     </row>
     <row r="76" spans="1:135">
+      <c r="B76" s="93"/>
+      <c r="C76" s="97"/>
       <c r="D76"/>
       <c r="E76"/>
       <c r="J76"/>
@@ -12919,18 +12995,16 @@
       <c r="EA76"/>
     </row>
     <row r="77" spans="1:135">
-      <c r="C77" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="D77" s="36" t="e">
-        <f>SUM(D3:D65)+SUM(#REF!)+SUM(#REF!)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="B77" s="94" t="s">
+        <v>89</v>
+      </c>
+      <c r="C77" s="98">
+        <f>SUM(CJ68+CP68+CV68+DB68+DH68+DN68+DT68+DZ68)</f>
+        <v>2.2916666666666661</v>
+      </c>
+      <c r="D77" s="36"/>
       <c r="E77" s="37"/>
-      <c r="J77" s="36" t="e">
-        <f>SUM(J3:J65)+SUM(#REF!)+SUM(#REF!)+SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="J77" s="36"/>
       <c r="K77" s="37"/>
       <c r="P77" s="36" t="e">
         <f>SUM(P3:P65)+SUM(#REF!)+SUM(#REF!)+SUM(#REF!)</f>
@@ -13034,8 +13108,12 @@
       <c r="EA77" s="37"/>
     </row>
     <row r="78" spans="1:135">
-      <c r="C78" s="32" t="s">
-        <v>43</v>
+      <c r="B78" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="C78" s="98">
+        <f>SUM(CK68+CQ68+CW68+DC68+DI68+DO68+DU68+EA68)</f>
+        <v>2.208333333333333</v>
       </c>
       <c r="D78" s="36"/>
       <c r="J78" s="36"/>
@@ -13061,9 +13139,8 @@
       <c r="DZ78" s="36"/>
     </row>
     <row r="79" spans="1:135">
-      <c r="C79" s="32" t="s">
-        <v>44</v>
-      </c>
+      <c r="B79" s="22"/>
+      <c r="C79" s="99"/>
       <c r="D79" s="36"/>
       <c r="J79" s="36"/>
       <c r="P79" s="36"/>
@@ -13088,8 +13165,12 @@
       <c r="DZ79" s="36"/>
     </row>
     <row r="80" spans="1:135">
-      <c r="C80" s="32" t="s">
-        <v>45</v>
+      <c r="B80" s="95" t="s">
+        <v>93</v>
+      </c>
+      <c r="C80" s="98">
+        <f>SUM(C71+C74+C77)</f>
+        <v>6.5416666666666661</v>
       </c>
       <c r="D80" s="33"/>
       <c r="J80" s="33"/>
@@ -13114,8 +13195,35 @@
       <c r="DT80" s="33"/>
       <c r="DZ80" s="33"/>
     </row>
+    <row r="81" spans="2:3">
+      <c r="B81" s="95" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="96">
+        <f>SUM(C72+C75+C78)</f>
+        <v>5.6875</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="DN1:DR1"/>
+    <mergeCell ref="DT1:DX1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BL1:BP1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BX1:CB1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="DZ1:ED1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="CP1:CT1"/>
+    <mergeCell ref="CV1:CZ1"/>
+    <mergeCell ref="DB1:DF1"/>
+    <mergeCell ref="DH1:DL1"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="AH1:AL1"/>
     <mergeCell ref="AN1:AR1"/>
@@ -13128,24 +13236,6 @@
     <mergeCell ref="P1:T1"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="DZ1:ED1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="CP1:CT1"/>
-    <mergeCell ref="CV1:CZ1"/>
-    <mergeCell ref="DB1:DF1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="DN1:DR1"/>
-    <mergeCell ref="DT1:DX1"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BL1:BP1"/>
-    <mergeCell ref="BR1:BV1"/>
-    <mergeCell ref="BX1:CB1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="AB1:AF1"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -13178,27 +13268,27 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B3" s="49"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B4" s="15"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B5" s="51"/>
     </row>
@@ -13227,7 +13317,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="92" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B1" s="92"/>
       <c r="C1" s="92"/>
@@ -13241,30 +13331,30 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="38" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D3" s="38" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="22" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" s="40">
         <v>42322</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4">

</xml_diff>